<commit_message>
Minor spelling mistakes, preparations for demo.
This software is about to go public, this commit is to ready for a demonstation
which will occur. Final nits to make things better.
</commit_message>
<xml_diff>
--- a/Doc/testPlan.xlsx
+++ b/Doc/testPlan.xlsx
@@ -356,9 +356,6 @@
   </si>
   <si>
     <t>Group I/O specific Q operations</t>
-  </si>
-  <si>
-    <t>Group admin specific Q operations</t>
   </si>
   <si>
     <t>Validate SQ, CQ illegal sizes</t>
@@ -1544,6 +1541,9 @@
   </si>
   <si>
     <t>TestNvmeReadNoncontig()</t>
+  </si>
+  <si>
+    <t>Group admin Q operations</t>
   </si>
 </sst>
 </file>
@@ -1811,7 +1811,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1969,26 +1969,79 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1996,17 +2049,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2029,27 +2094,6 @@
     <xf numFmtId="49" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -2089,48 +2133,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3078,8 +3081,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E311"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="D74" sqref="D74"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="D121" sqref="D121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3093,32 +3096,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="17" customFormat="1" ht="15" customHeight="1">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="88" t="s">
+        <v>329</v>
+      </c>
+      <c r="B1" s="89" t="s">
+        <v>359</v>
+      </c>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="18"/>
+    </row>
+    <row r="2" spans="1:5" s="17" customFormat="1" ht="15" customHeight="1">
+      <c r="A2" s="88"/>
+      <c r="B2" s="106" t="s">
+        <v>384</v>
+      </c>
+      <c r="C2" s="106"/>
+      <c r="D2" s="106"/>
+      <c r="E2" s="18"/>
+    </row>
+    <row r="3" spans="1:5" s="17" customFormat="1" ht="15" customHeight="1">
+      <c r="A3" s="88"/>
+      <c r="B3" s="107" t="s">
         <v>330</v>
       </c>
-      <c r="B1" s="66" t="s">
-        <v>360</v>
-      </c>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="18"/>
-    </row>
-    <row r="2" spans="1:5" s="17" customFormat="1" ht="15" customHeight="1">
-      <c r="A2" s="93"/>
-      <c r="B2" s="90" t="s">
-        <v>385</v>
-      </c>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="18"/>
-    </row>
-    <row r="3" spans="1:5" s="17" customFormat="1" ht="15" customHeight="1">
-      <c r="A3" s="93"/>
-      <c r="B3" s="91" t="s">
-        <v>331</v>
-      </c>
-      <c r="C3" s="92"/>
-      <c r="D3" s="92"/>
+      <c r="C3" s="108"/>
+      <c r="D3" s="108"/>
       <c r="E3" s="44"/>
     </row>
     <row r="4" spans="1:5">
@@ -3129,7 +3132,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D4" s="32" t="s">
         <v>2</v>
@@ -3145,69 +3148,69 @@
       <c r="B5" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="C5" s="67"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="69"/>
+      <c r="C5" s="90"/>
+      <c r="D5" s="91"/>
+      <c r="E5" s="92"/>
     </row>
     <row r="6" spans="1:5" s="4" customFormat="1">
-      <c r="A6" s="76"/>
-      <c r="B6" s="77"/>
-      <c r="C6" s="88"/>
-      <c r="D6" s="86" t="s">
+      <c r="A6" s="69"/>
+      <c r="B6" s="70"/>
+      <c r="C6" s="104"/>
+      <c r="D6" s="102" t="s">
         <v>99</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="4" customFormat="1">
+      <c r="A7" s="71"/>
+      <c r="B7" s="72"/>
+      <c r="C7" s="105"/>
+      <c r="D7" s="103"/>
+      <c r="E7" s="1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="4" customFormat="1">
-      <c r="A7" s="78"/>
-      <c r="B7" s="79"/>
-      <c r="C7" s="89"/>
-      <c r="D7" s="87"/>
-      <c r="E7" s="1" t="s">
+    <row r="8" spans="1:5" s="4" customFormat="1">
+      <c r="A8" s="71"/>
+      <c r="B8" s="72"/>
+      <c r="C8" s="105"/>
+      <c r="D8" s="103"/>
+      <c r="E8" s="1" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="4" customFormat="1">
-      <c r="A8" s="78"/>
-      <c r="B8" s="79"/>
-      <c r="C8" s="89"/>
-      <c r="D8" s="87"/>
-      <c r="E8" s="1" t="s">
+    <row r="9" spans="1:5" s="4" customFormat="1">
+      <c r="A9" s="71"/>
+      <c r="B9" s="72"/>
+      <c r="C9" s="105"/>
+      <c r="D9" s="103"/>
+      <c r="E9" s="1" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="4" customFormat="1">
-      <c r="A9" s="78"/>
-      <c r="B9" s="79"/>
-      <c r="C9" s="89"/>
-      <c r="D9" s="87"/>
-      <c r="E9" s="1" t="s">
+    <row r="10" spans="1:5" s="4" customFormat="1">
+      <c r="A10" s="71"/>
+      <c r="B10" s="72"/>
+      <c r="C10" s="105"/>
+      <c r="D10" s="103"/>
+      <c r="E10" s="1" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="4" customFormat="1">
-      <c r="A10" s="78"/>
-      <c r="B10" s="79"/>
-      <c r="C10" s="89"/>
-      <c r="D10" s="87"/>
-      <c r="E10" s="1" t="s">
+    <row r="11" spans="1:5" s="4" customFormat="1" ht="30" customHeight="1">
+      <c r="A11" s="71"/>
+      <c r="B11" s="72"/>
+      <c r="C11" s="105"/>
+      <c r="D11" s="103"/>
+      <c r="E11" s="28" t="s">
         <v>241</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" s="4" customFormat="1" ht="30" customHeight="1">
-      <c r="A11" s="78"/>
-      <c r="B11" s="79"/>
-      <c r="C11" s="89"/>
-      <c r="D11" s="87"/>
-      <c r="E11" s="28" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="4" customFormat="1" ht="30" customHeight="1">
       <c r="A12" s="7" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>86</v>
@@ -3217,234 +3220,234 @@
       <c r="E12" s="31"/>
     </row>
     <row r="13" spans="1:5" s="4" customFormat="1" ht="30" customHeight="1">
-      <c r="A13" s="76"/>
-      <c r="B13" s="77"/>
+      <c r="A13" s="69"/>
+      <c r="B13" s="70"/>
       <c r="C13" s="20"/>
       <c r="D13" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A14" s="78"/>
-      <c r="B14" s="79"/>
+      <c r="A14" s="71"/>
+      <c r="B14" s="72"/>
       <c r="C14" s="29"/>
       <c r="D14" s="3" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="4" customFormat="1" ht="30" customHeight="1">
-      <c r="A15" s="78"/>
-      <c r="B15" s="79"/>
+      <c r="A15" s="71"/>
+      <c r="B15" s="72"/>
       <c r="C15" s="49"/>
       <c r="D15" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="4" customFormat="1" ht="30" customHeight="1">
-      <c r="A16" s="78"/>
-      <c r="B16" s="79"/>
+      <c r="A16" s="71"/>
+      <c r="B16" s="72"/>
       <c r="C16" s="20"/>
       <c r="D16" s="3" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="4" customFormat="1" ht="30" customHeight="1">
-      <c r="A17" s="78"/>
-      <c r="B17" s="79"/>
+      <c r="A17" s="71"/>
+      <c r="B17" s="72"/>
       <c r="C17" s="20"/>
       <c r="D17" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="4" customFormat="1" ht="30" customHeight="1">
-      <c r="A18" s="78"/>
-      <c r="B18" s="79"/>
+      <c r="A18" s="71"/>
+      <c r="B18" s="72"/>
       <c r="C18" s="20"/>
       <c r="D18" s="3" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="4" customFormat="1" ht="30" customHeight="1">
-      <c r="A19" s="78"/>
-      <c r="B19" s="79"/>
+      <c r="A19" s="71"/>
+      <c r="B19" s="72"/>
       <c r="C19" s="20"/>
       <c r="D19" s="3" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="4" customFormat="1" ht="45">
-      <c r="A20" s="78"/>
-      <c r="B20" s="79"/>
+      <c r="A20" s="71"/>
+      <c r="B20" s="72"/>
       <c r="C20" s="49"/>
       <c r="D20" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="4" customFormat="1" ht="30" customHeight="1">
-      <c r="A21" s="78"/>
-      <c r="B21" s="79"/>
+      <c r="A21" s="71"/>
+      <c r="B21" s="72"/>
       <c r="C21" s="20"/>
       <c r="D21" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="4" customFormat="1" ht="30" customHeight="1">
-      <c r="A22" s="78"/>
-      <c r="B22" s="79"/>
+      <c r="A22" s="71"/>
+      <c r="B22" s="72"/>
       <c r="C22" s="20"/>
       <c r="D22" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="4" customFormat="1" ht="30" customHeight="1">
-      <c r="A23" s="78"/>
-      <c r="B23" s="79"/>
+      <c r="A23" s="71"/>
+      <c r="B23" s="72"/>
       <c r="C23" s="20"/>
       <c r="D23" s="3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="4" customFormat="1" ht="30" customHeight="1">
-      <c r="A24" s="78"/>
-      <c r="B24" s="79"/>
+      <c r="A24" s="71"/>
+      <c r="B24" s="72"/>
       <c r="C24" s="49"/>
       <c r="D24" s="3" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="4" customFormat="1" ht="30" customHeight="1">
-      <c r="A25" s="78"/>
-      <c r="B25" s="79"/>
+      <c r="A25" s="71"/>
+      <c r="B25" s="72"/>
       <c r="C25" s="20"/>
       <c r="D25" s="3" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E25" s="16" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="26" spans="1:5" s="4" customFormat="1" ht="45">
-      <c r="A26" s="78"/>
-      <c r="B26" s="79"/>
+      <c r="A26" s="71"/>
+      <c r="B26" s="72"/>
       <c r="C26" s="49"/>
       <c r="D26" s="3" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="27" spans="1:5" s="4" customFormat="1" ht="45">
-      <c r="A27" s="78"/>
-      <c r="B27" s="79"/>
+      <c r="A27" s="71"/>
+      <c r="B27" s="72"/>
       <c r="C27" s="49"/>
       <c r="D27" s="3" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="4" customFormat="1">
-      <c r="A28" s="78"/>
-      <c r="B28" s="79"/>
+      <c r="A28" s="71"/>
+      <c r="B28" s="72"/>
       <c r="C28" s="45"/>
       <c r="D28" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="E28" s="16" t="s">
         <v>408</v>
       </c>
-      <c r="E28" s="16" t="s">
-        <v>409</v>
-      </c>
     </row>
     <row r="29" spans="1:5" s="4" customFormat="1">
-      <c r="A29" s="78"/>
-      <c r="B29" s="79"/>
+      <c r="A29" s="71"/>
+      <c r="B29" s="72"/>
       <c r="C29" s="45"/>
       <c r="D29" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E29" s="16" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="30" spans="1:5" s="4" customFormat="1">
-      <c r="A30" s="78"/>
-      <c r="B30" s="79"/>
+      <c r="A30" s="71"/>
+      <c r="B30" s="72"/>
       <c r="C30" s="45"/>
       <c r="D30" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E30" s="16" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="4" customFormat="1">
-      <c r="A31" s="78"/>
-      <c r="B31" s="79"/>
+      <c r="A31" s="71"/>
+      <c r="B31" s="72"/>
       <c r="C31" s="45"/>
       <c r="D31" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E31" s="16" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="4" customFormat="1">
-      <c r="A32" s="78"/>
-      <c r="B32" s="79"/>
+      <c r="A32" s="71"/>
+      <c r="B32" s="72"/>
       <c r="C32" s="45"/>
       <c r="D32" s="3" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="4" customFormat="1">
-      <c r="A33" s="78"/>
-      <c r="B33" s="79"/>
+      <c r="A33" s="71"/>
+      <c r="B33" s="72"/>
       <c r="C33" s="45"/>
       <c r="D33" s="3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E33" s="16" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="34" spans="1:5" s="4" customFormat="1">
@@ -3454,44 +3457,44 @@
       <c r="B34" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="C34" s="70" t="s">
+      <c r="C34" s="93" t="s">
         <v>88</v>
       </c>
-      <c r="D34" s="71"/>
-      <c r="E34" s="72"/>
+      <c r="D34" s="94"/>
+      <c r="E34" s="95"/>
     </row>
     <row r="35" spans="1:5" s="4" customFormat="1" ht="75">
-      <c r="A35" s="80"/>
-      <c r="B35" s="81"/>
+      <c r="A35" s="96"/>
+      <c r="B35" s="97"/>
       <c r="C35" s="19"/>
       <c r="D35" s="3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E35" s="10"/>
     </row>
     <row r="36" spans="1:5" s="4" customFormat="1" ht="75">
-      <c r="A36" s="82"/>
-      <c r="B36" s="83"/>
+      <c r="A36" s="98"/>
+      <c r="B36" s="99"/>
       <c r="C36" s="20"/>
       <c r="D36" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E36" s="10"/>
     </row>
     <row r="37" spans="1:5" s="4" customFormat="1" ht="75">
-      <c r="A37" s="82"/>
-      <c r="B37" s="83"/>
+      <c r="A37" s="98"/>
+      <c r="B37" s="99"/>
       <c r="C37" s="19"/>
       <c r="D37" s="3" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E37" s="10" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="38" spans="1:5" s="4" customFormat="1" ht="45">
-      <c r="A38" s="82"/>
-      <c r="B38" s="83"/>
+      <c r="A38" s="98"/>
+      <c r="B38" s="99"/>
       <c r="C38" s="19"/>
       <c r="D38" s="3" t="s">
         <v>89</v>
@@ -3501,19 +3504,19 @@
       </c>
     </row>
     <row r="39" spans="1:5" s="4" customFormat="1" ht="45">
-      <c r="A39" s="82"/>
-      <c r="B39" s="83"/>
+      <c r="A39" s="98"/>
+      <c r="B39" s="99"/>
       <c r="C39" s="19"/>
       <c r="D39" s="3" t="s">
         <v>96</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="40" spans="1:5" s="4" customFormat="1" ht="75">
-      <c r="A40" s="82"/>
-      <c r="B40" s="83"/>
+      <c r="A40" s="98"/>
+      <c r="B40" s="99"/>
       <c r="C40" s="19"/>
       <c r="D40" s="3" t="s">
         <v>97</v>
@@ -3521,8 +3524,8 @@
       <c r="E40" s="10"/>
     </row>
     <row r="41" spans="1:5" s="4" customFormat="1" ht="45">
-      <c r="A41" s="82"/>
-      <c r="B41" s="83"/>
+      <c r="A41" s="98"/>
+      <c r="B41" s="99"/>
       <c r="C41" s="19"/>
       <c r="D41" s="3" t="s">
         <v>101</v>
@@ -3530,14 +3533,14 @@
       <c r="E41" s="10"/>
     </row>
     <row r="42" spans="1:5" s="4" customFormat="1" ht="45">
-      <c r="A42" s="82"/>
-      <c r="B42" s="83"/>
+      <c r="A42" s="98"/>
+      <c r="B42" s="99"/>
       <c r="C42" s="19"/>
       <c r="D42" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="E42" s="10" t="s">
         <v>132</v>
-      </c>
-      <c r="E42" s="10" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="43" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1">
@@ -3547,16 +3550,16 @@
       <c r="B43" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="C43" s="70" t="s">
+      <c r="C43" s="93" t="s">
         <v>100</v>
       </c>
-      <c r="D43" s="71"/>
-      <c r="E43" s="72"/>
+      <c r="D43" s="94"/>
+      <c r="E43" s="95"/>
     </row>
     <row r="44" spans="1:5" s="4" customFormat="1">
-      <c r="A44" s="80"/>
-      <c r="B44" s="81"/>
-      <c r="C44" s="84"/>
+      <c r="A44" s="96"/>
+      <c r="B44" s="97"/>
+      <c r="C44" s="100"/>
       <c r="D44" s="3" t="s">
         <v>91</v>
       </c>
@@ -3565,9 +3568,9 @@
       </c>
     </row>
     <row r="45" spans="1:5" s="4" customFormat="1">
-      <c r="A45" s="82"/>
-      <c r="B45" s="83"/>
-      <c r="C45" s="85"/>
+      <c r="A45" s="98"/>
+      <c r="B45" s="99"/>
+      <c r="C45" s="101"/>
       <c r="D45" s="3" t="s">
         <v>93</v>
       </c>
@@ -3582,42 +3585,42 @@
       <c r="B46" s="8">
         <v>2</v>
       </c>
-      <c r="C46" s="73" t="s">
+      <c r="C46" s="66" t="s">
+        <v>232</v>
+      </c>
+      <c r="D46" s="67"/>
+      <c r="E46" s="68"/>
+    </row>
+    <row r="47" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1">
+      <c r="A47" s="69"/>
+      <c r="B47" s="70"/>
+      <c r="C47" s="73" t="s">
+        <v>235</v>
+      </c>
+      <c r="D47" s="74"/>
+      <c r="E47" s="75"/>
+    </row>
+    <row r="48" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1">
+      <c r="A48" s="71"/>
+      <c r="B48" s="72"/>
+      <c r="C48" s="66" t="s">
         <v>233</v>
       </c>
-      <c r="D46" s="74"/>
-      <c r="E46" s="75"/>
-    </row>
-    <row r="47" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A47" s="76"/>
-      <c r="B47" s="77"/>
-      <c r="C47" s="101" t="s">
-        <v>236</v>
-      </c>
-      <c r="D47" s="102"/>
-      <c r="E47" s="103"/>
-    </row>
-    <row r="48" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A48" s="78"/>
-      <c r="B48" s="79"/>
-      <c r="C48" s="73" t="s">
+      <c r="D48" s="67"/>
+      <c r="E48" s="68"/>
+    </row>
+    <row r="49" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1">
+      <c r="A49" s="71"/>
+      <c r="B49" s="72"/>
+      <c r="C49" s="66" t="s">
         <v>234</v>
       </c>
-      <c r="D48" s="74"/>
-      <c r="E48" s="75"/>
-    </row>
-    <row r="49" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A49" s="78"/>
-      <c r="B49" s="79"/>
-      <c r="C49" s="73" t="s">
-        <v>235</v>
-      </c>
-      <c r="D49" s="74"/>
-      <c r="E49" s="75"/>
+      <c r="D49" s="67"/>
+      <c r="E49" s="68"/>
     </row>
     <row r="50" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A50" s="78"/>
-      <c r="B50" s="79"/>
+      <c r="A50" s="71"/>
+      <c r="B50" s="72"/>
       <c r="C50" s="27"/>
       <c r="D50" s="3" t="s">
         <v>78</v>
@@ -3627,8 +3630,8 @@
       </c>
     </row>
     <row r="51" spans="1:5" s="4" customFormat="1">
-      <c r="A51" s="78"/>
-      <c r="B51" s="79"/>
+      <c r="A51" s="71"/>
+      <c r="B51" s="72"/>
       <c r="C51" s="27"/>
       <c r="D51" s="3" t="s">
         <v>80</v>
@@ -3636,8 +3639,8 @@
       <c r="E51" s="10"/>
     </row>
     <row r="52" spans="1:5" s="4" customFormat="1">
-      <c r="A52" s="78"/>
-      <c r="B52" s="79"/>
+      <c r="A52" s="71"/>
+      <c r="B52" s="72"/>
       <c r="C52" s="27"/>
       <c r="D52" s="3" t="s">
         <v>81</v>
@@ -3647,8 +3650,8 @@
       </c>
     </row>
     <row r="53" spans="1:5" s="4" customFormat="1">
-      <c r="A53" s="78"/>
-      <c r="B53" s="79"/>
+      <c r="A53" s="71"/>
+      <c r="B53" s="72"/>
       <c r="C53" s="27"/>
       <c r="D53" s="3" t="s">
         <v>83</v>
@@ -3658,8 +3661,8 @@
       </c>
     </row>
     <row r="54" spans="1:5" s="4" customFormat="1">
-      <c r="A54" s="78"/>
-      <c r="B54" s="79"/>
+      <c r="A54" s="71"/>
+      <c r="B54" s="72"/>
       <c r="C54" s="27"/>
       <c r="D54" s="3" t="s">
         <v>84</v>
@@ -3669,8 +3672,8 @@
       </c>
     </row>
     <row r="55" spans="1:5" s="4" customFormat="1">
-      <c r="A55" s="78"/>
-      <c r="B55" s="79"/>
+      <c r="A55" s="71"/>
+      <c r="B55" s="72"/>
       <c r="C55" s="27"/>
       <c r="D55" s="3" t="s">
         <v>85</v>
@@ -3680,59 +3683,59 @@
       </c>
     </row>
     <row r="56" spans="1:5" s="4" customFormat="1">
-      <c r="A56" s="78"/>
-      <c r="B56" s="79"/>
+      <c r="A56" s="71"/>
+      <c r="B56" s="72"/>
       <c r="C56" s="48"/>
       <c r="D56" s="48" t="s">
+        <v>414</v>
+      </c>
+      <c r="E56" s="48" t="s">
         <v>415</v>
-      </c>
-      <c r="E56" s="48" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="16.5" customHeight="1">
       <c r="A57" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B57" s="8">
         <v>3</v>
       </c>
-      <c r="C57" s="73" t="s">
+      <c r="C57" s="66" t="s">
+        <v>232</v>
+      </c>
+      <c r="D57" s="67"/>
+      <c r="E57" s="68"/>
+    </row>
+    <row r="58" spans="1:5" ht="16.5" customHeight="1">
+      <c r="A58" s="55"/>
+      <c r="B58" s="56"/>
+      <c r="C58" s="76" t="s">
+        <v>235</v>
+      </c>
+      <c r="D58" s="77"/>
+      <c r="E58" s="78"/>
+    </row>
+    <row r="59" spans="1:5" ht="16.5" customHeight="1">
+      <c r="A59" s="57"/>
+      <c r="B59" s="58"/>
+      <c r="C59" s="66" t="s">
         <v>233</v>
       </c>
-      <c r="D57" s="74"/>
-      <c r="E57" s="75"/>
-    </row>
-    <row r="58" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A58" s="97"/>
-      <c r="B58" s="56"/>
-      <c r="C58" s="63" t="s">
-        <v>236</v>
-      </c>
-      <c r="D58" s="64"/>
-      <c r="E58" s="65"/>
-    </row>
-    <row r="59" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A59" s="53"/>
-      <c r="B59" s="54"/>
-      <c r="C59" s="73" t="s">
+      <c r="D59" s="67"/>
+      <c r="E59" s="68"/>
+    </row>
+    <row r="60" spans="1:5" ht="16.5" customHeight="1">
+      <c r="A60" s="57"/>
+      <c r="B60" s="58"/>
+      <c r="C60" s="66" t="s">
         <v>234</v>
       </c>
-      <c r="D59" s="74"/>
-      <c r="E59" s="75"/>
-    </row>
-    <row r="60" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A60" s="53"/>
-      <c r="B60" s="54"/>
-      <c r="C60" s="73" t="s">
-        <v>235</v>
-      </c>
-      <c r="D60" s="74"/>
-      <c r="E60" s="75"/>
+      <c r="D60" s="67"/>
+      <c r="E60" s="68"/>
     </row>
     <row r="61" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A61" s="53"/>
-      <c r="B61" s="54"/>
+      <c r="A61" s="57"/>
+      <c r="B61" s="58"/>
       <c r="C61" s="20"/>
       <c r="D61" s="3" t="s">
         <v>13</v>
@@ -3740,8 +3743,8 @@
       <c r="E61" s="10"/>
     </row>
     <row r="62" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A62" s="53"/>
-      <c r="B62" s="54"/>
+      <c r="A62" s="57"/>
+      <c r="B62" s="58"/>
       <c r="C62" s="19"/>
       <c r="D62" s="3" t="s">
         <v>3</v>
@@ -3749,8 +3752,8 @@
       <c r="E62" s="10"/>
     </row>
     <row r="63" spans="1:5">
-      <c r="A63" s="53"/>
-      <c r="B63" s="54"/>
+      <c r="A63" s="57"/>
+      <c r="B63" s="58"/>
       <c r="C63" s="19"/>
       <c r="D63" s="3" t="s">
         <v>12</v>
@@ -3758,8 +3761,8 @@
       <c r="E63" s="10"/>
     </row>
     <row r="64" spans="1:5">
-      <c r="A64" s="53"/>
-      <c r="B64" s="54"/>
+      <c r="A64" s="57"/>
+      <c r="B64" s="58"/>
       <c r="C64" s="19"/>
       <c r="D64" s="3" t="s">
         <v>11</v>
@@ -3767,8 +3770,8 @@
       <c r="E64" s="10"/>
     </row>
     <row r="65" spans="1:5">
-      <c r="A65" s="53"/>
-      <c r="B65" s="54"/>
+      <c r="A65" s="57"/>
+      <c r="B65" s="58"/>
       <c r="C65" s="19"/>
       <c r="D65" s="3" t="s">
         <v>10</v>
@@ -3776,8 +3779,8 @@
       <c r="E65" s="10"/>
     </row>
     <row r="66" spans="1:5">
-      <c r="A66" s="53"/>
-      <c r="B66" s="54"/>
+      <c r="A66" s="57"/>
+      <c r="B66" s="58"/>
       <c r="C66" s="19"/>
       <c r="D66" s="3" t="s">
         <v>9</v>
@@ -3785,8 +3788,8 @@
       <c r="E66" s="10"/>
     </row>
     <row r="67" spans="1:5">
-      <c r="A67" s="53"/>
-      <c r="B67" s="54"/>
+      <c r="A67" s="57"/>
+      <c r="B67" s="58"/>
       <c r="C67" s="19"/>
       <c r="D67" s="3" t="s">
         <v>8</v>
@@ -3794,8 +3797,8 @@
       <c r="E67" s="10"/>
     </row>
     <row r="68" spans="1:5">
-      <c r="A68" s="53"/>
-      <c r="B68" s="54"/>
+      <c r="A68" s="57"/>
+      <c r="B68" s="58"/>
       <c r="C68" s="19"/>
       <c r="D68" s="3" t="s">
         <v>7</v>
@@ -3803,258 +3806,258 @@
       <c r="E68" s="10"/>
     </row>
     <row r="69" spans="1:5">
-      <c r="A69" s="53"/>
-      <c r="B69" s="54"/>
+      <c r="A69" s="57"/>
+      <c r="B69" s="58"/>
       <c r="C69" s="19"/>
       <c r="D69" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E69" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="70" spans="1:5">
-      <c r="A70" s="98"/>
-      <c r="B70" s="59"/>
+      <c r="A70" s="59"/>
+      <c r="B70" s="60"/>
       <c r="C70" s="19"/>
       <c r="D70" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E70" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="16" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B71" s="16">
         <v>7</v>
       </c>
-      <c r="C71" s="106" t="s">
-        <v>401</v>
-      </c>
-      <c r="D71" s="107"/>
-      <c r="E71" s="108"/>
+      <c r="C71" s="81" t="s">
+        <v>400</v>
+      </c>
+      <c r="D71" s="82"/>
+      <c r="E71" s="83"/>
     </row>
     <row r="72" spans="1:5">
-      <c r="A72" s="53"/>
-      <c r="B72" s="54"/>
+      <c r="A72" s="57"/>
+      <c r="B72" s="58"/>
       <c r="C72" s="49"/>
       <c r="D72" s="16" t="s">
+        <v>385</v>
+      </c>
+      <c r="E72" s="16" t="s">
         <v>386</v>
       </c>
-      <c r="E72" s="16" t="s">
-        <v>387</v>
-      </c>
     </row>
     <row r="73" spans="1:5">
-      <c r="A73" s="53"/>
-      <c r="B73" s="54"/>
+      <c r="A73" s="57"/>
+      <c r="B73" s="58"/>
       <c r="C73" s="50"/>
       <c r="D73" s="16" t="s">
+        <v>387</v>
+      </c>
+      <c r="E73" s="16" t="s">
         <v>388</v>
       </c>
-      <c r="E73" s="16" t="s">
-        <v>389</v>
-      </c>
     </row>
     <row r="74" spans="1:5">
-      <c r="A74" s="53"/>
-      <c r="B74" s="54"/>
+      <c r="A74" s="57"/>
+      <c r="B74" s="58"/>
       <c r="C74" s="50"/>
       <c r="D74" s="16" t="s">
+        <v>389</v>
+      </c>
+      <c r="E74" s="16" t="s">
         <v>390</v>
       </c>
-      <c r="E74" s="16" t="s">
-        <v>391</v>
-      </c>
     </row>
     <row r="75" spans="1:5">
-      <c r="A75" s="53"/>
-      <c r="B75" s="54"/>
+      <c r="A75" s="57"/>
+      <c r="B75" s="58"/>
       <c r="C75" s="52"/>
       <c r="D75" s="16" t="s">
+        <v>416</v>
+      </c>
+      <c r="E75" s="16" t="s">
         <v>417</v>
       </c>
-      <c r="E75" s="16" t="s">
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" s="57"/>
+      <c r="B76" s="58"/>
+      <c r="C76" s="51"/>
+      <c r="D76" s="53" t="s">
+        <v>395</v>
+      </c>
+      <c r="E76" s="53" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" s="57"/>
+      <c r="B77" s="58"/>
+      <c r="C77" s="51"/>
+      <c r="D77" s="53" t="s">
+        <v>391</v>
+      </c>
+      <c r="E77" s="53" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" s="57"/>
+      <c r="B78" s="58"/>
+      <c r="C78" s="54"/>
+      <c r="D78" s="53" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="76" spans="1:5">
-      <c r="A76" s="53"/>
-      <c r="B76" s="54"/>
-      <c r="C76" s="51"/>
-      <c r="D76" s="104" t="s">
-        <v>396</v>
-      </c>
-      <c r="E76" s="104" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5">
-      <c r="A77" s="53"/>
-      <c r="B77" s="54"/>
-      <c r="C77" s="51"/>
-      <c r="D77" s="104" t="s">
-        <v>392</v>
-      </c>
-      <c r="E77" s="104" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5">
-      <c r="A78" s="53"/>
-      <c r="B78" s="54"/>
-      <c r="C78" s="105"/>
-      <c r="D78" s="104" t="s">
+      <c r="E78" s="53" t="s">
         <v>419</v>
       </c>
-      <c r="E78" s="104" t="s">
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" s="57"/>
+      <c r="B79" s="58"/>
+      <c r="C79" s="54"/>
+      <c r="D79" s="53" t="s">
+        <v>424</v>
+      </c>
+      <c r="E79" s="53" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="79" spans="1:5">
-      <c r="A79" s="53"/>
-      <c r="B79" s="54"/>
-      <c r="C79" s="105"/>
-      <c r="D79" s="104" t="s">
-        <v>425</v>
-      </c>
-      <c r="E79" s="104" t="s">
-        <v>421</v>
-      </c>
-    </row>
     <row r="80" spans="1:5">
-      <c r="A80" s="53"/>
-      <c r="B80" s="54"/>
+      <c r="A80" s="57"/>
+      <c r="B80" s="58"/>
       <c r="C80" s="51"/>
       <c r="D80" s="16" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E80" s="16" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="81" spans="1:5">
-      <c r="A81" s="53"/>
-      <c r="B81" s="54"/>
+      <c r="A81" s="57"/>
+      <c r="B81" s="58"/>
       <c r="C81" s="51"/>
       <c r="D81" s="16" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E81" s="16" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="82" spans="1:5">
-      <c r="A82" s="53"/>
-      <c r="B82" s="54"/>
-      <c r="C82" s="105"/>
+      <c r="A82" s="57"/>
+      <c r="B82" s="58"/>
+      <c r="C82" s="54"/>
       <c r="D82" s="16" t="s">
+        <v>425</v>
+      </c>
+      <c r="E82" s="16" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" s="57"/>
+      <c r="B83" s="58"/>
+      <c r="C83" s="54"/>
+      <c r="D83" s="16" t="s">
         <v>426</v>
       </c>
-      <c r="E82" s="16" t="s">
+      <c r="E83" s="16" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="83" spans="1:5">
-      <c r="A83" s="53"/>
-      <c r="B83" s="54"/>
-      <c r="C83" s="105"/>
-      <c r="D83" s="16" t="s">
-        <v>427</v>
-      </c>
-      <c r="E83" s="16" t="s">
+    <row r="84" spans="1:5">
+      <c r="A84" s="57"/>
+      <c r="B84" s="58"/>
+      <c r="C84" s="45"/>
+      <c r="D84" s="53" t="s">
+        <v>397</v>
+      </c>
+      <c r="E84" s="53" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85" s="57"/>
+      <c r="B85" s="58"/>
+      <c r="C85" s="45"/>
+      <c r="D85" s="53" t="s">
+        <v>391</v>
+      </c>
+      <c r="E85" s="53" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" s="57"/>
+      <c r="B86" s="58"/>
+      <c r="C86" s="45"/>
+      <c r="D86" s="53" t="s">
+        <v>418</v>
+      </c>
+      <c r="E86" s="53" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" s="57"/>
+      <c r="B87" s="58"/>
+      <c r="C87" s="45"/>
+      <c r="D87" s="53" t="s">
+        <v>424</v>
+      </c>
+      <c r="E87" s="53" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="84" spans="1:5">
-      <c r="A84" s="53"/>
-      <c r="B84" s="54"/>
-      <c r="C84" s="45"/>
-      <c r="D84" s="104" t="s">
-        <v>398</v>
-      </c>
-      <c r="E84" s="104" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5">
-      <c r="A85" s="53"/>
-      <c r="B85" s="54"/>
-      <c r="C85" s="45"/>
-      <c r="D85" s="104" t="s">
-        <v>392</v>
-      </c>
-      <c r="E85" s="104" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5">
-      <c r="A86" s="53"/>
-      <c r="B86" s="54"/>
-      <c r="C86" s="45"/>
-      <c r="D86" s="104" t="s">
-        <v>419</v>
-      </c>
-      <c r="E86" s="104" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5">
-      <c r="A87" s="53"/>
-      <c r="B87" s="54"/>
-      <c r="C87" s="45"/>
-      <c r="D87" s="104" t="s">
-        <v>425</v>
-      </c>
-      <c r="E87" s="104" t="s">
-        <v>424</v>
-      </c>
-    </row>
     <row r="88" spans="1:5">
-      <c r="A88" s="53"/>
-      <c r="B88" s="54"/>
+      <c r="A88" s="57"/>
+      <c r="B88" s="58"/>
       <c r="C88" s="45"/>
       <c r="D88" s="16" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E88" s="16" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="89" spans="1:5">
-      <c r="A89" s="53"/>
-      <c r="B89" s="54"/>
+      <c r="A89" s="57"/>
+      <c r="B89" s="58"/>
       <c r="C89" s="45"/>
       <c r="D89" s="16" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E89" s="16" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="90" spans="1:5">
-      <c r="A90" s="53"/>
-      <c r="B90" s="54"/>
+      <c r="A90" s="57"/>
+      <c r="B90" s="58"/>
       <c r="C90" s="45"/>
       <c r="D90" s="16" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E90" s="16" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="91" spans="1:5">
-      <c r="A91" s="53"/>
-      <c r="B91" s="54"/>
+      <c r="A91" s="57"/>
+      <c r="B91" s="58"/>
       <c r="C91" s="45"/>
       <c r="D91" s="16" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E91" s="16" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="92" spans="1:5">
@@ -4064,233 +4067,233 @@
       <c r="B92" s="8">
         <v>7</v>
       </c>
-      <c r="C92" s="63" t="s">
-        <v>332</v>
-      </c>
-      <c r="D92" s="64"/>
-      <c r="E92" s="65"/>
+      <c r="C92" s="76" t="s">
+        <v>331</v>
+      </c>
+      <c r="D92" s="77"/>
+      <c r="E92" s="78"/>
     </row>
     <row r="93" spans="1:5">
-      <c r="A93" s="55"/>
+      <c r="A93" s="62"/>
       <c r="B93" s="56"/>
       <c r="C93" s="16"/>
       <c r="D93" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E93" s="10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="94" spans="1:5">
-      <c r="A94" s="57"/>
-      <c r="B94" s="54"/>
+      <c r="A94" s="65"/>
+      <c r="B94" s="58"/>
       <c r="C94" s="16"/>
       <c r="D94" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E94" s="10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="95" spans="1:5">
-      <c r="A95" s="57"/>
-      <c r="B95" s="54"/>
+      <c r="A95" s="65"/>
+      <c r="B95" s="58"/>
       <c r="C95" s="16"/>
       <c r="D95" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="E95" s="10" t="s">
         <v>251</v>
       </c>
-      <c r="E95" s="10" t="s">
-        <v>252</v>
-      </c>
     </row>
     <row r="96" spans="1:5">
-      <c r="A96" s="57"/>
-      <c r="B96" s="54"/>
+      <c r="A96" s="65"/>
+      <c r="B96" s="58"/>
       <c r="C96" s="16"/>
       <c r="D96" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E96" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="97" spans="1:5">
-      <c r="A97" s="57"/>
-      <c r="B97" s="54"/>
+      <c r="A97" s="65"/>
+      <c r="B97" s="58"/>
       <c r="C97" s="16"/>
       <c r="D97" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E97" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="53.25" customHeight="1">
-      <c r="A98" s="57"/>
-      <c r="B98" s="54"/>
+      <c r="A98" s="65"/>
+      <c r="B98" s="58"/>
       <c r="C98" s="16"/>
       <c r="D98" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E98" s="10" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="99" spans="1:5">
-      <c r="A99" s="57"/>
-      <c r="B99" s="54"/>
+      <c r="A99" s="65"/>
+      <c r="B99" s="58"/>
       <c r="C99" s="16"/>
       <c r="D99" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E99" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="30">
-      <c r="A100" s="58"/>
-      <c r="B100" s="59"/>
+      <c r="A100" s="64"/>
+      <c r="B100" s="60"/>
       <c r="C100" s="16"/>
       <c r="D100" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E100" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="B101" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="B101" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="C101" s="60"/>
-      <c r="D101" s="61"/>
-      <c r="E101" s="61"/>
+      <c r="C101" s="79"/>
+      <c r="D101" s="80"/>
+      <c r="E101" s="80"/>
     </row>
     <row r="102" spans="1:5">
-      <c r="A102" s="55"/>
+      <c r="A102" s="62"/>
       <c r="B102" s="56"/>
       <c r="C102" s="16"/>
       <c r="D102" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="E102" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="E102" s="10" t="s">
-        <v>145</v>
-      </c>
     </row>
     <row r="103" spans="1:5">
-      <c r="A103" s="57"/>
-      <c r="B103" s="54"/>
+      <c r="A103" s="65"/>
+      <c r="B103" s="58"/>
       <c r="C103" s="16"/>
       <c r="D103" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E103" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="104" spans="1:5">
-      <c r="A104" s="57"/>
-      <c r="B104" s="54"/>
+      <c r="A104" s="65"/>
+      <c r="B104" s="58"/>
       <c r="C104" s="16"/>
       <c r="D104" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E104" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="30">
-      <c r="A105" s="57"/>
-      <c r="B105" s="54"/>
+      <c r="A105" s="65"/>
+      <c r="B105" s="58"/>
       <c r="C105" s="16"/>
       <c r="D105" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="E105" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="E105" s="10" t="s">
-        <v>150</v>
-      </c>
     </row>
     <row r="106" spans="1:5" ht="30">
-      <c r="A106" s="57"/>
-      <c r="B106" s="54"/>
+      <c r="A106" s="65"/>
+      <c r="B106" s="58"/>
       <c r="C106" s="16"/>
       <c r="D106" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="E106" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="E106" s="10" t="s">
-        <v>152</v>
-      </c>
     </row>
     <row r="107" spans="1:5">
-      <c r="A107" s="57"/>
-      <c r="B107" s="54"/>
+      <c r="A107" s="65"/>
+      <c r="B107" s="58"/>
       <c r="C107" s="16"/>
       <c r="D107" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E107" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="E107" s="10" t="s">
-        <v>154</v>
-      </c>
     </row>
     <row r="108" spans="1:5" ht="30">
-      <c r="A108" s="58"/>
-      <c r="B108" s="59"/>
+      <c r="A108" s="64"/>
+      <c r="B108" s="60"/>
       <c r="C108" s="16"/>
       <c r="D108" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="E108" s="10" t="s">
         <v>155</v>
-      </c>
-      <c r="E108" s="10" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="9" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B109" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="C109" s="99" t="s">
-        <v>362</v>
-      </c>
-      <c r="D109" s="99"/>
-      <c r="E109" s="99"/>
+      <c r="C109" s="61" t="s">
+        <v>361</v>
+      </c>
+      <c r="D109" s="61"/>
+      <c r="E109" s="61"/>
     </row>
     <row r="110" spans="1:5" ht="15" customHeight="1">
-      <c r="A110" s="55"/>
+      <c r="A110" s="62"/>
       <c r="B110" s="56"/>
-      <c r="C110" s="99" t="s">
-        <v>361</v>
-      </c>
-      <c r="D110" s="99"/>
-      <c r="E110" s="99"/>
+      <c r="C110" s="61" t="s">
+        <v>360</v>
+      </c>
+      <c r="D110" s="61"/>
+      <c r="E110" s="61"/>
     </row>
     <row r="111" spans="1:5">
-      <c r="A111" s="100"/>
-      <c r="B111" s="54"/>
+      <c r="A111" s="63"/>
+      <c r="B111" s="58"/>
       <c r="C111" s="47"/>
       <c r="D111" s="47" t="s">
         <v>107</v>
       </c>
       <c r="E111" s="47" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="45">
-      <c r="A112" s="100"/>
-      <c r="B112" s="54"/>
+      <c r="A112" s="63"/>
+      <c r="B112" s="58"/>
       <c r="C112" s="45"/>
       <c r="D112" s="42" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E112" s="43"/>
     </row>
     <row r="113" spans="1:5" ht="45">
-      <c r="A113" s="100"/>
-      <c r="B113" s="54"/>
+      <c r="A113" s="63"/>
+      <c r="B113" s="58"/>
       <c r="C113" s="45"/>
       <c r="D113" s="42" t="s">
         <v>108</v>
@@ -4298,30 +4301,30 @@
       <c r="E113" s="43"/>
     </row>
     <row r="114" spans="1:5" ht="45">
-      <c r="A114" s="100"/>
-      <c r="B114" s="54"/>
+      <c r="A114" s="63"/>
+      <c r="B114" s="58"/>
       <c r="C114" s="45"/>
       <c r="D114" s="42" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E114" s="43" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="75">
-      <c r="A115" s="100"/>
-      <c r="B115" s="54"/>
+      <c r="A115" s="63"/>
+      <c r="B115" s="58"/>
       <c r="C115" s="45"/>
       <c r="D115" s="42" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E115" s="43" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="45">
-      <c r="A116" s="58"/>
-      <c r="B116" s="59"/>
+      <c r="A116" s="64"/>
+      <c r="B116" s="60"/>
       <c r="C116"/>
       <c r="D116" s="42" t="s">
         <v>106</v>
@@ -4330,17 +4333,17 @@
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="9" t="s">
-        <v>114</v>
+        <v>427</v>
       </c>
       <c r="B117" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C117" s="94"/>
-      <c r="D117" s="95"/>
-      <c r="E117" s="96"/>
+      <c r="C117" s="85"/>
+      <c r="D117" s="86"/>
+      <c r="E117" s="87"/>
     </row>
     <row r="118" spans="1:5">
-      <c r="A118" s="55"/>
+      <c r="A118" s="62"/>
       <c r="B118" s="56"/>
       <c r="C118" s="16"/>
       <c r="D118" s="3" t="s">
@@ -4351,36 +4354,36 @@
       </c>
     </row>
     <row r="119" spans="1:5">
-      <c r="A119" s="57"/>
-      <c r="B119" s="54"/>
+      <c r="A119" s="65"/>
+      <c r="B119" s="58"/>
       <c r="C119" s="16"/>
       <c r="D119" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E119" s="10" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="120" spans="1:5">
-      <c r="A120" s="57"/>
-      <c r="B120" s="54"/>
+      <c r="A120" s="65"/>
+      <c r="B120" s="58"/>
       <c r="C120" s="16"/>
       <c r="D120" s="3" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E120" s="10" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="45">
-      <c r="A121" s="58"/>
-      <c r="B121" s="59"/>
+      <c r="A121" s="64"/>
+      <c r="B121" s="60"/>
       <c r="C121" s="16"/>
-      <c r="D121" s="3" t="s">
-        <v>128</v>
+      <c r="D121" s="109" t="s">
+        <v>127</v>
       </c>
       <c r="E121" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="122" spans="1:5">
@@ -4390,14 +4393,14 @@
       <c r="B122" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C122" s="63" t="s">
+      <c r="C122" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="D122" s="64"/>
-      <c r="E122" s="65"/>
+      <c r="D122" s="77"/>
+      <c r="E122" s="78"/>
     </row>
     <row r="123" spans="1:5" ht="45">
-      <c r="A123" s="55"/>
+      <c r="A123" s="62"/>
       <c r="B123" s="56"/>
       <c r="C123" s="16"/>
       <c r="D123" s="3" t="s">
@@ -4408,8 +4411,8 @@
       </c>
     </row>
     <row r="124" spans="1:5" ht="45">
-      <c r="A124" s="57"/>
-      <c r="B124" s="54"/>
+      <c r="A124" s="65"/>
+      <c r="B124" s="58"/>
       <c r="C124" s="16"/>
       <c r="D124" s="3" t="s">
         <v>111</v>
@@ -4419,8 +4422,8 @@
       </c>
     </row>
     <row r="125" spans="1:5">
-      <c r="A125" s="57"/>
-      <c r="B125" s="54"/>
+      <c r="A125" s="65"/>
+      <c r="B125" s="58"/>
       <c r="C125" s="16"/>
       <c r="D125" s="3" t="s">
         <v>104</v>
@@ -4430,296 +4433,296 @@
       </c>
     </row>
     <row r="126" spans="1:5">
-      <c r="A126" s="57"/>
-      <c r="B126" s="54"/>
+      <c r="A126" s="65"/>
+      <c r="B126" s="58"/>
       <c r="C126" s="16"/>
       <c r="D126" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E126" s="10"/>
     </row>
     <row r="127" spans="1:5">
-      <c r="A127" s="57"/>
-      <c r="B127" s="54"/>
+      <c r="A127" s="65"/>
+      <c r="B127" s="58"/>
       <c r="C127" s="16"/>
       <c r="D127" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E127" s="10"/>
     </row>
     <row r="128" spans="1:5" ht="45">
-      <c r="A128" s="57"/>
-      <c r="B128" s="54"/>
+      <c r="A128" s="65"/>
+      <c r="B128" s="58"/>
       <c r="C128" s="16"/>
       <c r="D128" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E128" s="10" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="45">
-      <c r="A129" s="57"/>
-      <c r="B129" s="54"/>
+      <c r="A129" s="65"/>
+      <c r="B129" s="58"/>
       <c r="C129" s="16"/>
       <c r="D129" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E129" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="E129" s="10" t="s">
-        <v>139</v>
-      </c>
     </row>
     <row r="130" spans="1:5">
-      <c r="A130" s="57"/>
-      <c r="B130" s="54"/>
+      <c r="A130" s="65"/>
+      <c r="B130" s="58"/>
       <c r="C130" s="16"/>
       <c r="D130" s="33" t="s">
         <v>58</v>
       </c>
       <c r="E130" s="12" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="45">
-      <c r="A131" s="57"/>
-      <c r="B131" s="54"/>
+      <c r="A131" s="65"/>
+      <c r="B131" s="58"/>
       <c r="C131" s="16"/>
       <c r="D131" s="3" t="s">
         <v>105</v>
       </c>
       <c r="E131" s="10" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="132" spans="1:5">
-      <c r="A132" s="57"/>
-      <c r="B132" s="54"/>
+      <c r="A132" s="65"/>
+      <c r="B132" s="58"/>
       <c r="C132" s="16"/>
       <c r="D132" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="E132" s="10" t="s">
         <v>286</v>
       </c>
-      <c r="E132" s="10" t="s">
-        <v>287</v>
-      </c>
     </row>
     <row r="133" spans="1:5">
-      <c r="A133" s="57"/>
-      <c r="B133" s="54"/>
+      <c r="A133" s="65"/>
+      <c r="B133" s="58"/>
       <c r="C133" s="16"/>
       <c r="D133" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E133" s="10" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="134" spans="1:5">
-      <c r="A134" s="57"/>
-      <c r="B134" s="54"/>
+      <c r="A134" s="65"/>
+      <c r="B134" s="58"/>
       <c r="C134" s="16"/>
       <c r="D134" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="E134" s="10" t="s">
         <v>283</v>
       </c>
-      <c r="E134" s="10" t="s">
-        <v>284</v>
-      </c>
     </row>
     <row r="135" spans="1:5">
-      <c r="A135" s="57"/>
-      <c r="B135" s="54"/>
+      <c r="A135" s="65"/>
+      <c r="B135" s="58"/>
       <c r="C135" s="16"/>
       <c r="D135" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E135" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="E135" s="10" t="s">
-        <v>141</v>
-      </c>
     </row>
     <row r="136" spans="1:5">
-      <c r="A136" s="57"/>
-      <c r="B136" s="54"/>
+      <c r="A136" s="65"/>
+      <c r="B136" s="58"/>
       <c r="C136" s="16"/>
       <c r="D136" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E136" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="137" spans="1:5" ht="30">
-      <c r="A137" s="57"/>
-      <c r="B137" s="54"/>
+      <c r="A137" s="65"/>
+      <c r="B137" s="58"/>
       <c r="C137" s="16"/>
       <c r="D137" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E137" s="10" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="138" spans="1:5" ht="30">
-      <c r="A138" s="57"/>
-      <c r="B138" s="54"/>
+      <c r="A138" s="65"/>
+      <c r="B138" s="58"/>
       <c r="C138" s="16"/>
       <c r="D138" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E138" s="10" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="139" spans="1:5" ht="30">
-      <c r="A139" s="57"/>
-      <c r="B139" s="54"/>
+      <c r="A139" s="65"/>
+      <c r="B139" s="58"/>
       <c r="C139" s="16"/>
       <c r="D139" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E139" s="10" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="140" spans="1:5" ht="30">
-      <c r="A140" s="57"/>
-      <c r="B140" s="54"/>
+      <c r="A140" s="65"/>
+      <c r="B140" s="58"/>
       <c r="C140" s="16"/>
       <c r="D140" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E140" s="10" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="141" spans="1:5" ht="15" customHeight="1">
-      <c r="A141" s="57"/>
-      <c r="B141" s="54"/>
+      <c r="A141" s="65"/>
+      <c r="B141" s="58"/>
       <c r="C141" s="16"/>
       <c r="D141" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E141" s="10" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="142" spans="1:5" ht="15" customHeight="1">
-      <c r="A142" s="58"/>
-      <c r="B142" s="59"/>
+      <c r="A142" s="64"/>
+      <c r="B142" s="60"/>
       <c r="C142" s="16"/>
       <c r="D142" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E142" s="10" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="143" spans="1:5" ht="15" customHeight="1">
       <c r="A143" s="9" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B143" s="9">
         <v>5</v>
       </c>
-      <c r="C143" s="94"/>
-      <c r="D143" s="95"/>
-      <c r="E143" s="96"/>
+      <c r="C143" s="85"/>
+      <c r="D143" s="86"/>
+      <c r="E143" s="87"/>
     </row>
     <row r="144" spans="1:5" ht="15" customHeight="1">
-      <c r="A144" s="55"/>
+      <c r="A144" s="62"/>
       <c r="B144" s="56"/>
       <c r="C144" s="16"/>
       <c r="D144" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E144" s="10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="145" spans="1:5">
-      <c r="A145" s="57"/>
-      <c r="B145" s="54"/>
+      <c r="A145" s="65"/>
+      <c r="B145" s="58"/>
       <c r="C145" s="16"/>
       <c r="D145" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E145" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="E145" s="10" t="s">
-        <v>187</v>
-      </c>
     </row>
     <row r="146" spans="1:5">
-      <c r="A146" s="57"/>
-      <c r="B146" s="54"/>
+      <c r="A146" s="65"/>
+      <c r="B146" s="58"/>
       <c r="C146" s="16"/>
       <c r="D146" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E146" s="10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="147" spans="1:5">
-      <c r="A147" s="57"/>
-      <c r="B147" s="54"/>
+      <c r="A147" s="65"/>
+      <c r="B147" s="58"/>
       <c r="C147" s="16"/>
       <c r="D147" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E147" s="10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="148" spans="1:5">
-      <c r="A148" s="57"/>
-      <c r="B148" s="54"/>
+      <c r="A148" s="65"/>
+      <c r="B148" s="58"/>
       <c r="C148" s="16"/>
       <c r="D148" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="E148" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="E148" s="10" t="s">
-        <v>190</v>
-      </c>
     </row>
     <row r="149" spans="1:5">
-      <c r="A149" s="57"/>
-      <c r="B149" s="54"/>
+      <c r="A149" s="65"/>
+      <c r="B149" s="58"/>
       <c r="C149" s="16"/>
       <c r="D149" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E149" s="10" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="150" spans="1:5">
-      <c r="A150" s="58"/>
-      <c r="B150" s="59"/>
+      <c r="A150" s="64"/>
+      <c r="B150" s="60"/>
       <c r="C150" s="16"/>
       <c r="D150" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="E150" s="10" t="s">
         <v>192</v>
-      </c>
-      <c r="E150" s="10" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="151" spans="1:5">
       <c r="A151" s="9" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B151" s="8">
         <v>5</v>
       </c>
-      <c r="C151" s="60"/>
-      <c r="D151" s="61"/>
-      <c r="E151" s="62"/>
+      <c r="C151" s="79"/>
+      <c r="D151" s="80"/>
+      <c r="E151" s="84"/>
     </row>
     <row r="152" spans="1:5">
-      <c r="A152" s="94"/>
-      <c r="B152" s="96"/>
+      <c r="A152" s="85"/>
+      <c r="B152" s="87"/>
       <c r="C152" s="41"/>
       <c r="D152" s="33" t="s">
+        <v>198</v>
+      </c>
+      <c r="E152" s="10" t="s">
         <v>199</v>
-      </c>
-      <c r="E152" s="10" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="153" spans="1:5">
@@ -4729,36 +4732,36 @@
       <c r="B153" s="8">
         <v>4</v>
       </c>
-      <c r="C153" s="60" t="s">
-        <v>322</v>
-      </c>
-      <c r="D153" s="61"/>
-      <c r="E153" s="62"/>
+      <c r="C153" s="79" t="s">
+        <v>321</v>
+      </c>
+      <c r="D153" s="80"/>
+      <c r="E153" s="84"/>
     </row>
     <row r="154" spans="1:5">
       <c r="A154" s="25"/>
       <c r="B154" s="26"/>
-      <c r="C154" s="60" t="s">
+      <c r="C154" s="79" t="s">
+        <v>322</v>
+      </c>
+      <c r="D154" s="80"/>
+      <c r="E154" s="84"/>
+    </row>
+    <row r="155" spans="1:5">
+      <c r="C155" s="79" t="s">
         <v>323</v>
       </c>
-      <c r="D154" s="61"/>
-      <c r="E154" s="62"/>
-    </row>
-    <row r="155" spans="1:5">
-      <c r="C155" s="60" t="s">
-        <v>324</v>
-      </c>
-      <c r="D155" s="61"/>
-      <c r="E155" s="62"/>
+      <c r="D155" s="80"/>
+      <c r="E155" s="84"/>
     </row>
     <row r="156" spans="1:5">
       <c r="A156" s="37"/>
       <c r="B156" s="38"/>
-      <c r="C156" s="60" t="s">
-        <v>333</v>
-      </c>
-      <c r="D156" s="61"/>
-      <c r="E156" s="62"/>
+      <c r="C156" s="79" t="s">
+        <v>332</v>
+      </c>
+      <c r="D156" s="80"/>
+      <c r="E156" s="84"/>
     </row>
     <row r="157" spans="1:5">
       <c r="A157" s="39"/>
@@ -4774,7 +4777,7 @@
       <c r="B158" s="40"/>
       <c r="C158" s="16"/>
       <c r="D158" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E158" s="10"/>
     </row>
@@ -4792,7 +4795,7 @@
       <c r="B160" s="40"/>
       <c r="C160" s="16"/>
       <c r="D160" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E160" s="10"/>
     </row>
@@ -4801,7 +4804,7 @@
       <c r="B161" s="40"/>
       <c r="C161" s="16"/>
       <c r="D161" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E161" s="10"/>
     </row>
@@ -4810,7 +4813,7 @@
       <c r="B162" s="40"/>
       <c r="C162" s="16"/>
       <c r="D162" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E162" s="10"/>
     </row>
@@ -4828,7 +4831,7 @@
       <c r="B164" s="40"/>
       <c r="C164" s="16"/>
       <c r="D164" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E164" s="10"/>
     </row>
@@ -4837,7 +4840,7 @@
       <c r="B165" s="40"/>
       <c r="C165" s="16"/>
       <c r="D165" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E165" s="10"/>
     </row>
@@ -4846,7 +4849,7 @@
       <c r="B166" s="40"/>
       <c r="C166" s="16"/>
       <c r="D166" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E166" s="10"/>
     </row>
@@ -4864,7 +4867,7 @@
       <c r="B168" s="40"/>
       <c r="C168" s="16"/>
       <c r="D168" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E168" s="10"/>
     </row>
@@ -4882,7 +4885,7 @@
       <c r="B170" s="40"/>
       <c r="C170" s="16"/>
       <c r="D170" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E170" s="10"/>
     </row>
@@ -4891,7 +4894,7 @@
       <c r="B171" s="40"/>
       <c r="C171" s="16"/>
       <c r="D171" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E171" s="10"/>
     </row>
@@ -4900,7 +4903,7 @@
       <c r="B172" s="40"/>
       <c r="C172" s="16"/>
       <c r="D172" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E172" s="10"/>
     </row>
@@ -4909,10 +4912,10 @@
       <c r="B173" s="40"/>
       <c r="C173" s="16"/>
       <c r="D173" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="E173" s="46" t="s">
         <v>334</v>
-      </c>
-      <c r="E173" s="46" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="174" spans="1:5">
@@ -4929,10 +4932,10 @@
       <c r="B175" s="40"/>
       <c r="C175" s="16"/>
       <c r="D175" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E175" s="10" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="176" spans="1:5">
@@ -4940,10 +4943,10 @@
       <c r="B176" s="40"/>
       <c r="C176" s="16"/>
       <c r="D176" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E176" s="46" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="177" spans="1:5">
@@ -4960,7 +4963,7 @@
       <c r="B178" s="40"/>
       <c r="C178" s="16"/>
       <c r="D178" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E178" s="10"/>
     </row>
@@ -4978,7 +4981,7 @@
       <c r="B180" s="40"/>
       <c r="C180" s="16"/>
       <c r="D180" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E180" s="10"/>
     </row>
@@ -4996,7 +4999,7 @@
       <c r="B182" s="40"/>
       <c r="C182" s="16"/>
       <c r="D182" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E182" s="10"/>
     </row>
@@ -5014,7 +5017,7 @@
       <c r="B184" s="40"/>
       <c r="C184" s="16"/>
       <c r="D184" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E184" s="10"/>
     </row>
@@ -5032,7 +5035,7 @@
       <c r="B186" s="40"/>
       <c r="C186" s="16"/>
       <c r="D186" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E186" s="10"/>
     </row>
@@ -5041,7 +5044,7 @@
       <c r="B187" s="40"/>
       <c r="C187" s="16"/>
       <c r="D187" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E187" s="10"/>
     </row>
@@ -5059,7 +5062,7 @@
       <c r="B189" s="40"/>
       <c r="C189" s="16"/>
       <c r="D189" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E189" s="10"/>
     </row>
@@ -5077,7 +5080,7 @@
       <c r="B191" s="40"/>
       <c r="C191" s="16"/>
       <c r="D191" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E191" s="10"/>
     </row>
@@ -5095,7 +5098,7 @@
       <c r="B193" s="40"/>
       <c r="C193" s="16"/>
       <c r="D193" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E193" s="10"/>
     </row>
@@ -5113,7 +5116,7 @@
       <c r="B195" s="40"/>
       <c r="C195" s="16"/>
       <c r="D195" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E195" s="10"/>
     </row>
@@ -5122,7 +5125,7 @@
       <c r="B196" s="40"/>
       <c r="C196" s="16"/>
       <c r="D196" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E196" s="10"/>
     </row>
@@ -5131,7 +5134,7 @@
       <c r="B197" s="40"/>
       <c r="C197" s="16"/>
       <c r="D197" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E197" s="10"/>
     </row>
@@ -5142,107 +5145,107 @@
       <c r="B198" s="8">
         <v>4</v>
       </c>
-      <c r="C198" s="60"/>
-      <c r="D198" s="61"/>
-      <c r="E198" s="62"/>
+      <c r="C198" s="79"/>
+      <c r="D198" s="80"/>
+      <c r="E198" s="84"/>
     </row>
     <row r="199" spans="1:5" ht="15" customHeight="1">
-      <c r="A199" s="55"/>
+      <c r="A199" s="62"/>
       <c r="B199" s="56"/>
       <c r="C199" s="16"/>
       <c r="D199" s="3" t="s">
         <v>40</v>
       </c>
       <c r="E199" s="12" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="200" spans="1:5">
-      <c r="A200" s="57"/>
-      <c r="B200" s="54"/>
+      <c r="A200" s="65"/>
+      <c r="B200" s="58"/>
       <c r="C200" s="16"/>
       <c r="D200" s="3" t="s">
         <v>41</v>
       </c>
       <c r="E200" s="12" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="201" spans="1:5" ht="45">
-      <c r="A201" s="57"/>
-      <c r="B201" s="54"/>
+      <c r="A201" s="65"/>
+      <c r="B201" s="58"/>
       <c r="C201" s="16"/>
       <c r="D201" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E201" s="10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="202" spans="1:5">
-      <c r="A202" s="57"/>
-      <c r="B202" s="54"/>
+      <c r="A202" s="65"/>
+      <c r="B202" s="58"/>
       <c r="C202" s="16"/>
       <c r="D202" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E202" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="E202" s="10" t="s">
-        <v>173</v>
-      </c>
     </row>
     <row r="203" spans="1:5" ht="30">
-      <c r="A203" s="57"/>
-      <c r="B203" s="54"/>
+      <c r="A203" s="65"/>
+      <c r="B203" s="58"/>
       <c r="C203" s="16"/>
       <c r="D203" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="E203" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="E203" s="10" t="s">
-        <v>175</v>
-      </c>
     </row>
     <row r="204" spans="1:5" ht="30">
-      <c r="A204" s="57"/>
-      <c r="B204" s="54"/>
+      <c r="A204" s="65"/>
+      <c r="B204" s="58"/>
       <c r="C204" s="16"/>
       <c r="D204" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="E204" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="E204" s="10" t="s">
-        <v>177</v>
-      </c>
     </row>
     <row r="205" spans="1:5" ht="30">
-      <c r="A205" s="57"/>
-      <c r="B205" s="54"/>
+      <c r="A205" s="65"/>
+      <c r="B205" s="58"/>
       <c r="C205" s="16"/>
       <c r="D205" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E205" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="206" spans="1:5" ht="30">
-      <c r="A206" s="57"/>
-      <c r="B206" s="54"/>
+      <c r="A206" s="65"/>
+      <c r="B206" s="58"/>
       <c r="C206" s="16"/>
       <c r="D206" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="E206" s="10" t="s">
         <v>180</v>
       </c>
-      <c r="E206" s="10" t="s">
-        <v>181</v>
-      </c>
     </row>
     <row r="207" spans="1:5" ht="45">
-      <c r="A207" s="58"/>
-      <c r="B207" s="59"/>
+      <c r="A207" s="64"/>
+      <c r="B207" s="60"/>
       <c r="C207" s="16"/>
       <c r="D207" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="E207" s="1" t="s">
         <v>305</v>
-      </c>
-      <c r="E207" s="1" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="208" spans="1:5">
@@ -5252,42 +5255,42 @@
       <c r="B208" s="8">
         <v>6</v>
       </c>
-      <c r="C208" s="60" t="s">
+      <c r="C208" s="79" t="s">
+        <v>321</v>
+      </c>
+      <c r="D208" s="80"/>
+      <c r="E208" s="84"/>
+    </row>
+    <row r="209" spans="1:5">
+      <c r="A209" s="62"/>
+      <c r="B209" s="56"/>
+      <c r="C209" s="79" t="s">
         <v>322</v>
       </c>
-      <c r="D208" s="61"/>
-      <c r="E208" s="62"/>
-    </row>
-    <row r="209" spans="1:5">
-      <c r="A209" s="55"/>
-      <c r="B209" s="56"/>
-      <c r="C209" s="60" t="s">
+      <c r="D209" s="80"/>
+      <c r="E209" s="84"/>
+    </row>
+    <row r="210" spans="1:5">
+      <c r="A210" s="65"/>
+      <c r="B210" s="58"/>
+      <c r="C210" s="79" t="s">
         <v>323</v>
       </c>
-      <c r="D209" s="61"/>
-      <c r="E209" s="62"/>
-    </row>
-    <row r="210" spans="1:5">
-      <c r="A210" s="57"/>
-      <c r="B210" s="54"/>
-      <c r="C210" s="60" t="s">
+      <c r="D210" s="80"/>
+      <c r="E210" s="84"/>
+    </row>
+    <row r="211" spans="1:5">
+      <c r="A211" s="65"/>
+      <c r="B211" s="58"/>
+      <c r="C211" s="79" t="s">
         <v>324</v>
       </c>
-      <c r="D210" s="61"/>
-      <c r="E210" s="62"/>
-    </row>
-    <row r="211" spans="1:5">
-      <c r="A211" s="57"/>
-      <c r="B211" s="54"/>
-      <c r="C211" s="60" t="s">
-        <v>325</v>
-      </c>
-      <c r="D211" s="61"/>
-      <c r="E211" s="62"/>
+      <c r="D211" s="80"/>
+      <c r="E211" s="84"/>
     </row>
     <row r="212" spans="1:5">
-      <c r="A212" s="57"/>
-      <c r="B212" s="54"/>
+      <c r="A212" s="65"/>
+      <c r="B212" s="58"/>
       <c r="C212" s="16"/>
       <c r="D212" s="3" t="s">
         <v>42</v>
@@ -5295,17 +5298,17 @@
       <c r="E212" s="10"/>
     </row>
     <row r="213" spans="1:5">
-      <c r="A213" s="57"/>
-      <c r="B213" s="54"/>
+      <c r="A213" s="65"/>
+      <c r="B213" s="58"/>
       <c r="C213" s="16"/>
       <c r="D213" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E213" s="10"/>
     </row>
     <row r="214" spans="1:5">
-      <c r="A214" s="57"/>
-      <c r="B214" s="54"/>
+      <c r="A214" s="65"/>
+      <c r="B214" s="58"/>
       <c r="C214" s="16"/>
       <c r="D214" s="3" t="s">
         <v>43</v>
@@ -5313,35 +5316,35 @@
       <c r="E214" s="10"/>
     </row>
     <row r="215" spans="1:5">
-      <c r="A215" s="57"/>
-      <c r="B215" s="54"/>
+      <c r="A215" s="65"/>
+      <c r="B215" s="58"/>
       <c r="C215" s="16"/>
       <c r="D215" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E215" s="10"/>
     </row>
     <row r="216" spans="1:5">
-      <c r="A216" s="57"/>
-      <c r="B216" s="54"/>
+      <c r="A216" s="65"/>
+      <c r="B216" s="58"/>
       <c r="C216" s="16"/>
       <c r="D216" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E216" s="10"/>
     </row>
     <row r="217" spans="1:5">
-      <c r="A217" s="57"/>
-      <c r="B217" s="54"/>
+      <c r="A217" s="65"/>
+      <c r="B217" s="58"/>
       <c r="C217" s="16"/>
       <c r="D217" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E217" s="10"/>
     </row>
     <row r="218" spans="1:5">
-      <c r="A218" s="57"/>
-      <c r="B218" s="54"/>
+      <c r="A218" s="65"/>
+      <c r="B218" s="58"/>
       <c r="C218" s="16"/>
       <c r="D218" s="3" t="s">
         <v>50</v>
@@ -5349,17 +5352,17 @@
       <c r="E218" s="10"/>
     </row>
     <row r="219" spans="1:5">
-      <c r="A219" s="57"/>
-      <c r="B219" s="54"/>
+      <c r="A219" s="65"/>
+      <c r="B219" s="58"/>
       <c r="C219" s="16"/>
       <c r="D219" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E219" s="10"/>
     </row>
     <row r="220" spans="1:5">
-      <c r="A220" s="57"/>
-      <c r="B220" s="54"/>
+      <c r="A220" s="65"/>
+      <c r="B220" s="58"/>
       <c r="C220" s="16"/>
       <c r="D220" s="3" t="s">
         <v>44</v>
@@ -5367,26 +5370,26 @@
       <c r="E220" s="10"/>
     </row>
     <row r="221" spans="1:5">
-      <c r="A221" s="57"/>
-      <c r="B221" s="54"/>
+      <c r="A221" s="65"/>
+      <c r="B221" s="58"/>
       <c r="C221" s="16"/>
       <c r="D221" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E221" s="10"/>
     </row>
     <row r="222" spans="1:5">
-      <c r="A222" s="57"/>
-      <c r="B222" s="54"/>
+      <c r="A222" s="65"/>
+      <c r="B222" s="58"/>
       <c r="C222" s="16"/>
       <c r="D222" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E222" s="10"/>
     </row>
     <row r="223" spans="1:5">
-      <c r="A223" s="57"/>
-      <c r="B223" s="54"/>
+      <c r="A223" s="65"/>
+      <c r="B223" s="58"/>
       <c r="C223" s="16"/>
       <c r="D223" s="3" t="s">
         <v>45</v>
@@ -5394,17 +5397,17 @@
       <c r="E223" s="10"/>
     </row>
     <row r="224" spans="1:5">
-      <c r="A224" s="57"/>
-      <c r="B224" s="54"/>
+      <c r="A224" s="65"/>
+      <c r="B224" s="58"/>
       <c r="C224" s="16"/>
       <c r="D224" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E224" s="10"/>
     </row>
     <row r="225" spans="1:5">
-      <c r="A225" s="57"/>
-      <c r="B225" s="54"/>
+      <c r="A225" s="65"/>
+      <c r="B225" s="58"/>
       <c r="C225" s="16"/>
       <c r="D225" s="3" t="s">
         <v>46</v>
@@ -5412,11 +5415,11 @@
       <c r="E225" s="10"/>
     </row>
     <row r="226" spans="1:5">
-      <c r="A226" s="58"/>
-      <c r="B226" s="59"/>
+      <c r="A226" s="64"/>
+      <c r="B226" s="60"/>
       <c r="C226" s="16"/>
       <c r="D226" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E226" s="10"/>
     </row>
@@ -5427,96 +5430,96 @@
       <c r="B227" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C227" s="60"/>
-      <c r="D227" s="61"/>
-      <c r="E227" s="62"/>
+      <c r="C227" s="79"/>
+      <c r="D227" s="80"/>
+      <c r="E227" s="84"/>
     </row>
     <row r="228" spans="1:5" ht="32.25">
-      <c r="A228" s="55"/>
+      <c r="A228" s="62"/>
       <c r="B228" s="56"/>
       <c r="C228" s="16"/>
       <c r="D228" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E228" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="E228" s="10" t="s">
-        <v>170</v>
-      </c>
     </row>
     <row r="229" spans="1:5" ht="34.5">
-      <c r="A229" s="57"/>
-      <c r="B229" s="54"/>
+      <c r="A229" s="65"/>
+      <c r="B229" s="58"/>
       <c r="C229" s="16"/>
       <c r="D229" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="E229" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="E229" s="10" t="s">
-        <v>168</v>
-      </c>
     </row>
     <row r="230" spans="1:5" ht="32.25">
-      <c r="A230" s="57"/>
-      <c r="B230" s="54"/>
+      <c r="A230" s="65"/>
+      <c r="B230" s="58"/>
       <c r="C230" s="16"/>
       <c r="D230" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="E230" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="E230" s="10" t="s">
-        <v>166</v>
-      </c>
     </row>
     <row r="231" spans="1:5">
-      <c r="A231" s="57"/>
-      <c r="B231" s="54"/>
+      <c r="A231" s="65"/>
+      <c r="B231" s="58"/>
       <c r="C231" s="16"/>
       <c r="D231" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="E231" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="E231" s="10" t="s">
-        <v>164</v>
-      </c>
     </row>
     <row r="232" spans="1:5">
-      <c r="A232" s="57"/>
-      <c r="B232" s="54"/>
+      <c r="A232" s="65"/>
+      <c r="B232" s="58"/>
       <c r="C232" s="16"/>
       <c r="D232" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E232" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="233" spans="1:5">
-      <c r="A233" s="57"/>
-      <c r="B233" s="54"/>
+      <c r="A233" s="65"/>
+      <c r="B233" s="58"/>
       <c r="C233" s="16"/>
       <c r="D233" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="E233" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="E233" s="10" t="s">
-        <v>161</v>
-      </c>
     </row>
     <row r="234" spans="1:5">
-      <c r="A234" s="57"/>
-      <c r="B234" s="54"/>
+      <c r="A234" s="65"/>
+      <c r="B234" s="58"/>
       <c r="C234" s="16"/>
       <c r="D234" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E234" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="235" spans="1:5" ht="17.25">
-      <c r="A235" s="58"/>
-      <c r="B235" s="59"/>
+      <c r="A235" s="64"/>
+      <c r="B235" s="60"/>
       <c r="C235" s="16"/>
       <c r="D235" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="E235" s="10" t="s">
         <v>157</v>
-      </c>
-      <c r="E235" s="10" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="236" spans="1:5">
@@ -5526,173 +5529,173 @@
       <c r="B236" s="8">
         <v>5</v>
       </c>
-      <c r="C236" s="60"/>
-      <c r="D236" s="61"/>
-      <c r="E236" s="62"/>
+      <c r="C236" s="79"/>
+      <c r="D236" s="80"/>
+      <c r="E236" s="84"/>
     </row>
     <row r="237" spans="1:5">
-      <c r="A237" s="55"/>
+      <c r="A237" s="62"/>
       <c r="B237" s="56"/>
       <c r="C237" s="16"/>
       <c r="D237" s="34" t="s">
         <v>57</v>
       </c>
       <c r="E237" s="12" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="238" spans="1:5">
-      <c r="A238" s="57"/>
-      <c r="B238" s="54"/>
+      <c r="A238" s="65"/>
+      <c r="B238" s="58"/>
       <c r="C238" s="16"/>
       <c r="D238" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="E238" s="10" t="s">
         <v>342</v>
       </c>
-      <c r="E238" s="10" t="s">
-        <v>343</v>
-      </c>
     </row>
     <row r="239" spans="1:5">
-      <c r="A239" s="57"/>
-      <c r="B239" s="54"/>
+      <c r="A239" s="65"/>
+      <c r="B239" s="58"/>
       <c r="C239" s="5"/>
       <c r="D239" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="E239" s="10" t="s">
         <v>270</v>
       </c>
-      <c r="E239" s="10" t="s">
-        <v>271</v>
-      </c>
     </row>
     <row r="240" spans="1:5">
-      <c r="A240" s="57"/>
-      <c r="B240" s="54"/>
+      <c r="A240" s="65"/>
+      <c r="B240" s="58"/>
       <c r="C240" s="5"/>
       <c r="D240" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="E240" s="10" t="s">
         <v>268</v>
       </c>
-      <c r="E240" s="10" t="s">
-        <v>269</v>
-      </c>
     </row>
     <row r="241" spans="1:5">
-      <c r="A241" s="57"/>
-      <c r="B241" s="54"/>
+      <c r="A241" s="65"/>
+      <c r="B241" s="58"/>
       <c r="C241" s="5"/>
       <c r="D241" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E241" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="242" spans="1:5">
-      <c r="A242" s="57"/>
-      <c r="B242" s="54"/>
+      <c r="A242" s="65"/>
+      <c r="B242" s="58"/>
       <c r="C242" s="5"/>
       <c r="D242" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E242" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="243" spans="1:5">
-      <c r="A243" s="57"/>
-      <c r="B243" s="54"/>
+      <c r="A243" s="65"/>
+      <c r="B243" s="58"/>
       <c r="C243" s="5"/>
       <c r="D243" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E243" s="10" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="244" spans="1:5">
-      <c r="A244" s="57"/>
-      <c r="B244" s="54"/>
+      <c r="A244" s="65"/>
+      <c r="B244" s="58"/>
       <c r="C244" s="5"/>
       <c r="D244" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E244" s="10" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="245" spans="1:5" ht="30">
-      <c r="A245" s="57"/>
-      <c r="B245" s="54"/>
+      <c r="A245" s="65"/>
+      <c r="B245" s="58"/>
       <c r="C245" s="5"/>
       <c r="D245" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E245" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="E245" s="10" t="s">
-        <v>118</v>
-      </c>
     </row>
     <row r="246" spans="1:5">
-      <c r="A246" s="57"/>
-      <c r="B246" s="54"/>
+      <c r="A246" s="65"/>
+      <c r="B246" s="58"/>
       <c r="C246" s="5"/>
       <c r="D246" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E246" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="247" spans="1:5">
-      <c r="A247" s="57"/>
-      <c r="B247" s="54"/>
+      <c r="A247" s="65"/>
+      <c r="B247" s="58"/>
       <c r="C247" s="5"/>
       <c r="D247" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="E247" s="10" t="s">
         <v>258</v>
       </c>
-      <c r="E247" s="10" t="s">
-        <v>259</v>
-      </c>
     </row>
     <row r="248" spans="1:5" ht="30">
-      <c r="A248" s="57"/>
-      <c r="B248" s="54"/>
+      <c r="A248" s="65"/>
+      <c r="B248" s="58"/>
       <c r="C248" s="5"/>
       <c r="D248" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="E248" s="10" t="s">
         <v>255</v>
       </c>
-      <c r="E248" s="10" t="s">
-        <v>256</v>
-      </c>
     </row>
     <row r="249" spans="1:5">
-      <c r="A249" s="57"/>
-      <c r="B249" s="54"/>
+      <c r="A249" s="65"/>
+      <c r="B249" s="58"/>
       <c r="C249" s="5"/>
       <c r="D249" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="E249" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="E249" s="10" t="s">
-        <v>183</v>
-      </c>
     </row>
     <row r="250" spans="1:5" ht="30">
-      <c r="A250" s="57"/>
-      <c r="B250" s="54"/>
+      <c r="A250" s="65"/>
+      <c r="B250" s="58"/>
       <c r="C250" s="5"/>
       <c r="D250" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E250" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="251" spans="1:5" ht="30">
-      <c r="A251" s="58"/>
-      <c r="B251" s="59"/>
+      <c r="A251" s="64"/>
+      <c r="B251" s="60"/>
       <c r="C251" s="16"/>
       <c r="D251" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E251" s="10" t="s">
         <v>120</v>
-      </c>
-      <c r="E251" s="10" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="252" spans="1:5">
@@ -5702,132 +5705,132 @@
       <c r="B252" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="C252" s="60"/>
-      <c r="D252" s="61"/>
-      <c r="E252" s="62"/>
+      <c r="C252" s="79"/>
+      <c r="D252" s="80"/>
+      <c r="E252" s="84"/>
     </row>
     <row r="253" spans="1:5" ht="15" customHeight="1">
-      <c r="A253" s="55"/>
+      <c r="A253" s="62"/>
       <c r="B253" s="56"/>
       <c r="C253" s="16"/>
       <c r="D253" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E253" s="10" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="254" spans="1:5" ht="15" customHeight="1">
-      <c r="A254" s="57"/>
-      <c r="B254" s="54"/>
+      <c r="A254" s="65"/>
+      <c r="B254" s="58"/>
       <c r="C254" s="16"/>
       <c r="D254" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E254" s="10" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="255" spans="1:5" ht="30">
-      <c r="A255" s="57"/>
-      <c r="B255" s="54"/>
+      <c r="A255" s="65"/>
+      <c r="B255" s="58"/>
       <c r="C255" s="16"/>
       <c r="D255" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E255" s="10" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="256" spans="1:5" ht="15" customHeight="1">
-      <c r="A256" s="57"/>
-      <c r="B256" s="54"/>
+      <c r="A256" s="65"/>
+      <c r="B256" s="58"/>
       <c r="C256" s="16"/>
       <c r="D256" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E256" s="10" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="257" spans="1:5" ht="15" customHeight="1">
-      <c r="A257" s="57"/>
-      <c r="B257" s="54"/>
+      <c r="A257" s="65"/>
+      <c r="B257" s="58"/>
       <c r="C257" s="16"/>
       <c r="D257" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="E257" s="10" t="s">
         <v>290</v>
       </c>
-      <c r="E257" s="10" t="s">
-        <v>291</v>
-      </c>
     </row>
     <row r="258" spans="1:5" ht="30">
-      <c r="A258" s="57"/>
-      <c r="B258" s="54"/>
+      <c r="A258" s="65"/>
+      <c r="B258" s="58"/>
       <c r="C258" s="16"/>
       <c r="D258" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E258" s="10" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="259" spans="1:5" ht="15" customHeight="1">
-      <c r="A259" s="57"/>
-      <c r="B259" s="54"/>
+      <c r="A259" s="65"/>
+      <c r="B259" s="58"/>
       <c r="C259" s="16"/>
       <c r="D259" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E259" s="10" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="260" spans="1:5" ht="15" customHeight="1">
-      <c r="A260" s="57"/>
-      <c r="B260" s="54"/>
+      <c r="A260" s="65"/>
+      <c r="B260" s="58"/>
       <c r="C260" s="16"/>
       <c r="D260" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E260" s="10"/>
     </row>
     <row r="261" spans="1:5" ht="15" customHeight="1">
-      <c r="A261" s="57"/>
-      <c r="B261" s="54"/>
+      <c r="A261" s="65"/>
+      <c r="B261" s="58"/>
       <c r="C261" s="16"/>
       <c r="D261" s="33" t="s">
+        <v>298</v>
+      </c>
+      <c r="E261" s="10" t="s">
         <v>299</v>
       </c>
-      <c r="E261" s="10" t="s">
-        <v>300</v>
-      </c>
     </row>
     <row r="262" spans="1:5" ht="15" customHeight="1">
-      <c r="A262" s="57"/>
-      <c r="B262" s="54"/>
+      <c r="A262" s="65"/>
+      <c r="B262" s="58"/>
       <c r="C262" s="16"/>
       <c r="D262" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E262" s="10" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="263" spans="1:5">
-      <c r="A263" s="57"/>
-      <c r="B263" s="54"/>
+      <c r="A263" s="65"/>
+      <c r="B263" s="58"/>
       <c r="C263" s="16"/>
       <c r="D263" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="E263" s="10" t="s">
         <v>302</v>
       </c>
-      <c r="E263" s="10" t="s">
-        <v>303</v>
-      </c>
     </row>
     <row r="264" spans="1:5" ht="15" customHeight="1">
-      <c r="A264" s="58"/>
-      <c r="B264" s="59"/>
+      <c r="A264" s="64"/>
+      <c r="B264" s="60"/>
       <c r="C264" s="16"/>
       <c r="D264" s="3" t="s">
         <v>76</v>
@@ -5841,27 +5844,27 @@
       <c r="B265" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="C265" s="60" t="s">
+      <c r="C265" s="79" t="s">
         <v>64</v>
       </c>
-      <c r="D265" s="61"/>
-      <c r="E265" s="62"/>
+      <c r="D265" s="80"/>
+      <c r="E265" s="84"/>
     </row>
     <row r="266" spans="1:5" ht="15" customHeight="1">
-      <c r="A266" s="55"/>
+      <c r="A266" s="62"/>
       <c r="B266" s="56"/>
-      <c r="C266" s="60" t="s">
+      <c r="C266" s="79" t="s">
         <v>65</v>
       </c>
-      <c r="D266" s="61"/>
-      <c r="E266" s="62"/>
+      <c r="D266" s="80"/>
+      <c r="E266" s="84"/>
     </row>
     <row r="267" spans="1:5">
-      <c r="A267" s="58"/>
-      <c r="B267" s="59"/>
+      <c r="A267" s="64"/>
+      <c r="B267" s="60"/>
       <c r="C267" s="16"/>
       <c r="D267" s="34" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E267" s="10"/>
     </row>
@@ -5872,27 +5875,27 @@
       <c r="B268" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C268" s="60" t="s">
-        <v>338</v>
-      </c>
-      <c r="D268" s="61"/>
-      <c r="E268" s="62"/>
+      <c r="C268" s="79" t="s">
+        <v>337</v>
+      </c>
+      <c r="D268" s="80"/>
+      <c r="E268" s="84"/>
     </row>
     <row r="269" spans="1:5">
-      <c r="A269" s="55"/>
+      <c r="A269" s="62"/>
       <c r="B269" s="56"/>
-      <c r="C269" s="60" t="s">
+      <c r="C269" s="79" t="s">
         <v>62</v>
       </c>
-      <c r="D269" s="61"/>
-      <c r="E269" s="62"/>
+      <c r="D269" s="80"/>
+      <c r="E269" s="84"/>
     </row>
     <row r="270" spans="1:5">
-      <c r="A270" s="58"/>
-      <c r="B270" s="59"/>
+      <c r="A270" s="64"/>
+      <c r="B270" s="60"/>
       <c r="C270" s="16"/>
       <c r="D270" s="34" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E270" s="10"/>
     </row>
@@ -5903,216 +5906,216 @@
       <c r="B271" s="8">
         <v>7</v>
       </c>
-      <c r="C271" s="60" t="s">
+      <c r="C271" s="79" t="s">
+        <v>310</v>
+      </c>
+      <c r="D271" s="80"/>
+      <c r="E271" s="84"/>
+    </row>
+    <row r="272" spans="1:5">
+      <c r="A272" s="62"/>
+      <c r="B272" s="56"/>
+      <c r="C272" s="76" t="s">
+        <v>66</v>
+      </c>
+      <c r="D272" s="77"/>
+      <c r="E272" s="77"/>
+    </row>
+    <row r="273" spans="1:5">
+      <c r="A273" s="65"/>
+      <c r="B273" s="58"/>
+      <c r="C273" s="76" t="s">
         <v>311</v>
       </c>
-      <c r="D271" s="61"/>
-      <c r="E271" s="62"/>
-    </row>
-    <row r="272" spans="1:5">
-      <c r="A272" s="55"/>
-      <c r="B272" s="56"/>
-      <c r="C272" s="63" t="s">
-        <v>66</v>
-      </c>
-      <c r="D272" s="64"/>
-      <c r="E272" s="64"/>
-    </row>
-    <row r="273" spans="1:5">
-      <c r="A273" s="57"/>
-      <c r="B273" s="54"/>
-      <c r="C273" s="63" t="s">
-        <v>312</v>
-      </c>
-      <c r="D273" s="64"/>
-      <c r="E273" s="65"/>
+      <c r="D273" s="77"/>
+      <c r="E273" s="78"/>
     </row>
     <row r="274" spans="1:5">
-      <c r="A274" s="57"/>
-      <c r="B274" s="54"/>
-      <c r="C274" s="63" t="s">
+      <c r="A274" s="65"/>
+      <c r="B274" s="58"/>
+      <c r="C274" s="76" t="s">
         <v>67</v>
       </c>
-      <c r="D274" s="64"/>
-      <c r="E274" s="65"/>
+      <c r="D274" s="77"/>
+      <c r="E274" s="78"/>
     </row>
     <row r="275" spans="1:5">
-      <c r="A275" s="58"/>
-      <c r="B275" s="59"/>
+      <c r="A275" s="64"/>
+      <c r="B275" s="60"/>
       <c r="C275" s="16"/>
       <c r="D275" s="34" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E275" s="10"/>
     </row>
     <row r="276" spans="1:5">
       <c r="A276" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="B276" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="B276" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="C276" s="60" t="s">
+      <c r="C276" s="79" t="s">
+        <v>307</v>
+      </c>
+      <c r="D276" s="80"/>
+      <c r="E276" s="84"/>
+    </row>
+    <row r="277" spans="1:5">
+      <c r="A277" s="62"/>
+      <c r="B277" s="56"/>
+      <c r="C277" s="79" t="s">
+        <v>309</v>
+      </c>
+      <c r="D277" s="80"/>
+      <c r="E277" s="84"/>
+    </row>
+    <row r="278" spans="1:5">
+      <c r="A278" s="65"/>
+      <c r="B278" s="58"/>
+      <c r="C278" s="79" t="s">
         <v>308</v>
       </c>
-      <c r="D276" s="61"/>
-      <c r="E276" s="62"/>
-    </row>
-    <row r="277" spans="1:5">
-      <c r="A277" s="55"/>
-      <c r="B277" s="56"/>
-      <c r="C277" s="60" t="s">
-        <v>310</v>
-      </c>
-      <c r="D277" s="61"/>
-      <c r="E277" s="62"/>
-    </row>
-    <row r="278" spans="1:5">
-      <c r="A278" s="57"/>
-      <c r="B278" s="54"/>
-      <c r="C278" s="60" t="s">
-        <v>309</v>
-      </c>
-      <c r="D278" s="61"/>
-      <c r="E278" s="62"/>
+      <c r="D278" s="80"/>
+      <c r="E278" s="84"/>
     </row>
     <row r="279" spans="1:5">
-      <c r="A279" s="58"/>
-      <c r="B279" s="59"/>
+      <c r="A279" s="64"/>
+      <c r="B279" s="60"/>
       <c r="C279" s="16"/>
       <c r="D279" s="34" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E279" s="10"/>
     </row>
     <row r="280" spans="1:5">
       <c r="A280" s="9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B280" s="8">
         <v>5</v>
       </c>
-      <c r="C280" s="63" t="s">
-        <v>346</v>
-      </c>
-      <c r="D280" s="64"/>
-      <c r="E280" s="65"/>
+      <c r="C280" s="76" t="s">
+        <v>345</v>
+      </c>
+      <c r="D280" s="77"/>
+      <c r="E280" s="78"/>
     </row>
     <row r="281" spans="1:5" ht="15" customHeight="1">
-      <c r="A281" s="55"/>
+      <c r="A281" s="62"/>
       <c r="B281" s="56"/>
       <c r="C281" s="3"/>
       <c r="D281" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E281" s="3"/>
     </row>
     <row r="282" spans="1:5">
-      <c r="A282" s="57"/>
-      <c r="B282" s="54"/>
+      <c r="A282" s="65"/>
+      <c r="B282" s="58"/>
       <c r="C282" s="3"/>
       <c r="D282" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E282" s="3"/>
     </row>
     <row r="283" spans="1:5" ht="30">
-      <c r="A283" s="57"/>
-      <c r="B283" s="54"/>
+      <c r="A283" s="65"/>
+      <c r="B283" s="58"/>
       <c r="C283" s="3"/>
       <c r="D283" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="E283" s="3" t="s">
         <v>340</v>
       </c>
-      <c r="E283" s="3" t="s">
-        <v>341</v>
-      </c>
     </row>
     <row r="284" spans="1:5">
-      <c r="A284" s="57"/>
-      <c r="B284" s="54"/>
+      <c r="A284" s="65"/>
+      <c r="B284" s="58"/>
       <c r="C284" s="3"/>
       <c r="D284" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E284" s="3"/>
     </row>
     <row r="285" spans="1:5">
-      <c r="A285" s="57"/>
-      <c r="B285" s="54"/>
+      <c r="A285" s="65"/>
+      <c r="B285" s="58"/>
       <c r="C285" s="3"/>
       <c r="D285" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E285" s="3"/>
     </row>
     <row r="286" spans="1:5">
-      <c r="A286" s="57"/>
-      <c r="B286" s="54"/>
+      <c r="A286" s="65"/>
+      <c r="B286" s="58"/>
       <c r="C286" s="3"/>
       <c r="D286" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="E286" s="3" t="s">
         <v>351</v>
       </c>
-      <c r="E286" s="3" t="s">
-        <v>352</v>
-      </c>
     </row>
     <row r="287" spans="1:5" ht="30">
-      <c r="A287" s="57"/>
-      <c r="B287" s="54"/>
+      <c r="A287" s="65"/>
+      <c r="B287" s="58"/>
       <c r="C287" s="3"/>
       <c r="D287" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E287" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="288" spans="1:5">
-      <c r="A288" s="57"/>
-      <c r="B288" s="54"/>
+      <c r="A288" s="65"/>
+      <c r="B288" s="58"/>
       <c r="C288" s="3"/>
       <c r="D288" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E288" s="3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="289" spans="1:5">
-      <c r="A289" s="58"/>
-      <c r="B289" s="59"/>
+      <c r="A289" s="64"/>
+      <c r="B289" s="60"/>
       <c r="C289" s="16"/>
       <c r="D289" s="34" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E289" s="10"/>
     </row>
     <row r="290" spans="1:5">
       <c r="A290" s="9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B290" s="9">
         <v>5</v>
       </c>
-      <c r="C290" s="60"/>
-      <c r="D290" s="61"/>
-      <c r="E290" s="62"/>
+      <c r="C290" s="79"/>
+      <c r="D290" s="80"/>
+      <c r="E290" s="84"/>
     </row>
     <row r="291" spans="1:5">
       <c r="A291" s="25"/>
       <c r="B291" s="26"/>
       <c r="C291" s="41"/>
       <c r="D291" s="36" t="s">
+        <v>196</v>
+      </c>
+      <c r="E291" s="11" t="s">
         <v>197</v>
-      </c>
-      <c r="E291" s="11" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="292" spans="1:5">
       <c r="C292" s="16"/>
       <c r="D292" s="34" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E292" s="10"/>
     </row>
@@ -6123,107 +6126,107 @@
       <c r="B293" s="8">
         <v>4</v>
       </c>
-      <c r="C293" s="63" t="s">
-        <v>337</v>
-      </c>
-      <c r="D293" s="64"/>
-      <c r="E293" s="65"/>
+      <c r="C293" s="76" t="s">
+        <v>336</v>
+      </c>
+      <c r="D293" s="77"/>
+      <c r="E293" s="78"/>
     </row>
     <row r="294" spans="1:5">
-      <c r="A294" s="55"/>
+      <c r="A294" s="62"/>
       <c r="B294" s="56"/>
       <c r="C294" s="16"/>
       <c r="D294" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E294" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="E294" s="10" t="s">
-        <v>137</v>
-      </c>
     </row>
     <row r="295" spans="1:5">
-      <c r="A295" s="58"/>
-      <c r="B295" s="59"/>
+      <c r="A295" s="64"/>
+      <c r="B295" s="60"/>
       <c r="C295" s="16"/>
       <c r="D295" s="34" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E295" s="10"/>
     </row>
     <row r="296" spans="1:5">
       <c r="A296" s="9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B296" s="8">
         <v>6</v>
       </c>
-      <c r="C296" s="60"/>
-      <c r="D296" s="61"/>
-      <c r="E296" s="62"/>
+      <c r="C296" s="79"/>
+      <c r="D296" s="80"/>
+      <c r="E296" s="84"/>
     </row>
     <row r="297" spans="1:5">
-      <c r="A297" s="55"/>
+      <c r="A297" s="62"/>
       <c r="B297" s="56"/>
       <c r="C297" s="16"/>
       <c r="D297" s="3" t="s">
         <v>47</v>
       </c>
       <c r="E297" s="12" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="298" spans="1:5">
-      <c r="A298" s="57"/>
-      <c r="B298" s="54"/>
+      <c r="A298" s="65"/>
+      <c r="B298" s="58"/>
       <c r="C298" s="16"/>
       <c r="D298" s="3" t="s">
         <v>48</v>
       </c>
       <c r="E298" s="12" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="299" spans="1:5">
-      <c r="A299" s="57"/>
-      <c r="B299" s="54"/>
+      <c r="A299" s="65"/>
+      <c r="B299" s="58"/>
       <c r="C299" s="16"/>
       <c r="D299" s="3" t="s">
         <v>49</v>
       </c>
       <c r="E299" s="12" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="300" spans="1:5">
-      <c r="A300" s="57"/>
-      <c r="B300" s="54"/>
+      <c r="A300" s="65"/>
+      <c r="B300" s="58"/>
       <c r="C300" s="16"/>
       <c r="D300" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E300" s="12" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="301" spans="1:5">
-      <c r="A301" s="57"/>
-      <c r="B301" s="54"/>
+      <c r="A301" s="65"/>
+      <c r="B301" s="58"/>
       <c r="C301" s="16"/>
       <c r="D301" s="3" t="s">
         <v>52</v>
       </c>
       <c r="E301" s="12" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="302" spans="1:5">
-      <c r="A302" s="58"/>
-      <c r="B302" s="59"/>
+      <c r="A302" s="64"/>
+      <c r="B302" s="60"/>
       <c r="C302" s="16"/>
       <c r="D302" s="3" t="s">
         <v>53</v>
       </c>
       <c r="E302" s="12" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="303" spans="1:5">
@@ -6233,73 +6236,73 @@
       <c r="B303" s="8">
         <v>7</v>
       </c>
-      <c r="C303" s="60"/>
-      <c r="D303" s="61"/>
-      <c r="E303" s="62"/>
+      <c r="C303" s="79"/>
+      <c r="D303" s="80"/>
+      <c r="E303" s="84"/>
     </row>
     <row r="304" spans="1:5">
-      <c r="A304" s="55"/>
+      <c r="A304" s="62"/>
       <c r="B304" s="56"/>
       <c r="C304" s="16"/>
       <c r="D304" s="3" t="s">
         <v>33</v>
       </c>
       <c r="E304" s="12" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="305" spans="1:5">
-      <c r="A305" s="57"/>
-      <c r="B305" s="54"/>
+      <c r="A305" s="65"/>
+      <c r="B305" s="58"/>
       <c r="C305" s="16"/>
       <c r="D305" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E305" s="12" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="306" spans="1:5">
-      <c r="A306" s="57"/>
-      <c r="B306" s="54"/>
+      <c r="A306" s="65"/>
+      <c r="B306" s="58"/>
       <c r="C306" s="16"/>
       <c r="D306" s="3" t="s">
         <v>35</v>
       </c>
       <c r="E306" s="12" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="307" spans="1:5">
-      <c r="A307" s="57"/>
-      <c r="B307" s="54"/>
+      <c r="A307" s="65"/>
+      <c r="B307" s="58"/>
       <c r="D307" s="3" t="s">
         <v>59</v>
       </c>
       <c r="E307" s="12" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="308" spans="1:5">
-      <c r="A308" s="57"/>
-      <c r="B308" s="54"/>
+      <c r="A308" s="65"/>
+      <c r="B308" s="58"/>
       <c r="C308" s="16"/>
       <c r="D308" s="3" t="s">
         <v>36</v>
       </c>
       <c r="E308" s="12" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="309" spans="1:5">
-      <c r="A309" s="57"/>
-      <c r="B309" s="54"/>
+      <c r="A309" s="65"/>
+      <c r="B309" s="58"/>
       <c r="C309" s="16"/>
       <c r="D309" s="3" t="s">
         <v>37</v>
       </c>
       <c r="E309" s="12" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="310" spans="1:5">
@@ -6312,6 +6315,72 @@
     </row>
   </sheetData>
   <mergeCells count="82">
+    <mergeCell ref="A72:B91"/>
+    <mergeCell ref="A93:B100"/>
+    <mergeCell ref="C303:E303"/>
+    <mergeCell ref="C155:E155"/>
+    <mergeCell ref="C210:E210"/>
+    <mergeCell ref="C209:E209"/>
+    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C265:E265"/>
+    <mergeCell ref="C268:E268"/>
+    <mergeCell ref="C266:E266"/>
+    <mergeCell ref="C276:E276"/>
+    <mergeCell ref="C293:E293"/>
+    <mergeCell ref="C271:E271"/>
+    <mergeCell ref="C227:E227"/>
+    <mergeCell ref="C156:E156"/>
+    <mergeCell ref="C296:E296"/>
+    <mergeCell ref="C198:E198"/>
+    <mergeCell ref="C280:E280"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="A6:B11"/>
+    <mergeCell ref="A35:B42"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="A13:B33"/>
+    <mergeCell ref="D6:D11"/>
+    <mergeCell ref="C6:C11"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="C252:E252"/>
+    <mergeCell ref="C269:E269"/>
+    <mergeCell ref="C290:E290"/>
+    <mergeCell ref="C278:E278"/>
+    <mergeCell ref="C211:E211"/>
+    <mergeCell ref="C272:E272"/>
+    <mergeCell ref="C236:E236"/>
+    <mergeCell ref="C277:E277"/>
+    <mergeCell ref="C274:E274"/>
+    <mergeCell ref="C273:E273"/>
+    <mergeCell ref="A253:B264"/>
+    <mergeCell ref="A228:B235"/>
+    <mergeCell ref="A237:B251"/>
+    <mergeCell ref="C117:E117"/>
+    <mergeCell ref="C122:E122"/>
+    <mergeCell ref="A199:B207"/>
+    <mergeCell ref="A209:B226"/>
+    <mergeCell ref="A297:B302"/>
+    <mergeCell ref="A304:B309"/>
+    <mergeCell ref="A266:B267"/>
+    <mergeCell ref="A269:B270"/>
+    <mergeCell ref="A272:B275"/>
+    <mergeCell ref="A277:B279"/>
+    <mergeCell ref="A281:B289"/>
+    <mergeCell ref="A294:B295"/>
+    <mergeCell ref="A118:B121"/>
+    <mergeCell ref="C153:E153"/>
+    <mergeCell ref="C154:E154"/>
+    <mergeCell ref="C151:E151"/>
+    <mergeCell ref="C143:E143"/>
+    <mergeCell ref="A123:B142"/>
+    <mergeCell ref="A144:B150"/>
+    <mergeCell ref="A152:B152"/>
     <mergeCell ref="A58:B70"/>
     <mergeCell ref="C110:E110"/>
     <mergeCell ref="A110:B116"/>
@@ -6328,72 +6397,6 @@
     <mergeCell ref="C101:E101"/>
     <mergeCell ref="C109:E109"/>
     <mergeCell ref="C71:E71"/>
-    <mergeCell ref="A118:B121"/>
-    <mergeCell ref="C153:E153"/>
-    <mergeCell ref="C154:E154"/>
-    <mergeCell ref="C151:E151"/>
-    <mergeCell ref="C143:E143"/>
-    <mergeCell ref="A123:B142"/>
-    <mergeCell ref="A144:B150"/>
-    <mergeCell ref="A152:B152"/>
-    <mergeCell ref="A199:B207"/>
-    <mergeCell ref="A209:B226"/>
-    <mergeCell ref="A297:B302"/>
-    <mergeCell ref="A304:B309"/>
-    <mergeCell ref="A266:B267"/>
-    <mergeCell ref="A269:B270"/>
-    <mergeCell ref="A272:B275"/>
-    <mergeCell ref="A277:B279"/>
-    <mergeCell ref="A281:B289"/>
-    <mergeCell ref="A294:B295"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="C252:E252"/>
-    <mergeCell ref="C269:E269"/>
-    <mergeCell ref="C290:E290"/>
-    <mergeCell ref="C278:E278"/>
-    <mergeCell ref="C211:E211"/>
-    <mergeCell ref="C272:E272"/>
-    <mergeCell ref="C236:E236"/>
-    <mergeCell ref="C277:E277"/>
-    <mergeCell ref="C274:E274"/>
-    <mergeCell ref="C273:E273"/>
-    <mergeCell ref="A253:B264"/>
-    <mergeCell ref="A228:B235"/>
-    <mergeCell ref="A237:B251"/>
-    <mergeCell ref="C117:E117"/>
-    <mergeCell ref="C122:E122"/>
-    <mergeCell ref="C198:E198"/>
-    <mergeCell ref="C280:E280"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="A6:B11"/>
-    <mergeCell ref="A35:B42"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="A13:B33"/>
-    <mergeCell ref="D6:D11"/>
-    <mergeCell ref="C6:C11"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="A72:B91"/>
-    <mergeCell ref="A93:B100"/>
-    <mergeCell ref="C303:E303"/>
-    <mergeCell ref="C155:E155"/>
-    <mergeCell ref="C210:E210"/>
-    <mergeCell ref="C209:E209"/>
-    <mergeCell ref="C208:E208"/>
-    <mergeCell ref="C265:E265"/>
-    <mergeCell ref="C268:E268"/>
-    <mergeCell ref="C266:E266"/>
-    <mergeCell ref="C276:E276"/>
-    <mergeCell ref="C293:E293"/>
-    <mergeCell ref="C271:E271"/>
-    <mergeCell ref="C227:E227"/>
-    <mergeCell ref="C156:E156"/>
-    <mergeCell ref="C296:E296"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Enhancements to facility understanding.
</commit_message>
<xml_diff>
--- a/Doc/testPlan.xlsx
+++ b/Doc/testPlan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="429">
   <si>
     <t>Group Assignment</t>
   </si>
@@ -1544,6 +1544,9 @@
   </si>
   <si>
     <t>Group admin Q operations</t>
+  </si>
+  <si>
+    <t>This class contains tests to target operations against ASQ/ACQ's. Operations can be defined to be legal or illegal against a Q.</t>
   </si>
 </sst>
 </file>
@@ -1973,58 +1976,151 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2034,21 +2130,6 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2056,84 +2137,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3082,7 +3085,7 @@
   <dimension ref="A1:E311"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="D121" sqref="D121"/>
+      <selection activeCell="C117" sqref="C117:E117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3096,32 +3099,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="17" customFormat="1" ht="15" customHeight="1">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="96" t="s">
         <v>329</v>
       </c>
-      <c r="B1" s="89" t="s">
+      <c r="B1" s="69" t="s">
         <v>359</v>
       </c>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
       <c r="E1" s="18"/>
     </row>
     <row r="2" spans="1:5" s="17" customFormat="1" ht="15" customHeight="1">
-      <c r="A2" s="88"/>
-      <c r="B2" s="106" t="s">
+      <c r="A2" s="96"/>
+      <c r="B2" s="93" t="s">
         <v>384</v>
       </c>
-      <c r="C2" s="106"/>
-      <c r="D2" s="106"/>
+      <c r="C2" s="93"/>
+      <c r="D2" s="93"/>
       <c r="E2" s="18"/>
     </row>
     <row r="3" spans="1:5" s="17" customFormat="1" ht="15" customHeight="1">
-      <c r="A3" s="88"/>
-      <c r="B3" s="107" t="s">
+      <c r="A3" s="96"/>
+      <c r="B3" s="94" t="s">
         <v>330</v>
       </c>
-      <c r="C3" s="108"/>
-      <c r="D3" s="108"/>
+      <c r="C3" s="95"/>
+      <c r="D3" s="95"/>
       <c r="E3" s="44"/>
     </row>
     <row r="4" spans="1:5">
@@ -3148,15 +3151,15 @@
       <c r="B5" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="C5" s="90"/>
-      <c r="D5" s="91"/>
-      <c r="E5" s="92"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="72"/>
     </row>
     <row r="6" spans="1:5" s="4" customFormat="1">
-      <c r="A6" s="69"/>
-      <c r="B6" s="70"/>
-      <c r="C6" s="104"/>
-      <c r="D6" s="102" t="s">
+      <c r="A6" s="79"/>
+      <c r="B6" s="80"/>
+      <c r="C6" s="91"/>
+      <c r="D6" s="89" t="s">
         <v>99</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -3164,46 +3167,46 @@
       </c>
     </row>
     <row r="7" spans="1:5" s="4" customFormat="1">
-      <c r="A7" s="71"/>
-      <c r="B7" s="72"/>
-      <c r="C7" s="105"/>
-      <c r="D7" s="103"/>
+      <c r="A7" s="81"/>
+      <c r="B7" s="82"/>
+      <c r="C7" s="92"/>
+      <c r="D7" s="90"/>
       <c r="E7" s="1" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="4" customFormat="1">
-      <c r="A8" s="71"/>
-      <c r="B8" s="72"/>
-      <c r="C8" s="105"/>
-      <c r="D8" s="103"/>
+      <c r="A8" s="81"/>
+      <c r="B8" s="82"/>
+      <c r="C8" s="92"/>
+      <c r="D8" s="90"/>
       <c r="E8" s="1" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="4" customFormat="1">
-      <c r="A9" s="71"/>
-      <c r="B9" s="72"/>
-      <c r="C9" s="105"/>
-      <c r="D9" s="103"/>
+      <c r="A9" s="81"/>
+      <c r="B9" s="82"/>
+      <c r="C9" s="92"/>
+      <c r="D9" s="90"/>
       <c r="E9" s="1" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="4" customFormat="1">
-      <c r="A10" s="71"/>
-      <c r="B10" s="72"/>
-      <c r="C10" s="105"/>
-      <c r="D10" s="103"/>
+      <c r="A10" s="81"/>
+      <c r="B10" s="82"/>
+      <c r="C10" s="92"/>
+      <c r="D10" s="90"/>
       <c r="E10" s="1" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="4" customFormat="1" ht="30" customHeight="1">
-      <c r="A11" s="71"/>
-      <c r="B11" s="72"/>
-      <c r="C11" s="105"/>
-      <c r="D11" s="103"/>
+      <c r="A11" s="81"/>
+      <c r="B11" s="82"/>
+      <c r="C11" s="92"/>
+      <c r="D11" s="90"/>
       <c r="E11" s="28" t="s">
         <v>241</v>
       </c>
@@ -3220,8 +3223,8 @@
       <c r="E12" s="31"/>
     </row>
     <row r="13" spans="1:5" s="4" customFormat="1" ht="30" customHeight="1">
-      <c r="A13" s="69"/>
-      <c r="B13" s="70"/>
+      <c r="A13" s="79"/>
+      <c r="B13" s="80"/>
       <c r="C13" s="20"/>
       <c r="D13" s="3" t="s">
         <v>362</v>
@@ -3231,8 +3234,8 @@
       </c>
     </row>
     <row r="14" spans="1:5" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A14" s="71"/>
-      <c r="B14" s="72"/>
+      <c r="A14" s="81"/>
+      <c r="B14" s="82"/>
       <c r="C14" s="29"/>
       <c r="D14" s="3" t="s">
         <v>364</v>
@@ -3242,8 +3245,8 @@
       </c>
     </row>
     <row r="15" spans="1:5" s="4" customFormat="1" ht="30" customHeight="1">
-      <c r="A15" s="71"/>
-      <c r="B15" s="72"/>
+      <c r="A15" s="81"/>
+      <c r="B15" s="82"/>
       <c r="C15" s="49"/>
       <c r="D15" s="3" t="s">
         <v>365</v>
@@ -3253,8 +3256,8 @@
       </c>
     </row>
     <row r="16" spans="1:5" s="4" customFormat="1" ht="30" customHeight="1">
-      <c r="A16" s="71"/>
-      <c r="B16" s="72"/>
+      <c r="A16" s="81"/>
+      <c r="B16" s="82"/>
       <c r="C16" s="20"/>
       <c r="D16" s="3" t="s">
         <v>366</v>
@@ -3264,8 +3267,8 @@
       </c>
     </row>
     <row r="17" spans="1:5" s="4" customFormat="1" ht="30" customHeight="1">
-      <c r="A17" s="71"/>
-      <c r="B17" s="72"/>
+      <c r="A17" s="81"/>
+      <c r="B17" s="82"/>
       <c r="C17" s="20"/>
       <c r="D17" s="3" t="s">
         <v>368</v>
@@ -3275,8 +3278,8 @@
       </c>
     </row>
     <row r="18" spans="1:5" s="4" customFormat="1" ht="30" customHeight="1">
-      <c r="A18" s="71"/>
-      <c r="B18" s="72"/>
+      <c r="A18" s="81"/>
+      <c r="B18" s="82"/>
       <c r="C18" s="20"/>
       <c r="D18" s="3" t="s">
         <v>369</v>
@@ -3286,8 +3289,8 @@
       </c>
     </row>
     <row r="19" spans="1:5" s="4" customFormat="1" ht="30" customHeight="1">
-      <c r="A19" s="71"/>
-      <c r="B19" s="72"/>
+      <c r="A19" s="81"/>
+      <c r="B19" s="82"/>
       <c r="C19" s="20"/>
       <c r="D19" s="3" t="s">
         <v>370</v>
@@ -3297,8 +3300,8 @@
       </c>
     </row>
     <row r="20" spans="1:5" s="4" customFormat="1" ht="45">
-      <c r="A20" s="71"/>
-      <c r="B20" s="72"/>
+      <c r="A20" s="81"/>
+      <c r="B20" s="82"/>
       <c r="C20" s="49"/>
       <c r="D20" s="3" t="s">
         <v>371</v>
@@ -3308,8 +3311,8 @@
       </c>
     </row>
     <row r="21" spans="1:5" s="4" customFormat="1" ht="30" customHeight="1">
-      <c r="A21" s="71"/>
-      <c r="B21" s="72"/>
+      <c r="A21" s="81"/>
+      <c r="B21" s="82"/>
       <c r="C21" s="20"/>
       <c r="D21" s="3" t="s">
         <v>376</v>
@@ -3319,8 +3322,8 @@
       </c>
     </row>
     <row r="22" spans="1:5" s="4" customFormat="1" ht="30" customHeight="1">
-      <c r="A22" s="71"/>
-      <c r="B22" s="72"/>
+      <c r="A22" s="81"/>
+      <c r="B22" s="82"/>
       <c r="C22" s="20"/>
       <c r="D22" s="3" t="s">
         <v>377</v>
@@ -3330,8 +3333,8 @@
       </c>
     </row>
     <row r="23" spans="1:5" s="4" customFormat="1" ht="30" customHeight="1">
-      <c r="A23" s="71"/>
-      <c r="B23" s="72"/>
+      <c r="A23" s="81"/>
+      <c r="B23" s="82"/>
       <c r="C23" s="20"/>
       <c r="D23" s="3" t="s">
         <v>372</v>
@@ -3341,8 +3344,8 @@
       </c>
     </row>
     <row r="24" spans="1:5" s="4" customFormat="1" ht="30" customHeight="1">
-      <c r="A24" s="71"/>
-      <c r="B24" s="72"/>
+      <c r="A24" s="81"/>
+      <c r="B24" s="82"/>
       <c r="C24" s="49"/>
       <c r="D24" s="3" t="s">
         <v>373</v>
@@ -3352,8 +3355,8 @@
       </c>
     </row>
     <row r="25" spans="1:5" s="4" customFormat="1" ht="30" customHeight="1">
-      <c r="A25" s="71"/>
-      <c r="B25" s="72"/>
+      <c r="A25" s="81"/>
+      <c r="B25" s="82"/>
       <c r="C25" s="20"/>
       <c r="D25" s="3" t="s">
         <v>374</v>
@@ -3363,8 +3366,8 @@
       </c>
     </row>
     <row r="26" spans="1:5" s="4" customFormat="1" ht="45">
-      <c r="A26" s="71"/>
-      <c r="B26" s="72"/>
+      <c r="A26" s="81"/>
+      <c r="B26" s="82"/>
       <c r="C26" s="49"/>
       <c r="D26" s="3" t="s">
         <v>375</v>
@@ -3374,8 +3377,8 @@
       </c>
     </row>
     <row r="27" spans="1:5" s="4" customFormat="1" ht="45">
-      <c r="A27" s="71"/>
-      <c r="B27" s="72"/>
+      <c r="A27" s="81"/>
+      <c r="B27" s="82"/>
       <c r="C27" s="49"/>
       <c r="D27" s="3" t="s">
         <v>367</v>
@@ -3385,8 +3388,8 @@
       </c>
     </row>
     <row r="28" spans="1:5" s="4" customFormat="1">
-      <c r="A28" s="71"/>
-      <c r="B28" s="72"/>
+      <c r="A28" s="81"/>
+      <c r="B28" s="82"/>
       <c r="C28" s="45"/>
       <c r="D28" s="3" t="s">
         <v>407</v>
@@ -3396,8 +3399,8 @@
       </c>
     </row>
     <row r="29" spans="1:5" s="4" customFormat="1">
-      <c r="A29" s="71"/>
-      <c r="B29" s="72"/>
+      <c r="A29" s="81"/>
+      <c r="B29" s="82"/>
       <c r="C29" s="45"/>
       <c r="D29" s="3" t="s">
         <v>409</v>
@@ -3407,8 +3410,8 @@
       </c>
     </row>
     <row r="30" spans="1:5" s="4" customFormat="1">
-      <c r="A30" s="71"/>
-      <c r="B30" s="72"/>
+      <c r="A30" s="81"/>
+      <c r="B30" s="82"/>
       <c r="C30" s="45"/>
       <c r="D30" s="3" t="s">
         <v>410</v>
@@ -3418,8 +3421,8 @@
       </c>
     </row>
     <row r="31" spans="1:5" s="4" customFormat="1">
-      <c r="A31" s="71"/>
-      <c r="B31" s="72"/>
+      <c r="A31" s="81"/>
+      <c r="B31" s="82"/>
       <c r="C31" s="45"/>
       <c r="D31" s="3" t="s">
         <v>411</v>
@@ -3429,8 +3432,8 @@
       </c>
     </row>
     <row r="32" spans="1:5" s="4" customFormat="1">
-      <c r="A32" s="71"/>
-      <c r="B32" s="72"/>
+      <c r="A32" s="81"/>
+      <c r="B32" s="82"/>
       <c r="C32" s="45"/>
       <c r="D32" s="3" t="s">
         <v>412</v>
@@ -3440,8 +3443,8 @@
       </c>
     </row>
     <row r="33" spans="1:5" s="4" customFormat="1">
-      <c r="A33" s="71"/>
-      <c r="B33" s="72"/>
+      <c r="A33" s="81"/>
+      <c r="B33" s="82"/>
       <c r="C33" s="45"/>
       <c r="D33" s="3" t="s">
         <v>413</v>
@@ -3457,15 +3460,15 @@
       <c r="B34" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="C34" s="93" t="s">
+      <c r="C34" s="73" t="s">
         <v>88</v>
       </c>
-      <c r="D34" s="94"/>
-      <c r="E34" s="95"/>
+      <c r="D34" s="74"/>
+      <c r="E34" s="75"/>
     </row>
     <row r="35" spans="1:5" s="4" customFormat="1" ht="75">
-      <c r="A35" s="96"/>
-      <c r="B35" s="97"/>
+      <c r="A35" s="83"/>
+      <c r="B35" s="84"/>
       <c r="C35" s="19"/>
       <c r="D35" s="3" t="s">
         <v>317</v>
@@ -3473,8 +3476,8 @@
       <c r="E35" s="10"/>
     </row>
     <row r="36" spans="1:5" s="4" customFormat="1" ht="75">
-      <c r="A36" s="98"/>
-      <c r="B36" s="99"/>
+      <c r="A36" s="85"/>
+      <c r="B36" s="86"/>
       <c r="C36" s="20"/>
       <c r="D36" s="3" t="s">
         <v>318</v>
@@ -3482,8 +3485,8 @@
       <c r="E36" s="10"/>
     </row>
     <row r="37" spans="1:5" s="4" customFormat="1" ht="75">
-      <c r="A37" s="98"/>
-      <c r="B37" s="99"/>
+      <c r="A37" s="85"/>
+      <c r="B37" s="86"/>
       <c r="C37" s="19"/>
       <c r="D37" s="3" t="s">
         <v>358</v>
@@ -3493,8 +3496,8 @@
       </c>
     </row>
     <row r="38" spans="1:5" s="4" customFormat="1" ht="45">
-      <c r="A38" s="98"/>
-      <c r="B38" s="99"/>
+      <c r="A38" s="85"/>
+      <c r="B38" s="86"/>
       <c r="C38" s="19"/>
       <c r="D38" s="3" t="s">
         <v>89</v>
@@ -3504,8 +3507,8 @@
       </c>
     </row>
     <row r="39" spans="1:5" s="4" customFormat="1" ht="45">
-      <c r="A39" s="98"/>
-      <c r="B39" s="99"/>
+      <c r="A39" s="85"/>
+      <c r="B39" s="86"/>
       <c r="C39" s="19"/>
       <c r="D39" s="3" t="s">
         <v>96</v>
@@ -3515,8 +3518,8 @@
       </c>
     </row>
     <row r="40" spans="1:5" s="4" customFormat="1" ht="75">
-      <c r="A40" s="98"/>
-      <c r="B40" s="99"/>
+      <c r="A40" s="85"/>
+      <c r="B40" s="86"/>
       <c r="C40" s="19"/>
       <c r="D40" s="3" t="s">
         <v>97</v>
@@ -3524,8 +3527,8 @@
       <c r="E40" s="10"/>
     </row>
     <row r="41" spans="1:5" s="4" customFormat="1" ht="45">
-      <c r="A41" s="98"/>
-      <c r="B41" s="99"/>
+      <c r="A41" s="85"/>
+      <c r="B41" s="86"/>
       <c r="C41" s="19"/>
       <c r="D41" s="3" t="s">
         <v>101</v>
@@ -3533,8 +3536,8 @@
       <c r="E41" s="10"/>
     </row>
     <row r="42" spans="1:5" s="4" customFormat="1" ht="45">
-      <c r="A42" s="98"/>
-      <c r="B42" s="99"/>
+      <c r="A42" s="85"/>
+      <c r="B42" s="86"/>
       <c r="C42" s="19"/>
       <c r="D42" s="3" t="s">
         <v>131</v>
@@ -3550,16 +3553,16 @@
       <c r="B43" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="C43" s="93" t="s">
+      <c r="C43" s="73" t="s">
         <v>100</v>
       </c>
-      <c r="D43" s="94"/>
-      <c r="E43" s="95"/>
+      <c r="D43" s="74"/>
+      <c r="E43" s="75"/>
     </row>
     <row r="44" spans="1:5" s="4" customFormat="1">
-      <c r="A44" s="96"/>
-      <c r="B44" s="97"/>
-      <c r="C44" s="100"/>
+      <c r="A44" s="83"/>
+      <c r="B44" s="84"/>
+      <c r="C44" s="87"/>
       <c r="D44" s="3" t="s">
         <v>91</v>
       </c>
@@ -3568,9 +3571,9 @@
       </c>
     </row>
     <row r="45" spans="1:5" s="4" customFormat="1">
-      <c r="A45" s="98"/>
-      <c r="B45" s="99"/>
-      <c r="C45" s="101"/>
+      <c r="A45" s="85"/>
+      <c r="B45" s="86"/>
+      <c r="C45" s="88"/>
       <c r="D45" s="3" t="s">
         <v>93</v>
       </c>
@@ -3585,42 +3588,42 @@
       <c r="B46" s="8">
         <v>2</v>
       </c>
-      <c r="C46" s="66" t="s">
+      <c r="C46" s="76" t="s">
         <v>232</v>
       </c>
-      <c r="D46" s="67"/>
-      <c r="E46" s="68"/>
+      <c r="D46" s="77"/>
+      <c r="E46" s="78"/>
     </row>
     <row r="47" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A47" s="69"/>
-      <c r="B47" s="70"/>
-      <c r="C47" s="73" t="s">
+      <c r="A47" s="79"/>
+      <c r="B47" s="80"/>
+      <c r="C47" s="104" t="s">
         <v>235</v>
       </c>
-      <c r="D47" s="74"/>
-      <c r="E47" s="75"/>
+      <c r="D47" s="105"/>
+      <c r="E47" s="106"/>
     </row>
     <row r="48" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A48" s="71"/>
-      <c r="B48" s="72"/>
-      <c r="C48" s="66" t="s">
+      <c r="A48" s="81"/>
+      <c r="B48" s="82"/>
+      <c r="C48" s="76" t="s">
         <v>233</v>
       </c>
-      <c r="D48" s="67"/>
-      <c r="E48" s="68"/>
+      <c r="D48" s="77"/>
+      <c r="E48" s="78"/>
     </row>
     <row r="49" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A49" s="71"/>
-      <c r="B49" s="72"/>
-      <c r="C49" s="66" t="s">
+      <c r="A49" s="81"/>
+      <c r="B49" s="82"/>
+      <c r="C49" s="76" t="s">
         <v>234</v>
       </c>
-      <c r="D49" s="67"/>
-      <c r="E49" s="68"/>
+      <c r="D49" s="77"/>
+      <c r="E49" s="78"/>
     </row>
     <row r="50" spans="1:5" s="4" customFormat="1" ht="15" customHeight="1">
-      <c r="A50" s="71"/>
-      <c r="B50" s="72"/>
+      <c r="A50" s="81"/>
+      <c r="B50" s="82"/>
       <c r="C50" s="27"/>
       <c r="D50" s="3" t="s">
         <v>78</v>
@@ -3630,8 +3633,8 @@
       </c>
     </row>
     <row r="51" spans="1:5" s="4" customFormat="1">
-      <c r="A51" s="71"/>
-      <c r="B51" s="72"/>
+      <c r="A51" s="81"/>
+      <c r="B51" s="82"/>
       <c r="C51" s="27"/>
       <c r="D51" s="3" t="s">
         <v>80</v>
@@ -3639,8 +3642,8 @@
       <c r="E51" s="10"/>
     </row>
     <row r="52" spans="1:5" s="4" customFormat="1">
-      <c r="A52" s="71"/>
-      <c r="B52" s="72"/>
+      <c r="A52" s="81"/>
+      <c r="B52" s="82"/>
       <c r="C52" s="27"/>
       <c r="D52" s="3" t="s">
         <v>81</v>
@@ -3650,8 +3653,8 @@
       </c>
     </row>
     <row r="53" spans="1:5" s="4" customFormat="1">
-      <c r="A53" s="71"/>
-      <c r="B53" s="72"/>
+      <c r="A53" s="81"/>
+      <c r="B53" s="82"/>
       <c r="C53" s="27"/>
       <c r="D53" s="3" t="s">
         <v>83</v>
@@ -3661,8 +3664,8 @@
       </c>
     </row>
     <row r="54" spans="1:5" s="4" customFormat="1">
-      <c r="A54" s="71"/>
-      <c r="B54" s="72"/>
+      <c r="A54" s="81"/>
+      <c r="B54" s="82"/>
       <c r="C54" s="27"/>
       <c r="D54" s="3" t="s">
         <v>84</v>
@@ -3672,8 +3675,8 @@
       </c>
     </row>
     <row r="55" spans="1:5" s="4" customFormat="1">
-      <c r="A55" s="71"/>
-      <c r="B55" s="72"/>
+      <c r="A55" s="81"/>
+      <c r="B55" s="82"/>
       <c r="C55" s="27"/>
       <c r="D55" s="3" t="s">
         <v>85</v>
@@ -3683,8 +3686,8 @@
       </c>
     </row>
     <row r="56" spans="1:5" s="4" customFormat="1">
-      <c r="A56" s="71"/>
-      <c r="B56" s="72"/>
+      <c r="A56" s="81"/>
+      <c r="B56" s="82"/>
       <c r="C56" s="48"/>
       <c r="D56" s="48" t="s">
         <v>414</v>
@@ -3700,42 +3703,42 @@
       <c r="B57" s="8">
         <v>3</v>
       </c>
-      <c r="C57" s="66" t="s">
+      <c r="C57" s="76" t="s">
         <v>232</v>
       </c>
-      <c r="D57" s="67"/>
-      <c r="E57" s="68"/>
+      <c r="D57" s="77"/>
+      <c r="E57" s="78"/>
     </row>
     <row r="58" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A58" s="55"/>
-      <c r="B58" s="56"/>
-      <c r="C58" s="76" t="s">
+      <c r="A58" s="100"/>
+      <c r="B58" s="59"/>
+      <c r="C58" s="66" t="s">
         <v>235</v>
       </c>
-      <c r="D58" s="77"/>
-      <c r="E58" s="78"/>
+      <c r="D58" s="67"/>
+      <c r="E58" s="68"/>
     </row>
     <row r="59" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A59" s="57"/>
-      <c r="B59" s="58"/>
-      <c r="C59" s="66" t="s">
+      <c r="A59" s="56"/>
+      <c r="B59" s="57"/>
+      <c r="C59" s="76" t="s">
         <v>233</v>
       </c>
-      <c r="D59" s="67"/>
-      <c r="E59" s="68"/>
+      <c r="D59" s="77"/>
+      <c r="E59" s="78"/>
     </row>
     <row r="60" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A60" s="57"/>
-      <c r="B60" s="58"/>
-      <c r="C60" s="66" t="s">
+      <c r="A60" s="56"/>
+      <c r="B60" s="57"/>
+      <c r="C60" s="76" t="s">
         <v>234</v>
       </c>
-      <c r="D60" s="67"/>
-      <c r="E60" s="68"/>
+      <c r="D60" s="77"/>
+      <c r="E60" s="78"/>
     </row>
     <row r="61" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A61" s="57"/>
-      <c r="B61" s="58"/>
+      <c r="A61" s="56"/>
+      <c r="B61" s="57"/>
       <c r="C61" s="20"/>
       <c r="D61" s="3" t="s">
         <v>13</v>
@@ -3743,8 +3746,8 @@
       <c r="E61" s="10"/>
     </row>
     <row r="62" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A62" s="57"/>
-      <c r="B62" s="58"/>
+      <c r="A62" s="56"/>
+      <c r="B62" s="57"/>
       <c r="C62" s="19"/>
       <c r="D62" s="3" t="s">
         <v>3</v>
@@ -3752,8 +3755,8 @@
       <c r="E62" s="10"/>
     </row>
     <row r="63" spans="1:5">
-      <c r="A63" s="57"/>
-      <c r="B63" s="58"/>
+      <c r="A63" s="56"/>
+      <c r="B63" s="57"/>
       <c r="C63" s="19"/>
       <c r="D63" s="3" t="s">
         <v>12</v>
@@ -3761,8 +3764,8 @@
       <c r="E63" s="10"/>
     </row>
     <row r="64" spans="1:5">
-      <c r="A64" s="57"/>
-      <c r="B64" s="58"/>
+      <c r="A64" s="56"/>
+      <c r="B64" s="57"/>
       <c r="C64" s="19"/>
       <c r="D64" s="3" t="s">
         <v>11</v>
@@ -3770,8 +3773,8 @@
       <c r="E64" s="10"/>
     </row>
     <row r="65" spans="1:5">
-      <c r="A65" s="57"/>
-      <c r="B65" s="58"/>
+      <c r="A65" s="56"/>
+      <c r="B65" s="57"/>
       <c r="C65" s="19"/>
       <c r="D65" s="3" t="s">
         <v>10</v>
@@ -3779,8 +3782,8 @@
       <c r="E65" s="10"/>
     </row>
     <row r="66" spans="1:5">
-      <c r="A66" s="57"/>
-      <c r="B66" s="58"/>
+      <c r="A66" s="56"/>
+      <c r="B66" s="57"/>
       <c r="C66" s="19"/>
       <c r="D66" s="3" t="s">
         <v>9</v>
@@ -3788,8 +3791,8 @@
       <c r="E66" s="10"/>
     </row>
     <row r="67" spans="1:5">
-      <c r="A67" s="57"/>
-      <c r="B67" s="58"/>
+      <c r="A67" s="56"/>
+      <c r="B67" s="57"/>
       <c r="C67" s="19"/>
       <c r="D67" s="3" t="s">
         <v>8</v>
@@ -3797,8 +3800,8 @@
       <c r="E67" s="10"/>
     </row>
     <row r="68" spans="1:5">
-      <c r="A68" s="57"/>
-      <c r="B68" s="58"/>
+      <c r="A68" s="56"/>
+      <c r="B68" s="57"/>
       <c r="C68" s="19"/>
       <c r="D68" s="3" t="s">
         <v>7</v>
@@ -3806,8 +3809,8 @@
       <c r="E68" s="10"/>
     </row>
     <row r="69" spans="1:5">
-      <c r="A69" s="57"/>
-      <c r="B69" s="58"/>
+      <c r="A69" s="56"/>
+      <c r="B69" s="57"/>
       <c r="C69" s="19"/>
       <c r="D69" s="3" t="s">
         <v>6</v>
@@ -3817,8 +3820,8 @@
       </c>
     </row>
     <row r="70" spans="1:5">
-      <c r="A70" s="59"/>
-      <c r="B70" s="60"/>
+      <c r="A70" s="101"/>
+      <c r="B70" s="62"/>
       <c r="C70" s="19"/>
       <c r="D70" s="3" t="s">
         <v>5</v>
@@ -3834,15 +3837,15 @@
       <c r="B71" s="16">
         <v>7</v>
       </c>
-      <c r="C71" s="81" t="s">
+      <c r="C71" s="107" t="s">
         <v>400</v>
       </c>
-      <c r="D71" s="82"/>
-      <c r="E71" s="83"/>
+      <c r="D71" s="108"/>
+      <c r="E71" s="109"/>
     </row>
     <row r="72" spans="1:5">
-      <c r="A72" s="57"/>
-      <c r="B72" s="58"/>
+      <c r="A72" s="56"/>
+      <c r="B72" s="57"/>
       <c r="C72" s="49"/>
       <c r="D72" s="16" t="s">
         <v>385</v>
@@ -3852,8 +3855,8 @@
       </c>
     </row>
     <row r="73" spans="1:5">
-      <c r="A73" s="57"/>
-      <c r="B73" s="58"/>
+      <c r="A73" s="56"/>
+      <c r="B73" s="57"/>
       <c r="C73" s="50"/>
       <c r="D73" s="16" t="s">
         <v>387</v>
@@ -3863,8 +3866,8 @@
       </c>
     </row>
     <row r="74" spans="1:5">
-      <c r="A74" s="57"/>
-      <c r="B74" s="58"/>
+      <c r="A74" s="56"/>
+      <c r="B74" s="57"/>
       <c r="C74" s="50"/>
       <c r="D74" s="16" t="s">
         <v>389</v>
@@ -3874,8 +3877,8 @@
       </c>
     </row>
     <row r="75" spans="1:5">
-      <c r="A75" s="57"/>
-      <c r="B75" s="58"/>
+      <c r="A75" s="56"/>
+      <c r="B75" s="57"/>
       <c r="C75" s="52"/>
       <c r="D75" s="16" t="s">
         <v>416</v>
@@ -3885,8 +3888,8 @@
       </c>
     </row>
     <row r="76" spans="1:5">
-      <c r="A76" s="57"/>
-      <c r="B76" s="58"/>
+      <c r="A76" s="56"/>
+      <c r="B76" s="57"/>
       <c r="C76" s="51"/>
       <c r="D76" s="53" t="s">
         <v>395</v>
@@ -3896,8 +3899,8 @@
       </c>
     </row>
     <row r="77" spans="1:5">
-      <c r="A77" s="57"/>
-      <c r="B77" s="58"/>
+      <c r="A77" s="56"/>
+      <c r="B77" s="57"/>
       <c r="C77" s="51"/>
       <c r="D77" s="53" t="s">
         <v>391</v>
@@ -3907,8 +3910,8 @@
       </c>
     </row>
     <row r="78" spans="1:5">
-      <c r="A78" s="57"/>
-      <c r="B78" s="58"/>
+      <c r="A78" s="56"/>
+      <c r="B78" s="57"/>
       <c r="C78" s="54"/>
       <c r="D78" s="53" t="s">
         <v>418</v>
@@ -3918,8 +3921,8 @@
       </c>
     </row>
     <row r="79" spans="1:5">
-      <c r="A79" s="57"/>
-      <c r="B79" s="58"/>
+      <c r="A79" s="56"/>
+      <c r="B79" s="57"/>
       <c r="C79" s="54"/>
       <c r="D79" s="53" t="s">
         <v>424</v>
@@ -3929,8 +3932,8 @@
       </c>
     </row>
     <row r="80" spans="1:5">
-      <c r="A80" s="57"/>
-      <c r="B80" s="58"/>
+      <c r="A80" s="56"/>
+      <c r="B80" s="57"/>
       <c r="C80" s="51"/>
       <c r="D80" s="16" t="s">
         <v>396</v>
@@ -3940,8 +3943,8 @@
       </c>
     </row>
     <row r="81" spans="1:5">
-      <c r="A81" s="57"/>
-      <c r="B81" s="58"/>
+      <c r="A81" s="56"/>
+      <c r="B81" s="57"/>
       <c r="C81" s="51"/>
       <c r="D81" s="16" t="s">
         <v>392</v>
@@ -3951,8 +3954,8 @@
       </c>
     </row>
     <row r="82" spans="1:5">
-      <c r="A82" s="57"/>
-      <c r="B82" s="58"/>
+      <c r="A82" s="56"/>
+      <c r="B82" s="57"/>
       <c r="C82" s="54"/>
       <c r="D82" s="16" t="s">
         <v>425</v>
@@ -3962,8 +3965,8 @@
       </c>
     </row>
     <row r="83" spans="1:5">
-      <c r="A83" s="57"/>
-      <c r="B83" s="58"/>
+      <c r="A83" s="56"/>
+      <c r="B83" s="57"/>
       <c r="C83" s="54"/>
       <c r="D83" s="16" t="s">
         <v>426</v>
@@ -3973,8 +3976,8 @@
       </c>
     </row>
     <row r="84" spans="1:5">
-      <c r="A84" s="57"/>
-      <c r="B84" s="58"/>
+      <c r="A84" s="56"/>
+      <c r="B84" s="57"/>
       <c r="C84" s="45"/>
       <c r="D84" s="53" t="s">
         <v>397</v>
@@ -3984,8 +3987,8 @@
       </c>
     </row>
     <row r="85" spans="1:5">
-      <c r="A85" s="57"/>
-      <c r="B85" s="58"/>
+      <c r="A85" s="56"/>
+      <c r="B85" s="57"/>
       <c r="C85" s="45"/>
       <c r="D85" s="53" t="s">
         <v>391</v>
@@ -3995,8 +3998,8 @@
       </c>
     </row>
     <row r="86" spans="1:5">
-      <c r="A86" s="57"/>
-      <c r="B86" s="58"/>
+      <c r="A86" s="56"/>
+      <c r="B86" s="57"/>
       <c r="C86" s="45"/>
       <c r="D86" s="53" t="s">
         <v>418</v>
@@ -4006,8 +4009,8 @@
       </c>
     </row>
     <row r="87" spans="1:5">
-      <c r="A87" s="57"/>
-      <c r="B87" s="58"/>
+      <c r="A87" s="56"/>
+      <c r="B87" s="57"/>
       <c r="C87" s="45"/>
       <c r="D87" s="53" t="s">
         <v>424</v>
@@ -4017,8 +4020,8 @@
       </c>
     </row>
     <row r="88" spans="1:5">
-      <c r="A88" s="57"/>
-      <c r="B88" s="58"/>
+      <c r="A88" s="56"/>
+      <c r="B88" s="57"/>
       <c r="C88" s="45"/>
       <c r="D88" s="16" t="s">
         <v>398</v>
@@ -4028,8 +4031,8 @@
       </c>
     </row>
     <row r="89" spans="1:5">
-      <c r="A89" s="57"/>
-      <c r="B89" s="58"/>
+      <c r="A89" s="56"/>
+      <c r="B89" s="57"/>
       <c r="C89" s="45"/>
       <c r="D89" s="16" t="s">
         <v>392</v>
@@ -4039,8 +4042,8 @@
       </c>
     </row>
     <row r="90" spans="1:5">
-      <c r="A90" s="57"/>
-      <c r="B90" s="58"/>
+      <c r="A90" s="56"/>
+      <c r="B90" s="57"/>
       <c r="C90" s="45"/>
       <c r="D90" s="16" t="s">
         <v>425</v>
@@ -4050,8 +4053,8 @@
       </c>
     </row>
     <row r="91" spans="1:5">
-      <c r="A91" s="57"/>
-      <c r="B91" s="58"/>
+      <c r="A91" s="56"/>
+      <c r="B91" s="57"/>
       <c r="C91" s="45"/>
       <c r="D91" s="16" t="s">
         <v>426</v>
@@ -4067,15 +4070,15 @@
       <c r="B92" s="8">
         <v>7</v>
       </c>
-      <c r="C92" s="76" t="s">
+      <c r="C92" s="66" t="s">
         <v>331</v>
       </c>
-      <c r="D92" s="77"/>
-      <c r="E92" s="78"/>
+      <c r="D92" s="67"/>
+      <c r="E92" s="68"/>
     </row>
     <row r="93" spans="1:5">
-      <c r="A93" s="62"/>
-      <c r="B93" s="56"/>
+      <c r="A93" s="58"/>
+      <c r="B93" s="59"/>
       <c r="C93" s="16"/>
       <c r="D93" s="3" t="s">
         <v>243</v>
@@ -4085,8 +4088,8 @@
       </c>
     </row>
     <row r="94" spans="1:5">
-      <c r="A94" s="65"/>
-      <c r="B94" s="58"/>
+      <c r="A94" s="60"/>
+      <c r="B94" s="57"/>
       <c r="C94" s="16"/>
       <c r="D94" s="3" t="s">
         <v>244</v>
@@ -4096,8 +4099,8 @@
       </c>
     </row>
     <row r="95" spans="1:5">
-      <c r="A95" s="65"/>
-      <c r="B95" s="58"/>
+      <c r="A95" s="60"/>
+      <c r="B95" s="57"/>
       <c r="C95" s="16"/>
       <c r="D95" s="3" t="s">
         <v>250</v>
@@ -4107,8 +4110,8 @@
       </c>
     </row>
     <row r="96" spans="1:5">
-      <c r="A96" s="65"/>
-      <c r="B96" s="58"/>
+      <c r="A96" s="60"/>
+      <c r="B96" s="57"/>
       <c r="C96" s="16"/>
       <c r="D96" s="3" t="s">
         <v>245</v>
@@ -4118,8 +4121,8 @@
       </c>
     </row>
     <row r="97" spans="1:5">
-      <c r="A97" s="65"/>
-      <c r="B97" s="58"/>
+      <c r="A97" s="60"/>
+      <c r="B97" s="57"/>
       <c r="C97" s="16"/>
       <c r="D97" s="3" t="s">
         <v>246</v>
@@ -4129,8 +4132,8 @@
       </c>
     </row>
     <row r="98" spans="1:5" ht="53.25" customHeight="1">
-      <c r="A98" s="65"/>
-      <c r="B98" s="58"/>
+      <c r="A98" s="60"/>
+      <c r="B98" s="57"/>
       <c r="C98" s="16"/>
       <c r="D98" s="3" t="s">
         <v>247</v>
@@ -4140,8 +4143,8 @@
       </c>
     </row>
     <row r="99" spans="1:5">
-      <c r="A99" s="65"/>
-      <c r="B99" s="58"/>
+      <c r="A99" s="60"/>
+      <c r="B99" s="57"/>
       <c r="C99" s="16"/>
       <c r="D99" s="3" t="s">
         <v>248</v>
@@ -4151,8 +4154,8 @@
       </c>
     </row>
     <row r="100" spans="1:5" ht="30">
-      <c r="A100" s="64"/>
-      <c r="B100" s="60"/>
+      <c r="A100" s="61"/>
+      <c r="B100" s="62"/>
       <c r="C100" s="16"/>
       <c r="D100" s="3" t="s">
         <v>249</v>
@@ -4168,13 +4171,13 @@
       <c r="B101" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="C101" s="79"/>
-      <c r="D101" s="80"/>
-      <c r="E101" s="80"/>
+      <c r="C101" s="63"/>
+      <c r="D101" s="64"/>
+      <c r="E101" s="64"/>
     </row>
     <row r="102" spans="1:5">
-      <c r="A102" s="62"/>
-      <c r="B102" s="56"/>
+      <c r="A102" s="58"/>
+      <c r="B102" s="59"/>
       <c r="C102" s="16"/>
       <c r="D102" s="3" t="s">
         <v>143</v>
@@ -4184,8 +4187,8 @@
       </c>
     </row>
     <row r="103" spans="1:5">
-      <c r="A103" s="65"/>
-      <c r="B103" s="58"/>
+      <c r="A103" s="60"/>
+      <c r="B103" s="57"/>
       <c r="C103" s="16"/>
       <c r="D103" s="3" t="s">
         <v>147</v>
@@ -4195,8 +4198,8 @@
       </c>
     </row>
     <row r="104" spans="1:5">
-      <c r="A104" s="65"/>
-      <c r="B104" s="58"/>
+      <c r="A104" s="60"/>
+      <c r="B104" s="57"/>
       <c r="C104" s="16"/>
       <c r="D104" s="3" t="s">
         <v>146</v>
@@ -4206,8 +4209,8 @@
       </c>
     </row>
     <row r="105" spans="1:5" ht="30">
-      <c r="A105" s="65"/>
-      <c r="B105" s="58"/>
+      <c r="A105" s="60"/>
+      <c r="B105" s="57"/>
       <c r="C105" s="16"/>
       <c r="D105" s="3" t="s">
         <v>148</v>
@@ -4217,8 +4220,8 @@
       </c>
     </row>
     <row r="106" spans="1:5" ht="30">
-      <c r="A106" s="65"/>
-      <c r="B106" s="58"/>
+      <c r="A106" s="60"/>
+      <c r="B106" s="57"/>
       <c r="C106" s="16"/>
       <c r="D106" s="3" t="s">
         <v>150</v>
@@ -4228,8 +4231,8 @@
       </c>
     </row>
     <row r="107" spans="1:5">
-      <c r="A107" s="65"/>
-      <c r="B107" s="58"/>
+      <c r="A107" s="60"/>
+      <c r="B107" s="57"/>
       <c r="C107" s="16"/>
       <c r="D107" s="3" t="s">
         <v>152</v>
@@ -4239,8 +4242,8 @@
       </c>
     </row>
     <row r="108" spans="1:5" ht="30">
-      <c r="A108" s="64"/>
-      <c r="B108" s="60"/>
+      <c r="A108" s="61"/>
+      <c r="B108" s="62"/>
       <c r="C108" s="16"/>
       <c r="D108" s="3" t="s">
         <v>154</v>
@@ -4256,24 +4259,24 @@
       <c r="B109" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="C109" s="61" t="s">
+      <c r="C109" s="102" t="s">
         <v>361</v>
       </c>
-      <c r="D109" s="61"/>
-      <c r="E109" s="61"/>
+      <c r="D109" s="102"/>
+      <c r="E109" s="102"/>
     </row>
     <row r="110" spans="1:5" ht="15" customHeight="1">
-      <c r="A110" s="62"/>
-      <c r="B110" s="56"/>
-      <c r="C110" s="61" t="s">
+      <c r="A110" s="58"/>
+      <c r="B110" s="59"/>
+      <c r="C110" s="102" t="s">
         <v>360</v>
       </c>
-      <c r="D110" s="61"/>
-      <c r="E110" s="61"/>
+      <c r="D110" s="102"/>
+      <c r="E110" s="102"/>
     </row>
     <row r="111" spans="1:5">
-      <c r="A111" s="63"/>
-      <c r="B111" s="58"/>
+      <c r="A111" s="103"/>
+      <c r="B111" s="57"/>
       <c r="C111" s="47"/>
       <c r="D111" s="47" t="s">
         <v>107</v>
@@ -4283,8 +4286,8 @@
       </c>
     </row>
     <row r="112" spans="1:5" ht="45">
-      <c r="A112" s="63"/>
-      <c r="B112" s="58"/>
+      <c r="A112" s="103"/>
+      <c r="B112" s="57"/>
       <c r="C112" s="45"/>
       <c r="D112" s="42" t="s">
         <v>393</v>
@@ -4292,8 +4295,8 @@
       <c r="E112" s="43"/>
     </row>
     <row r="113" spans="1:5" ht="45">
-      <c r="A113" s="63"/>
-      <c r="B113" s="58"/>
+      <c r="A113" s="103"/>
+      <c r="B113" s="57"/>
       <c r="C113" s="45"/>
       <c r="D113" s="42" t="s">
         <v>108</v>
@@ -4301,8 +4304,8 @@
       <c r="E113" s="43"/>
     </row>
     <row r="114" spans="1:5" ht="45">
-      <c r="A114" s="63"/>
-      <c r="B114" s="58"/>
+      <c r="A114" s="103"/>
+      <c r="B114" s="57"/>
       <c r="C114" s="45"/>
       <c r="D114" s="42" t="s">
         <v>124</v>
@@ -4312,8 +4315,8 @@
       </c>
     </row>
     <row r="115" spans="1:5" ht="75">
-      <c r="A115" s="63"/>
-      <c r="B115" s="58"/>
+      <c r="A115" s="103"/>
+      <c r="B115" s="57"/>
       <c r="C115" s="45"/>
       <c r="D115" s="42" t="s">
         <v>123</v>
@@ -4323,8 +4326,8 @@
       </c>
     </row>
     <row r="116" spans="1:5" ht="45">
-      <c r="A116" s="64"/>
-      <c r="B116" s="60"/>
+      <c r="A116" s="61"/>
+      <c r="B116" s="62"/>
       <c r="C116"/>
       <c r="D116" s="42" t="s">
         <v>106</v>
@@ -4338,13 +4341,15 @@
       <c r="B117" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C117" s="85"/>
-      <c r="D117" s="86"/>
-      <c r="E117" s="87"/>
+      <c r="C117" s="63" t="s">
+        <v>428</v>
+      </c>
+      <c r="D117" s="64"/>
+      <c r="E117" s="65"/>
     </row>
     <row r="118" spans="1:5">
-      <c r="A118" s="62"/>
-      <c r="B118" s="56"/>
+      <c r="A118" s="58"/>
+      <c r="B118" s="59"/>
       <c r="C118" s="16"/>
       <c r="D118" s="3" t="s">
         <v>103</v>
@@ -4354,8 +4359,8 @@
       </c>
     </row>
     <row r="119" spans="1:5">
-      <c r="A119" s="65"/>
-      <c r="B119" s="58"/>
+      <c r="A119" s="60"/>
+      <c r="B119" s="57"/>
       <c r="C119" s="16"/>
       <c r="D119" s="3" t="s">
         <v>114</v>
@@ -4365,8 +4370,8 @@
       </c>
     </row>
     <row r="120" spans="1:5">
-      <c r="A120" s="65"/>
-      <c r="B120" s="58"/>
+      <c r="A120" s="60"/>
+      <c r="B120" s="57"/>
       <c r="C120" s="16"/>
       <c r="D120" s="3" t="s">
         <v>357</v>
@@ -4376,10 +4381,10 @@
       </c>
     </row>
     <row r="121" spans="1:5" ht="45">
-      <c r="A121" s="64"/>
-      <c r="B121" s="60"/>
+      <c r="A121" s="61"/>
+      <c r="B121" s="62"/>
       <c r="C121" s="16"/>
-      <c r="D121" s="109" t="s">
+      <c r="D121" s="55" t="s">
         <v>127</v>
       </c>
       <c r="E121" s="10" t="s">
@@ -4393,15 +4398,15 @@
       <c r="B122" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C122" s="76" t="s">
+      <c r="C122" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="D122" s="77"/>
-      <c r="E122" s="78"/>
+      <c r="D122" s="67"/>
+      <c r="E122" s="68"/>
     </row>
     <row r="123" spans="1:5" ht="45">
-      <c r="A123" s="62"/>
-      <c r="B123" s="56"/>
+      <c r="A123" s="58"/>
+      <c r="B123" s="59"/>
       <c r="C123" s="16"/>
       <c r="D123" s="3" t="s">
         <v>109</v>
@@ -4411,8 +4416,8 @@
       </c>
     </row>
     <row r="124" spans="1:5" ht="45">
-      <c r="A124" s="65"/>
-      <c r="B124" s="58"/>
+      <c r="A124" s="60"/>
+      <c r="B124" s="57"/>
       <c r="C124" s="16"/>
       <c r="D124" s="3" t="s">
         <v>111</v>
@@ -4422,8 +4427,8 @@
       </c>
     </row>
     <row r="125" spans="1:5">
-      <c r="A125" s="65"/>
-      <c r="B125" s="58"/>
+      <c r="A125" s="60"/>
+      <c r="B125" s="57"/>
       <c r="C125" s="16"/>
       <c r="D125" s="3" t="s">
         <v>104</v>
@@ -4433,8 +4438,8 @@
       </c>
     </row>
     <row r="126" spans="1:5">
-      <c r="A126" s="65"/>
-      <c r="B126" s="58"/>
+      <c r="A126" s="60"/>
+      <c r="B126" s="57"/>
       <c r="C126" s="16"/>
       <c r="D126" s="3" t="s">
         <v>271</v>
@@ -4442,8 +4447,8 @@
       <c r="E126" s="10"/>
     </row>
     <row r="127" spans="1:5">
-      <c r="A127" s="65"/>
-      <c r="B127" s="58"/>
+      <c r="A127" s="60"/>
+      <c r="B127" s="57"/>
       <c r="C127" s="16"/>
       <c r="D127" s="3" t="s">
         <v>272</v>
@@ -4451,8 +4456,8 @@
       <c r="E127" s="10"/>
     </row>
     <row r="128" spans="1:5" ht="45">
-      <c r="A128" s="65"/>
-      <c r="B128" s="58"/>
+      <c r="A128" s="60"/>
+      <c r="B128" s="57"/>
       <c r="C128" s="16"/>
       <c r="D128" s="3" t="s">
         <v>133</v>
@@ -4462,8 +4467,8 @@
       </c>
     </row>
     <row r="129" spans="1:5" ht="45">
-      <c r="A129" s="65"/>
-      <c r="B129" s="58"/>
+      <c r="A129" s="60"/>
+      <c r="B129" s="57"/>
       <c r="C129" s="16"/>
       <c r="D129" s="3" t="s">
         <v>137</v>
@@ -4473,8 +4478,8 @@
       </c>
     </row>
     <row r="130" spans="1:5">
-      <c r="A130" s="65"/>
-      <c r="B130" s="58"/>
+      <c r="A130" s="60"/>
+      <c r="B130" s="57"/>
       <c r="C130" s="16"/>
       <c r="D130" s="33" t="s">
         <v>58</v>
@@ -4484,8 +4489,8 @@
       </c>
     </row>
     <row r="131" spans="1:5" ht="45">
-      <c r="A131" s="65"/>
-      <c r="B131" s="58"/>
+      <c r="A131" s="60"/>
+      <c r="B131" s="57"/>
       <c r="C131" s="16"/>
       <c r="D131" s="3" t="s">
         <v>105</v>
@@ -4495,8 +4500,8 @@
       </c>
     </row>
     <row r="132" spans="1:5">
-      <c r="A132" s="65"/>
-      <c r="B132" s="58"/>
+      <c r="A132" s="60"/>
+      <c r="B132" s="57"/>
       <c r="C132" s="16"/>
       <c r="D132" s="3" t="s">
         <v>285</v>
@@ -4506,8 +4511,8 @@
       </c>
     </row>
     <row r="133" spans="1:5">
-      <c r="A133" s="65"/>
-      <c r="B133" s="58"/>
+      <c r="A133" s="60"/>
+      <c r="B133" s="57"/>
       <c r="C133" s="16"/>
       <c r="D133" s="3" t="s">
         <v>284</v>
@@ -4517,8 +4522,8 @@
       </c>
     </row>
     <row r="134" spans="1:5">
-      <c r="A134" s="65"/>
-      <c r="B134" s="58"/>
+      <c r="A134" s="60"/>
+      <c r="B134" s="57"/>
       <c r="C134" s="16"/>
       <c r="D134" s="3" t="s">
         <v>282</v>
@@ -4528,8 +4533,8 @@
       </c>
     </row>
     <row r="135" spans="1:5">
-      <c r="A135" s="65"/>
-      <c r="B135" s="58"/>
+      <c r="A135" s="60"/>
+      <c r="B135" s="57"/>
       <c r="C135" s="16"/>
       <c r="D135" s="3" t="s">
         <v>139</v>
@@ -4539,8 +4544,8 @@
       </c>
     </row>
     <row r="136" spans="1:5">
-      <c r="A136" s="65"/>
-      <c r="B136" s="58"/>
+      <c r="A136" s="60"/>
+      <c r="B136" s="57"/>
       <c r="C136" s="16"/>
       <c r="D136" s="3" t="s">
         <v>277</v>
@@ -4550,8 +4555,8 @@
       </c>
     </row>
     <row r="137" spans="1:5" ht="30">
-      <c r="A137" s="65"/>
-      <c r="B137" s="58"/>
+      <c r="A137" s="60"/>
+      <c r="B137" s="57"/>
       <c r="C137" s="16"/>
       <c r="D137" s="3" t="s">
         <v>278</v>
@@ -4561,8 +4566,8 @@
       </c>
     </row>
     <row r="138" spans="1:5" ht="30">
-      <c r="A138" s="65"/>
-      <c r="B138" s="58"/>
+      <c r="A138" s="60"/>
+      <c r="B138" s="57"/>
       <c r="C138" s="16"/>
       <c r="D138" s="3" t="s">
         <v>275</v>
@@ -4572,8 +4577,8 @@
       </c>
     </row>
     <row r="139" spans="1:5" ht="30">
-      <c r="A139" s="65"/>
-      <c r="B139" s="58"/>
+      <c r="A139" s="60"/>
+      <c r="B139" s="57"/>
       <c r="C139" s="16"/>
       <c r="D139" s="3" t="s">
         <v>274</v>
@@ -4583,8 +4588,8 @@
       </c>
     </row>
     <row r="140" spans="1:5" ht="30">
-      <c r="A140" s="65"/>
-      <c r="B140" s="58"/>
+      <c r="A140" s="60"/>
+      <c r="B140" s="57"/>
       <c r="C140" s="16"/>
       <c r="D140" s="3" t="s">
         <v>276</v>
@@ -4594,8 +4599,8 @@
       </c>
     </row>
     <row r="141" spans="1:5" ht="15" customHeight="1">
-      <c r="A141" s="65"/>
-      <c r="B141" s="58"/>
+      <c r="A141" s="60"/>
+      <c r="B141" s="57"/>
       <c r="C141" s="16"/>
       <c r="D141" s="3" t="s">
         <v>253</v>
@@ -4605,8 +4610,8 @@
       </c>
     </row>
     <row r="142" spans="1:5" ht="15" customHeight="1">
-      <c r="A142" s="64"/>
-      <c r="B142" s="60"/>
+      <c r="A142" s="61"/>
+      <c r="B142" s="62"/>
       <c r="C142" s="16"/>
       <c r="D142" s="3" t="s">
         <v>114</v>
@@ -4622,13 +4627,13 @@
       <c r="B143" s="9">
         <v>5</v>
       </c>
-      <c r="C143" s="85"/>
-      <c r="D143" s="86"/>
-      <c r="E143" s="87"/>
+      <c r="C143" s="97"/>
+      <c r="D143" s="98"/>
+      <c r="E143" s="99"/>
     </row>
     <row r="144" spans="1:5" ht="15" customHeight="1">
-      <c r="A144" s="62"/>
-      <c r="B144" s="56"/>
+      <c r="A144" s="58"/>
+      <c r="B144" s="59"/>
       <c r="C144" s="16"/>
       <c r="D144" s="3" t="s">
         <v>184</v>
@@ -4638,8 +4643,8 @@
       </c>
     </row>
     <row r="145" spans="1:5">
-      <c r="A145" s="65"/>
-      <c r="B145" s="58"/>
+      <c r="A145" s="60"/>
+      <c r="B145" s="57"/>
       <c r="C145" s="16"/>
       <c r="D145" s="3" t="s">
         <v>185</v>
@@ -4649,8 +4654,8 @@
       </c>
     </row>
     <row r="146" spans="1:5">
-      <c r="A146" s="65"/>
-      <c r="B146" s="58"/>
+      <c r="A146" s="60"/>
+      <c r="B146" s="57"/>
       <c r="C146" s="16"/>
       <c r="D146" s="3" t="s">
         <v>193</v>
@@ -4660,8 +4665,8 @@
       </c>
     </row>
     <row r="147" spans="1:5">
-      <c r="A147" s="65"/>
-      <c r="B147" s="58"/>
+      <c r="A147" s="60"/>
+      <c r="B147" s="57"/>
       <c r="C147" s="16"/>
       <c r="D147" s="3" t="s">
         <v>194</v>
@@ -4671,8 +4676,8 @@
       </c>
     </row>
     <row r="148" spans="1:5">
-      <c r="A148" s="65"/>
-      <c r="B148" s="58"/>
+      <c r="A148" s="60"/>
+      <c r="B148" s="57"/>
       <c r="C148" s="16"/>
       <c r="D148" s="3" t="s">
         <v>188</v>
@@ -4682,8 +4687,8 @@
       </c>
     </row>
     <row r="149" spans="1:5">
-      <c r="A149" s="65"/>
-      <c r="B149" s="58"/>
+      <c r="A149" s="60"/>
+      <c r="B149" s="57"/>
       <c r="C149" s="16"/>
       <c r="D149" s="3" t="s">
         <v>190</v>
@@ -4693,8 +4698,8 @@
       </c>
     </row>
     <row r="150" spans="1:5">
-      <c r="A150" s="64"/>
-      <c r="B150" s="60"/>
+      <c r="A150" s="61"/>
+      <c r="B150" s="62"/>
       <c r="C150" s="16"/>
       <c r="D150" s="3" t="s">
         <v>191</v>
@@ -4710,13 +4715,13 @@
       <c r="B151" s="8">
         <v>5</v>
       </c>
-      <c r="C151" s="79"/>
-      <c r="D151" s="80"/>
-      <c r="E151" s="84"/>
+      <c r="C151" s="63"/>
+      <c r="D151" s="64"/>
+      <c r="E151" s="65"/>
     </row>
     <row r="152" spans="1:5">
-      <c r="A152" s="85"/>
-      <c r="B152" s="87"/>
+      <c r="A152" s="97"/>
+      <c r="B152" s="99"/>
       <c r="C152" s="41"/>
       <c r="D152" s="33" t="s">
         <v>198</v>
@@ -4732,36 +4737,36 @@
       <c r="B153" s="8">
         <v>4</v>
       </c>
-      <c r="C153" s="79" t="s">
+      <c r="C153" s="63" t="s">
         <v>321</v>
       </c>
-      <c r="D153" s="80"/>
-      <c r="E153" s="84"/>
+      <c r="D153" s="64"/>
+      <c r="E153" s="65"/>
     </row>
     <row r="154" spans="1:5">
       <c r="A154" s="25"/>
       <c r="B154" s="26"/>
-      <c r="C154" s="79" t="s">
+      <c r="C154" s="63" t="s">
         <v>322</v>
       </c>
-      <c r="D154" s="80"/>
-      <c r="E154" s="84"/>
+      <c r="D154" s="64"/>
+      <c r="E154" s="65"/>
     </row>
     <row r="155" spans="1:5">
-      <c r="C155" s="79" t="s">
+      <c r="C155" s="63" t="s">
         <v>323</v>
       </c>
-      <c r="D155" s="80"/>
-      <c r="E155" s="84"/>
+      <c r="D155" s="64"/>
+      <c r="E155" s="65"/>
     </row>
     <row r="156" spans="1:5">
       <c r="A156" s="37"/>
       <c r="B156" s="38"/>
-      <c r="C156" s="79" t="s">
+      <c r="C156" s="63" t="s">
         <v>332</v>
       </c>
-      <c r="D156" s="80"/>
-      <c r="E156" s="84"/>
+      <c r="D156" s="64"/>
+      <c r="E156" s="65"/>
     </row>
     <row r="157" spans="1:5">
       <c r="A157" s="39"/>
@@ -5145,13 +5150,13 @@
       <c r="B198" s="8">
         <v>4</v>
       </c>
-      <c r="C198" s="79"/>
-      <c r="D198" s="80"/>
-      <c r="E198" s="84"/>
+      <c r="C198" s="63"/>
+      <c r="D198" s="64"/>
+      <c r="E198" s="65"/>
     </row>
     <row r="199" spans="1:5" ht="15" customHeight="1">
-      <c r="A199" s="62"/>
-      <c r="B199" s="56"/>
+      <c r="A199" s="58"/>
+      <c r="B199" s="59"/>
       <c r="C199" s="16"/>
       <c r="D199" s="3" t="s">
         <v>40</v>
@@ -5161,8 +5166,8 @@
       </c>
     </row>
     <row r="200" spans="1:5">
-      <c r="A200" s="65"/>
-      <c r="B200" s="58"/>
+      <c r="A200" s="60"/>
+      <c r="B200" s="57"/>
       <c r="C200" s="16"/>
       <c r="D200" s="3" t="s">
         <v>41</v>
@@ -5172,8 +5177,8 @@
       </c>
     </row>
     <row r="201" spans="1:5" ht="45">
-      <c r="A201" s="65"/>
-      <c r="B201" s="58"/>
+      <c r="A201" s="60"/>
+      <c r="B201" s="57"/>
       <c r="C201" s="16"/>
       <c r="D201" s="3" t="s">
         <v>170</v>
@@ -5183,8 +5188,8 @@
       </c>
     </row>
     <row r="202" spans="1:5">
-      <c r="A202" s="65"/>
-      <c r="B202" s="58"/>
+      <c r="A202" s="60"/>
+      <c r="B202" s="57"/>
       <c r="C202" s="16"/>
       <c r="D202" s="3" t="s">
         <v>171</v>
@@ -5194,8 +5199,8 @@
       </c>
     </row>
     <row r="203" spans="1:5" ht="30">
-      <c r="A203" s="65"/>
-      <c r="B203" s="58"/>
+      <c r="A203" s="60"/>
+      <c r="B203" s="57"/>
       <c r="C203" s="16"/>
       <c r="D203" s="3" t="s">
         <v>173</v>
@@ -5205,8 +5210,8 @@
       </c>
     </row>
     <row r="204" spans="1:5" ht="30">
-      <c r="A204" s="65"/>
-      <c r="B204" s="58"/>
+      <c r="A204" s="60"/>
+      <c r="B204" s="57"/>
       <c r="C204" s="16"/>
       <c r="D204" s="3" t="s">
         <v>175</v>
@@ -5216,8 +5221,8 @@
       </c>
     </row>
     <row r="205" spans="1:5" ht="30">
-      <c r="A205" s="65"/>
-      <c r="B205" s="58"/>
+      <c r="A205" s="60"/>
+      <c r="B205" s="57"/>
       <c r="C205" s="16"/>
       <c r="D205" s="3" t="s">
         <v>178</v>
@@ -5227,8 +5232,8 @@
       </c>
     </row>
     <row r="206" spans="1:5" ht="30">
-      <c r="A206" s="65"/>
-      <c r="B206" s="58"/>
+      <c r="A206" s="60"/>
+      <c r="B206" s="57"/>
       <c r="C206" s="16"/>
       <c r="D206" s="3" t="s">
         <v>179</v>
@@ -5238,8 +5243,8 @@
       </c>
     </row>
     <row r="207" spans="1:5" ht="45">
-      <c r="A207" s="64"/>
-      <c r="B207" s="60"/>
+      <c r="A207" s="61"/>
+      <c r="B207" s="62"/>
       <c r="C207" s="16"/>
       <c r="D207" s="3" t="s">
         <v>304</v>
@@ -5255,42 +5260,42 @@
       <c r="B208" s="8">
         <v>6</v>
       </c>
-      <c r="C208" s="79" t="s">
+      <c r="C208" s="63" t="s">
         <v>321</v>
       </c>
-      <c r="D208" s="80"/>
-      <c r="E208" s="84"/>
+      <c r="D208" s="64"/>
+      <c r="E208" s="65"/>
     </row>
     <row r="209" spans="1:5">
-      <c r="A209" s="62"/>
-      <c r="B209" s="56"/>
-      <c r="C209" s="79" t="s">
+      <c r="A209" s="58"/>
+      <c r="B209" s="59"/>
+      <c r="C209" s="63" t="s">
         <v>322</v>
       </c>
-      <c r="D209" s="80"/>
-      <c r="E209" s="84"/>
+      <c r="D209" s="64"/>
+      <c r="E209" s="65"/>
     </row>
     <row r="210" spans="1:5">
-      <c r="A210" s="65"/>
-      <c r="B210" s="58"/>
-      <c r="C210" s="79" t="s">
+      <c r="A210" s="60"/>
+      <c r="B210" s="57"/>
+      <c r="C210" s="63" t="s">
         <v>323</v>
       </c>
-      <c r="D210" s="80"/>
-      <c r="E210" s="84"/>
+      <c r="D210" s="64"/>
+      <c r="E210" s="65"/>
     </row>
     <row r="211" spans="1:5">
-      <c r="A211" s="65"/>
-      <c r="B211" s="58"/>
-      <c r="C211" s="79" t="s">
+      <c r="A211" s="60"/>
+      <c r="B211" s="57"/>
+      <c r="C211" s="63" t="s">
         <v>324</v>
       </c>
-      <c r="D211" s="80"/>
-      <c r="E211" s="84"/>
+      <c r="D211" s="64"/>
+      <c r="E211" s="65"/>
     </row>
     <row r="212" spans="1:5">
-      <c r="A212" s="65"/>
-      <c r="B212" s="58"/>
+      <c r="A212" s="60"/>
+      <c r="B212" s="57"/>
       <c r="C212" s="16"/>
       <c r="D212" s="3" t="s">
         <v>42</v>
@@ -5298,8 +5303,8 @@
       <c r="E212" s="10"/>
     </row>
     <row r="213" spans="1:5">
-      <c r="A213" s="65"/>
-      <c r="B213" s="58"/>
+      <c r="A213" s="60"/>
+      <c r="B213" s="57"/>
       <c r="C213" s="16"/>
       <c r="D213" s="3" t="s">
         <v>217</v>
@@ -5307,8 +5312,8 @@
       <c r="E213" s="10"/>
     </row>
     <row r="214" spans="1:5">
-      <c r="A214" s="65"/>
-      <c r="B214" s="58"/>
+      <c r="A214" s="60"/>
+      <c r="B214" s="57"/>
       <c r="C214" s="16"/>
       <c r="D214" s="3" t="s">
         <v>43</v>
@@ -5316,8 +5321,8 @@
       <c r="E214" s="10"/>
     </row>
     <row r="215" spans="1:5">
-      <c r="A215" s="65"/>
-      <c r="B215" s="58"/>
+      <c r="A215" s="60"/>
+      <c r="B215" s="57"/>
       <c r="C215" s="16"/>
       <c r="D215" s="3" t="s">
         <v>218</v>
@@ -5325,8 +5330,8 @@
       <c r="E215" s="10"/>
     </row>
     <row r="216" spans="1:5">
-      <c r="A216" s="65"/>
-      <c r="B216" s="58"/>
+      <c r="A216" s="60"/>
+      <c r="B216" s="57"/>
       <c r="C216" s="16"/>
       <c r="D216" s="3" t="s">
         <v>229</v>
@@ -5334,8 +5339,8 @@
       <c r="E216" s="10"/>
     </row>
     <row r="217" spans="1:5">
-      <c r="A217" s="65"/>
-      <c r="B217" s="58"/>
+      <c r="A217" s="60"/>
+      <c r="B217" s="57"/>
       <c r="C217" s="16"/>
       <c r="D217" s="3" t="s">
         <v>328</v>
@@ -5343,8 +5348,8 @@
       <c r="E217" s="10"/>
     </row>
     <row r="218" spans="1:5">
-      <c r="A218" s="65"/>
-      <c r="B218" s="58"/>
+      <c r="A218" s="60"/>
+      <c r="B218" s="57"/>
       <c r="C218" s="16"/>
       <c r="D218" s="3" t="s">
         <v>50</v>
@@ -5352,8 +5357,8 @@
       <c r="E218" s="10"/>
     </row>
     <row r="219" spans="1:5">
-      <c r="A219" s="65"/>
-      <c r="B219" s="58"/>
+      <c r="A219" s="60"/>
+      <c r="B219" s="57"/>
       <c r="C219" s="16"/>
       <c r="D219" s="3" t="s">
         <v>219</v>
@@ -5361,8 +5366,8 @@
       <c r="E219" s="10"/>
     </row>
     <row r="220" spans="1:5">
-      <c r="A220" s="65"/>
-      <c r="B220" s="58"/>
+      <c r="A220" s="60"/>
+      <c r="B220" s="57"/>
       <c r="C220" s="16"/>
       <c r="D220" s="3" t="s">
         <v>44</v>
@@ -5370,8 +5375,8 @@
       <c r="E220" s="10"/>
     </row>
     <row r="221" spans="1:5">
-      <c r="A221" s="65"/>
-      <c r="B221" s="58"/>
+      <c r="A221" s="60"/>
+      <c r="B221" s="57"/>
       <c r="C221" s="16"/>
       <c r="D221" s="3" t="s">
         <v>220</v>
@@ -5379,8 +5384,8 @@
       <c r="E221" s="10"/>
     </row>
     <row r="222" spans="1:5">
-      <c r="A222" s="65"/>
-      <c r="B222" s="58"/>
+      <c r="A222" s="60"/>
+      <c r="B222" s="57"/>
       <c r="C222" s="16"/>
       <c r="D222" s="3" t="s">
         <v>230</v>
@@ -5388,8 +5393,8 @@
       <c r="E222" s="10"/>
     </row>
     <row r="223" spans="1:5">
-      <c r="A223" s="65"/>
-      <c r="B223" s="58"/>
+      <c r="A223" s="60"/>
+      <c r="B223" s="57"/>
       <c r="C223" s="16"/>
       <c r="D223" s="3" t="s">
         <v>45</v>
@@ -5397,8 +5402,8 @@
       <c r="E223" s="10"/>
     </row>
     <row r="224" spans="1:5">
-      <c r="A224" s="65"/>
-      <c r="B224" s="58"/>
+      <c r="A224" s="60"/>
+      <c r="B224" s="57"/>
       <c r="C224" s="16"/>
       <c r="D224" s="3" t="s">
         <v>221</v>
@@ -5406,8 +5411,8 @@
       <c r="E224" s="10"/>
     </row>
     <row r="225" spans="1:5">
-      <c r="A225" s="65"/>
-      <c r="B225" s="58"/>
+      <c r="A225" s="60"/>
+      <c r="B225" s="57"/>
       <c r="C225" s="16"/>
       <c r="D225" s="3" t="s">
         <v>46</v>
@@ -5415,8 +5420,8 @@
       <c r="E225" s="10"/>
     </row>
     <row r="226" spans="1:5">
-      <c r="A226" s="64"/>
-      <c r="B226" s="60"/>
+      <c r="A226" s="61"/>
+      <c r="B226" s="62"/>
       <c r="C226" s="16"/>
       <c r="D226" s="3" t="s">
         <v>222</v>
@@ -5430,13 +5435,13 @@
       <c r="B227" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C227" s="79"/>
-      <c r="D227" s="80"/>
-      <c r="E227" s="84"/>
+      <c r="C227" s="63"/>
+      <c r="D227" s="64"/>
+      <c r="E227" s="65"/>
     </row>
     <row r="228" spans="1:5" ht="32.25">
-      <c r="A228" s="62"/>
-      <c r="B228" s="56"/>
+      <c r="A228" s="58"/>
+      <c r="B228" s="59"/>
       <c r="C228" s="16"/>
       <c r="D228" s="3" t="s">
         <v>168</v>
@@ -5446,8 +5451,8 @@
       </c>
     </row>
     <row r="229" spans="1:5" ht="34.5">
-      <c r="A229" s="65"/>
-      <c r="B229" s="58"/>
+      <c r="A229" s="60"/>
+      <c r="B229" s="57"/>
       <c r="C229" s="16"/>
       <c r="D229" s="3" t="s">
         <v>166</v>
@@ -5457,8 +5462,8 @@
       </c>
     </row>
     <row r="230" spans="1:5" ht="32.25">
-      <c r="A230" s="65"/>
-      <c r="B230" s="58"/>
+      <c r="A230" s="60"/>
+      <c r="B230" s="57"/>
       <c r="C230" s="16"/>
       <c r="D230" s="3" t="s">
         <v>164</v>
@@ -5468,8 +5473,8 @@
       </c>
     </row>
     <row r="231" spans="1:5">
-      <c r="A231" s="65"/>
-      <c r="B231" s="58"/>
+      <c r="A231" s="60"/>
+      <c r="B231" s="57"/>
       <c r="C231" s="16"/>
       <c r="D231" s="3" t="s">
         <v>162</v>
@@ -5479,8 +5484,8 @@
       </c>
     </row>
     <row r="232" spans="1:5">
-      <c r="A232" s="65"/>
-      <c r="B232" s="58"/>
+      <c r="A232" s="60"/>
+      <c r="B232" s="57"/>
       <c r="C232" s="16"/>
       <c r="D232" s="3" t="s">
         <v>161</v>
@@ -5490,8 +5495,8 @@
       </c>
     </row>
     <row r="233" spans="1:5">
-      <c r="A233" s="65"/>
-      <c r="B233" s="58"/>
+      <c r="A233" s="60"/>
+      <c r="B233" s="57"/>
       <c r="C233" s="16"/>
       <c r="D233" s="3" t="s">
         <v>159</v>
@@ -5501,8 +5506,8 @@
       </c>
     </row>
     <row r="234" spans="1:5">
-      <c r="A234" s="65"/>
-      <c r="B234" s="58"/>
+      <c r="A234" s="60"/>
+      <c r="B234" s="57"/>
       <c r="C234" s="16"/>
       <c r="D234" s="3" t="s">
         <v>158</v>
@@ -5512,8 +5517,8 @@
       </c>
     </row>
     <row r="235" spans="1:5" ht="17.25">
-      <c r="A235" s="64"/>
-      <c r="B235" s="60"/>
+      <c r="A235" s="61"/>
+      <c r="B235" s="62"/>
       <c r="C235" s="16"/>
       <c r="D235" s="3" t="s">
         <v>156</v>
@@ -5529,13 +5534,13 @@
       <c r="B236" s="8">
         <v>5</v>
       </c>
-      <c r="C236" s="79"/>
-      <c r="D236" s="80"/>
-      <c r="E236" s="84"/>
+      <c r="C236" s="63"/>
+      <c r="D236" s="64"/>
+      <c r="E236" s="65"/>
     </row>
     <row r="237" spans="1:5">
-      <c r="A237" s="62"/>
-      <c r="B237" s="56"/>
+      <c r="A237" s="58"/>
+      <c r="B237" s="59"/>
       <c r="C237" s="16"/>
       <c r="D237" s="34" t="s">
         <v>57</v>
@@ -5545,8 +5550,8 @@
       </c>
     </row>
     <row r="238" spans="1:5">
-      <c r="A238" s="65"/>
-      <c r="B238" s="58"/>
+      <c r="A238" s="60"/>
+      <c r="B238" s="57"/>
       <c r="C238" s="16"/>
       <c r="D238" s="3" t="s">
         <v>341</v>
@@ -5556,8 +5561,8 @@
       </c>
     </row>
     <row r="239" spans="1:5">
-      <c r="A239" s="65"/>
-      <c r="B239" s="58"/>
+      <c r="A239" s="60"/>
+      <c r="B239" s="57"/>
       <c r="C239" s="5"/>
       <c r="D239" s="3" t="s">
         <v>269</v>
@@ -5567,8 +5572,8 @@
       </c>
     </row>
     <row r="240" spans="1:5">
-      <c r="A240" s="65"/>
-      <c r="B240" s="58"/>
+      <c r="A240" s="60"/>
+      <c r="B240" s="57"/>
       <c r="C240" s="5"/>
       <c r="D240" s="3" t="s">
         <v>267</v>
@@ -5578,8 +5583,8 @@
       </c>
     </row>
     <row r="241" spans="1:5">
-      <c r="A241" s="65"/>
-      <c r="B241" s="58"/>
+      <c r="A241" s="60"/>
+      <c r="B241" s="57"/>
       <c r="C241" s="5"/>
       <c r="D241" s="3" t="s">
         <v>264</v>
@@ -5589,8 +5594,8 @@
       </c>
     </row>
     <row r="242" spans="1:5">
-      <c r="A242" s="65"/>
-      <c r="B242" s="58"/>
+      <c r="A242" s="60"/>
+      <c r="B242" s="57"/>
       <c r="C242" s="5"/>
       <c r="D242" s="3" t="s">
         <v>265</v>
@@ -5600,8 +5605,8 @@
       </c>
     </row>
     <row r="243" spans="1:5">
-      <c r="A243" s="65"/>
-      <c r="B243" s="58"/>
+      <c r="A243" s="60"/>
+      <c r="B243" s="57"/>
       <c r="C243" s="5"/>
       <c r="D243" s="3" t="s">
         <v>261</v>
@@ -5611,8 +5616,8 @@
       </c>
     </row>
     <row r="244" spans="1:5">
-      <c r="A244" s="65"/>
-      <c r="B244" s="58"/>
+      <c r="A244" s="60"/>
+      <c r="B244" s="57"/>
       <c r="C244" s="5"/>
       <c r="D244" s="3" t="s">
         <v>260</v>
@@ -5622,8 +5627,8 @@
       </c>
     </row>
     <row r="245" spans="1:5" ht="30">
-      <c r="A245" s="65"/>
-      <c r="B245" s="58"/>
+      <c r="A245" s="60"/>
+      <c r="B245" s="57"/>
       <c r="C245" s="5"/>
       <c r="D245" s="3" t="s">
         <v>116</v>
@@ -5633,8 +5638,8 @@
       </c>
     </row>
     <row r="246" spans="1:5">
-      <c r="A246" s="65"/>
-      <c r="B246" s="58"/>
+      <c r="A246" s="60"/>
+      <c r="B246" s="57"/>
       <c r="C246" s="5"/>
       <c r="D246" s="3" t="s">
         <v>256</v>
@@ -5644,8 +5649,8 @@
       </c>
     </row>
     <row r="247" spans="1:5">
-      <c r="A247" s="65"/>
-      <c r="B247" s="58"/>
+      <c r="A247" s="60"/>
+      <c r="B247" s="57"/>
       <c r="C247" s="5"/>
       <c r="D247" s="3" t="s">
         <v>257</v>
@@ -5655,8 +5660,8 @@
       </c>
     </row>
     <row r="248" spans="1:5" ht="30">
-      <c r="A248" s="65"/>
-      <c r="B248" s="58"/>
+      <c r="A248" s="60"/>
+      <c r="B248" s="57"/>
       <c r="C248" s="5"/>
       <c r="D248" s="3" t="s">
         <v>254</v>
@@ -5666,8 +5671,8 @@
       </c>
     </row>
     <row r="249" spans="1:5">
-      <c r="A249" s="65"/>
-      <c r="B249" s="58"/>
+      <c r="A249" s="60"/>
+      <c r="B249" s="57"/>
       <c r="C249" s="5"/>
       <c r="D249" s="3" t="s">
         <v>181</v>
@@ -5677,8 +5682,8 @@
       </c>
     </row>
     <row r="250" spans="1:5" ht="30">
-      <c r="A250" s="65"/>
-      <c r="B250" s="58"/>
+      <c r="A250" s="60"/>
+      <c r="B250" s="57"/>
       <c r="C250" s="5"/>
       <c r="D250" s="3" t="s">
         <v>118</v>
@@ -5688,8 +5693,8 @@
       </c>
     </row>
     <row r="251" spans="1:5" ht="30">
-      <c r="A251" s="64"/>
-      <c r="B251" s="60"/>
+      <c r="A251" s="61"/>
+      <c r="B251" s="62"/>
       <c r="C251" s="16"/>
       <c r="D251" s="3" t="s">
         <v>119</v>
@@ -5705,13 +5710,13 @@
       <c r="B252" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="C252" s="79"/>
-      <c r="D252" s="80"/>
-      <c r="E252" s="84"/>
+      <c r="C252" s="63"/>
+      <c r="D252" s="64"/>
+      <c r="E252" s="65"/>
     </row>
     <row r="253" spans="1:5" ht="15" customHeight="1">
-      <c r="A253" s="62"/>
-      <c r="B253" s="56"/>
+      <c r="A253" s="58"/>
+      <c r="B253" s="59"/>
       <c r="C253" s="16"/>
       <c r="D253" s="3" t="s">
         <v>195</v>
@@ -5721,8 +5726,8 @@
       </c>
     </row>
     <row r="254" spans="1:5" ht="15" customHeight="1">
-      <c r="A254" s="65"/>
-      <c r="B254" s="58"/>
+      <c r="A254" s="60"/>
+      <c r="B254" s="57"/>
       <c r="C254" s="16"/>
       <c r="D254" s="3" t="s">
         <v>292</v>
@@ -5732,8 +5737,8 @@
       </c>
     </row>
     <row r="255" spans="1:5" ht="30">
-      <c r="A255" s="65"/>
-      <c r="B255" s="58"/>
+      <c r="A255" s="60"/>
+      <c r="B255" s="57"/>
       <c r="C255" s="16"/>
       <c r="D255" s="3" t="s">
         <v>287</v>
@@ -5743,8 +5748,8 @@
       </c>
     </row>
     <row r="256" spans="1:5" ht="15" customHeight="1">
-      <c r="A256" s="65"/>
-      <c r="B256" s="58"/>
+      <c r="A256" s="60"/>
+      <c r="B256" s="57"/>
       <c r="C256" s="16"/>
       <c r="D256" s="3" t="s">
         <v>288</v>
@@ -5754,8 +5759,8 @@
       </c>
     </row>
     <row r="257" spans="1:5" ht="15" customHeight="1">
-      <c r="A257" s="65"/>
-      <c r="B257" s="58"/>
+      <c r="A257" s="60"/>
+      <c r="B257" s="57"/>
       <c r="C257" s="16"/>
       <c r="D257" s="3" t="s">
         <v>289</v>
@@ -5765,8 +5770,8 @@
       </c>
     </row>
     <row r="258" spans="1:5" ht="30">
-      <c r="A258" s="65"/>
-      <c r="B258" s="58"/>
+      <c r="A258" s="60"/>
+      <c r="B258" s="57"/>
       <c r="C258" s="16"/>
       <c r="D258" s="3" t="s">
         <v>295</v>
@@ -5776,8 +5781,8 @@
       </c>
     </row>
     <row r="259" spans="1:5" ht="15" customHeight="1">
-      <c r="A259" s="65"/>
-      <c r="B259" s="58"/>
+      <c r="A259" s="60"/>
+      <c r="B259" s="57"/>
       <c r="C259" s="16"/>
       <c r="D259" s="3" t="s">
         <v>294</v>
@@ -5787,8 +5792,8 @@
       </c>
     </row>
     <row r="260" spans="1:5" ht="15" customHeight="1">
-      <c r="A260" s="65"/>
-      <c r="B260" s="58"/>
+      <c r="A260" s="60"/>
+      <c r="B260" s="57"/>
       <c r="C260" s="16"/>
       <c r="D260" s="3" t="s">
         <v>293</v>
@@ -5796,8 +5801,8 @@
       <c r="E260" s="10"/>
     </row>
     <row r="261" spans="1:5" ht="15" customHeight="1">
-      <c r="A261" s="65"/>
-      <c r="B261" s="58"/>
+      <c r="A261" s="60"/>
+      <c r="B261" s="57"/>
       <c r="C261" s="16"/>
       <c r="D261" s="33" t="s">
         <v>298</v>
@@ -5807,8 +5812,8 @@
       </c>
     </row>
     <row r="262" spans="1:5" ht="15" customHeight="1">
-      <c r="A262" s="65"/>
-      <c r="B262" s="58"/>
+      <c r="A262" s="60"/>
+      <c r="B262" s="57"/>
       <c r="C262" s="16"/>
       <c r="D262" s="3" t="s">
         <v>300</v>
@@ -5818,8 +5823,8 @@
       </c>
     </row>
     <row r="263" spans="1:5">
-      <c r="A263" s="65"/>
-      <c r="B263" s="58"/>
+      <c r="A263" s="60"/>
+      <c r="B263" s="57"/>
       <c r="C263" s="16"/>
       <c r="D263" s="3" t="s">
         <v>301</v>
@@ -5829,8 +5834,8 @@
       </c>
     </row>
     <row r="264" spans="1:5" ht="15" customHeight="1">
-      <c r="A264" s="64"/>
-      <c r="B264" s="60"/>
+      <c r="A264" s="61"/>
+      <c r="B264" s="62"/>
       <c r="C264" s="16"/>
       <c r="D264" s="3" t="s">
         <v>76</v>
@@ -5844,24 +5849,24 @@
       <c r="B265" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="C265" s="79" t="s">
+      <c r="C265" s="63" t="s">
         <v>64</v>
       </c>
-      <c r="D265" s="80"/>
-      <c r="E265" s="84"/>
+      <c r="D265" s="64"/>
+      <c r="E265" s="65"/>
     </row>
     <row r="266" spans="1:5" ht="15" customHeight="1">
-      <c r="A266" s="62"/>
-      <c r="B266" s="56"/>
-      <c r="C266" s="79" t="s">
+      <c r="A266" s="58"/>
+      <c r="B266" s="59"/>
+      <c r="C266" s="63" t="s">
         <v>65</v>
       </c>
-      <c r="D266" s="80"/>
-      <c r="E266" s="84"/>
+      <c r="D266" s="64"/>
+      <c r="E266" s="65"/>
     </row>
     <row r="267" spans="1:5">
-      <c r="A267" s="64"/>
-      <c r="B267" s="60"/>
+      <c r="A267" s="61"/>
+      <c r="B267" s="62"/>
       <c r="C267" s="16"/>
       <c r="D267" s="34" t="s">
         <v>306</v>
@@ -5875,24 +5880,24 @@
       <c r="B268" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C268" s="79" t="s">
+      <c r="C268" s="63" t="s">
         <v>337</v>
       </c>
-      <c r="D268" s="80"/>
-      <c r="E268" s="84"/>
+      <c r="D268" s="64"/>
+      <c r="E268" s="65"/>
     </row>
     <row r="269" spans="1:5">
-      <c r="A269" s="62"/>
-      <c r="B269" s="56"/>
-      <c r="C269" s="79" t="s">
+      <c r="A269" s="58"/>
+      <c r="B269" s="59"/>
+      <c r="C269" s="63" t="s">
         <v>62</v>
       </c>
-      <c r="D269" s="80"/>
-      <c r="E269" s="84"/>
+      <c r="D269" s="64"/>
+      <c r="E269" s="65"/>
     </row>
     <row r="270" spans="1:5">
-      <c r="A270" s="64"/>
-      <c r="B270" s="60"/>
+      <c r="A270" s="61"/>
+      <c r="B270" s="62"/>
       <c r="C270" s="16"/>
       <c r="D270" s="34" t="s">
         <v>306</v>
@@ -5906,42 +5911,42 @@
       <c r="B271" s="8">
         <v>7</v>
       </c>
-      <c r="C271" s="79" t="s">
+      <c r="C271" s="63" t="s">
         <v>310</v>
       </c>
-      <c r="D271" s="80"/>
-      <c r="E271" s="84"/>
+      <c r="D271" s="64"/>
+      <c r="E271" s="65"/>
     </row>
     <row r="272" spans="1:5">
-      <c r="A272" s="62"/>
-      <c r="B272" s="56"/>
-      <c r="C272" s="76" t="s">
+      <c r="A272" s="58"/>
+      <c r="B272" s="59"/>
+      <c r="C272" s="66" t="s">
         <v>66</v>
       </c>
-      <c r="D272" s="77"/>
-      <c r="E272" s="77"/>
+      <c r="D272" s="67"/>
+      <c r="E272" s="67"/>
     </row>
     <row r="273" spans="1:5">
-      <c r="A273" s="65"/>
-      <c r="B273" s="58"/>
-      <c r="C273" s="76" t="s">
+      <c r="A273" s="60"/>
+      <c r="B273" s="57"/>
+      <c r="C273" s="66" t="s">
         <v>311</v>
       </c>
-      <c r="D273" s="77"/>
-      <c r="E273" s="78"/>
+      <c r="D273" s="67"/>
+      <c r="E273" s="68"/>
     </row>
     <row r="274" spans="1:5">
-      <c r="A274" s="65"/>
-      <c r="B274" s="58"/>
-      <c r="C274" s="76" t="s">
+      <c r="A274" s="60"/>
+      <c r="B274" s="57"/>
+      <c r="C274" s="66" t="s">
         <v>67</v>
       </c>
-      <c r="D274" s="77"/>
-      <c r="E274" s="78"/>
+      <c r="D274" s="67"/>
+      <c r="E274" s="68"/>
     </row>
     <row r="275" spans="1:5">
-      <c r="A275" s="64"/>
-      <c r="B275" s="60"/>
+      <c r="A275" s="61"/>
+      <c r="B275" s="62"/>
       <c r="C275" s="16"/>
       <c r="D275" s="34" t="s">
         <v>306</v>
@@ -5955,33 +5960,33 @@
       <c r="B276" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="C276" s="79" t="s">
+      <c r="C276" s="63" t="s">
         <v>307</v>
       </c>
-      <c r="D276" s="80"/>
-      <c r="E276" s="84"/>
+      <c r="D276" s="64"/>
+      <c r="E276" s="65"/>
     </row>
     <row r="277" spans="1:5">
-      <c r="A277" s="62"/>
-      <c r="B277" s="56"/>
-      <c r="C277" s="79" t="s">
+      <c r="A277" s="58"/>
+      <c r="B277" s="59"/>
+      <c r="C277" s="63" t="s">
         <v>309</v>
       </c>
-      <c r="D277" s="80"/>
-      <c r="E277" s="84"/>
+      <c r="D277" s="64"/>
+      <c r="E277" s="65"/>
     </row>
     <row r="278" spans="1:5">
-      <c r="A278" s="65"/>
-      <c r="B278" s="58"/>
-      <c r="C278" s="79" t="s">
+      <c r="A278" s="60"/>
+      <c r="B278" s="57"/>
+      <c r="C278" s="63" t="s">
         <v>308</v>
       </c>
-      <c r="D278" s="80"/>
-      <c r="E278" s="84"/>
+      <c r="D278" s="64"/>
+      <c r="E278" s="65"/>
     </row>
     <row r="279" spans="1:5">
-      <c r="A279" s="64"/>
-      <c r="B279" s="60"/>
+      <c r="A279" s="61"/>
+      <c r="B279" s="62"/>
       <c r="C279" s="16"/>
       <c r="D279" s="34" t="s">
         <v>306</v>
@@ -5995,15 +6000,15 @@
       <c r="B280" s="8">
         <v>5</v>
       </c>
-      <c r="C280" s="76" t="s">
+      <c r="C280" s="66" t="s">
         <v>345</v>
       </c>
-      <c r="D280" s="77"/>
-      <c r="E280" s="78"/>
+      <c r="D280" s="67"/>
+      <c r="E280" s="68"/>
     </row>
     <row r="281" spans="1:5" ht="15" customHeight="1">
-      <c r="A281" s="62"/>
-      <c r="B281" s="56"/>
+      <c r="A281" s="58"/>
+      <c r="B281" s="59"/>
       <c r="C281" s="3"/>
       <c r="D281" s="3" t="s">
         <v>344</v>
@@ -6011,8 +6016,8 @@
       <c r="E281" s="3"/>
     </row>
     <row r="282" spans="1:5">
-      <c r="A282" s="65"/>
-      <c r="B282" s="58"/>
+      <c r="A282" s="60"/>
+      <c r="B282" s="57"/>
       <c r="C282" s="3"/>
       <c r="D282" s="3" t="s">
         <v>346</v>
@@ -6020,8 +6025,8 @@
       <c r="E282" s="3"/>
     </row>
     <row r="283" spans="1:5" ht="30">
-      <c r="A283" s="65"/>
-      <c r="B283" s="58"/>
+      <c r="A283" s="60"/>
+      <c r="B283" s="57"/>
       <c r="C283" s="3"/>
       <c r="D283" s="3" t="s">
         <v>339</v>
@@ -6031,8 +6036,8 @@
       </c>
     </row>
     <row r="284" spans="1:5">
-      <c r="A284" s="65"/>
-      <c r="B284" s="58"/>
+      <c r="A284" s="60"/>
+      <c r="B284" s="57"/>
       <c r="C284" s="3"/>
       <c r="D284" s="3" t="s">
         <v>343</v>
@@ -6040,8 +6045,8 @@
       <c r="E284" s="3"/>
     </row>
     <row r="285" spans="1:5">
-      <c r="A285" s="65"/>
-      <c r="B285" s="58"/>
+      <c r="A285" s="60"/>
+      <c r="B285" s="57"/>
       <c r="C285" s="3"/>
       <c r="D285" s="3" t="s">
         <v>347</v>
@@ -6049,8 +6054,8 @@
       <c r="E285" s="3"/>
     </row>
     <row r="286" spans="1:5">
-      <c r="A286" s="65"/>
-      <c r="B286" s="58"/>
+      <c r="A286" s="60"/>
+      <c r="B286" s="57"/>
       <c r="C286" s="3"/>
       <c r="D286" s="3" t="s">
         <v>350</v>
@@ -6060,8 +6065,8 @@
       </c>
     </row>
     <row r="287" spans="1:5" ht="30">
-      <c r="A287" s="65"/>
-      <c r="B287" s="58"/>
+      <c r="A287" s="60"/>
+      <c r="B287" s="57"/>
       <c r="C287" s="3"/>
       <c r="D287" s="3" t="s">
         <v>349</v>
@@ -6071,8 +6076,8 @@
       </c>
     </row>
     <row r="288" spans="1:5">
-      <c r="A288" s="65"/>
-      <c r="B288" s="58"/>
+      <c r="A288" s="60"/>
+      <c r="B288" s="57"/>
       <c r="C288" s="3"/>
       <c r="D288" s="3" t="s">
         <v>353</v>
@@ -6082,8 +6087,8 @@
       </c>
     </row>
     <row r="289" spans="1:5">
-      <c r="A289" s="64"/>
-      <c r="B289" s="60"/>
+      <c r="A289" s="61"/>
+      <c r="B289" s="62"/>
       <c r="C289" s="16"/>
       <c r="D289" s="34" t="s">
         <v>306</v>
@@ -6097,9 +6102,9 @@
       <c r="B290" s="9">
         <v>5</v>
       </c>
-      <c r="C290" s="79"/>
-      <c r="D290" s="80"/>
-      <c r="E290" s="84"/>
+      <c r="C290" s="63"/>
+      <c r="D290" s="64"/>
+      <c r="E290" s="65"/>
     </row>
     <row r="291" spans="1:5">
       <c r="A291" s="25"/>
@@ -6126,15 +6131,15 @@
       <c r="B293" s="8">
         <v>4</v>
       </c>
-      <c r="C293" s="76" t="s">
+      <c r="C293" s="66" t="s">
         <v>336</v>
       </c>
-      <c r="D293" s="77"/>
-      <c r="E293" s="78"/>
+      <c r="D293" s="67"/>
+      <c r="E293" s="68"/>
     </row>
     <row r="294" spans="1:5">
-      <c r="A294" s="62"/>
-      <c r="B294" s="56"/>
+      <c r="A294" s="58"/>
+      <c r="B294" s="59"/>
       <c r="C294" s="16"/>
       <c r="D294" s="3" t="s">
         <v>135</v>
@@ -6144,8 +6149,8 @@
       </c>
     </row>
     <row r="295" spans="1:5">
-      <c r="A295" s="64"/>
-      <c r="B295" s="60"/>
+      <c r="A295" s="61"/>
+      <c r="B295" s="62"/>
       <c r="C295" s="16"/>
       <c r="D295" s="34" t="s">
         <v>306</v>
@@ -6159,13 +6164,13 @@
       <c r="B296" s="8">
         <v>6</v>
       </c>
-      <c r="C296" s="79"/>
-      <c r="D296" s="80"/>
-      <c r="E296" s="84"/>
+      <c r="C296" s="63"/>
+      <c r="D296" s="64"/>
+      <c r="E296" s="65"/>
     </row>
     <row r="297" spans="1:5">
-      <c r="A297" s="62"/>
-      <c r="B297" s="56"/>
+      <c r="A297" s="58"/>
+      <c r="B297" s="59"/>
       <c r="C297" s="16"/>
       <c r="D297" s="3" t="s">
         <v>47</v>
@@ -6175,8 +6180,8 @@
       </c>
     </row>
     <row r="298" spans="1:5">
-      <c r="A298" s="65"/>
-      <c r="B298" s="58"/>
+      <c r="A298" s="60"/>
+      <c r="B298" s="57"/>
       <c r="C298" s="16"/>
       <c r="D298" s="3" t="s">
         <v>48</v>
@@ -6186,8 +6191,8 @@
       </c>
     </row>
     <row r="299" spans="1:5">
-      <c r="A299" s="65"/>
-      <c r="B299" s="58"/>
+      <c r="A299" s="60"/>
+      <c r="B299" s="57"/>
       <c r="C299" s="16"/>
       <c r="D299" s="3" t="s">
         <v>49</v>
@@ -6197,8 +6202,8 @@
       </c>
     </row>
     <row r="300" spans="1:5">
-      <c r="A300" s="65"/>
-      <c r="B300" s="58"/>
+      <c r="A300" s="60"/>
+      <c r="B300" s="57"/>
       <c r="C300" s="16"/>
       <c r="D300" s="3" t="s">
         <v>51</v>
@@ -6208,8 +6213,8 @@
       </c>
     </row>
     <row r="301" spans="1:5">
-      <c r="A301" s="65"/>
-      <c r="B301" s="58"/>
+      <c r="A301" s="60"/>
+      <c r="B301" s="57"/>
       <c r="C301" s="16"/>
       <c r="D301" s="3" t="s">
         <v>52</v>
@@ -6219,8 +6224,8 @@
       </c>
     </row>
     <row r="302" spans="1:5">
-      <c r="A302" s="64"/>
-      <c r="B302" s="60"/>
+      <c r="A302" s="61"/>
+      <c r="B302" s="62"/>
       <c r="C302" s="16"/>
       <c r="D302" s="3" t="s">
         <v>53</v>
@@ -6236,13 +6241,13 @@
       <c r="B303" s="8">
         <v>7</v>
       </c>
-      <c r="C303" s="79"/>
-      <c r="D303" s="80"/>
-      <c r="E303" s="84"/>
+      <c r="C303" s="63"/>
+      <c r="D303" s="64"/>
+      <c r="E303" s="65"/>
     </row>
     <row r="304" spans="1:5">
-      <c r="A304" s="62"/>
-      <c r="B304" s="56"/>
+      <c r="A304" s="58"/>
+      <c r="B304" s="59"/>
       <c r="C304" s="16"/>
       <c r="D304" s="3" t="s">
         <v>33</v>
@@ -6252,8 +6257,8 @@
       </c>
     </row>
     <row r="305" spans="1:5">
-      <c r="A305" s="65"/>
-      <c r="B305" s="58"/>
+      <c r="A305" s="60"/>
+      <c r="B305" s="57"/>
       <c r="C305" s="16"/>
       <c r="D305" s="3" t="s">
         <v>34</v>
@@ -6263,8 +6268,8 @@
       </c>
     </row>
     <row r="306" spans="1:5">
-      <c r="A306" s="65"/>
-      <c r="B306" s="58"/>
+      <c r="A306" s="60"/>
+      <c r="B306" s="57"/>
       <c r="C306" s="16"/>
       <c r="D306" s="3" t="s">
         <v>35</v>
@@ -6274,8 +6279,8 @@
       </c>
     </row>
     <row r="307" spans="1:5">
-      <c r="A307" s="65"/>
-      <c r="B307" s="58"/>
+      <c r="A307" s="60"/>
+      <c r="B307" s="57"/>
       <c r="D307" s="3" t="s">
         <v>59</v>
       </c>
@@ -6284,8 +6289,8 @@
       </c>
     </row>
     <row r="308" spans="1:5">
-      <c r="A308" s="65"/>
-      <c r="B308" s="58"/>
+      <c r="A308" s="60"/>
+      <c r="B308" s="57"/>
       <c r="C308" s="16"/>
       <c r="D308" s="3" t="s">
         <v>36</v>
@@ -6295,8 +6300,8 @@
       </c>
     </row>
     <row r="309" spans="1:5">
-      <c r="A309" s="65"/>
-      <c r="B309" s="58"/>
+      <c r="A309" s="60"/>
+      <c r="B309" s="57"/>
       <c r="C309" s="16"/>
       <c r="D309" s="3" t="s">
         <v>37</v>
@@ -6315,6 +6320,72 @@
     </row>
   </sheetData>
   <mergeCells count="82">
+    <mergeCell ref="A58:B70"/>
+    <mergeCell ref="C110:E110"/>
+    <mergeCell ref="A110:B116"/>
+    <mergeCell ref="A102:B108"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="A47:B56"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="C60:E60"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="C92:E92"/>
+    <mergeCell ref="C101:E101"/>
+    <mergeCell ref="C109:E109"/>
+    <mergeCell ref="C71:E71"/>
+    <mergeCell ref="A118:B121"/>
+    <mergeCell ref="C153:E153"/>
+    <mergeCell ref="C154:E154"/>
+    <mergeCell ref="C151:E151"/>
+    <mergeCell ref="C143:E143"/>
+    <mergeCell ref="A123:B142"/>
+    <mergeCell ref="A144:B150"/>
+    <mergeCell ref="A152:B152"/>
+    <mergeCell ref="A199:B207"/>
+    <mergeCell ref="A209:B226"/>
+    <mergeCell ref="A297:B302"/>
+    <mergeCell ref="A304:B309"/>
+    <mergeCell ref="A266:B267"/>
+    <mergeCell ref="A269:B270"/>
+    <mergeCell ref="A272:B275"/>
+    <mergeCell ref="A277:B279"/>
+    <mergeCell ref="A281:B289"/>
+    <mergeCell ref="A294:B295"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="C252:E252"/>
+    <mergeCell ref="C269:E269"/>
+    <mergeCell ref="C290:E290"/>
+    <mergeCell ref="C278:E278"/>
+    <mergeCell ref="C211:E211"/>
+    <mergeCell ref="C272:E272"/>
+    <mergeCell ref="C236:E236"/>
+    <mergeCell ref="C277:E277"/>
+    <mergeCell ref="C274:E274"/>
+    <mergeCell ref="C273:E273"/>
+    <mergeCell ref="A253:B264"/>
+    <mergeCell ref="A228:B235"/>
+    <mergeCell ref="A237:B251"/>
+    <mergeCell ref="C117:E117"/>
+    <mergeCell ref="C122:E122"/>
+    <mergeCell ref="C198:E198"/>
+    <mergeCell ref="C280:E280"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="A6:B11"/>
+    <mergeCell ref="A35:B42"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="A13:B33"/>
+    <mergeCell ref="D6:D11"/>
+    <mergeCell ref="C6:C11"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D3"/>
     <mergeCell ref="A72:B91"/>
     <mergeCell ref="A93:B100"/>
     <mergeCell ref="C303:E303"/>
@@ -6331,72 +6402,6 @@
     <mergeCell ref="C227:E227"/>
     <mergeCell ref="C156:E156"/>
     <mergeCell ref="C296:E296"/>
-    <mergeCell ref="C198:E198"/>
-    <mergeCell ref="C280:E280"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="A6:B11"/>
-    <mergeCell ref="A35:B42"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="A13:B33"/>
-    <mergeCell ref="D6:D11"/>
-    <mergeCell ref="C6:C11"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="C252:E252"/>
-    <mergeCell ref="C269:E269"/>
-    <mergeCell ref="C290:E290"/>
-    <mergeCell ref="C278:E278"/>
-    <mergeCell ref="C211:E211"/>
-    <mergeCell ref="C272:E272"/>
-    <mergeCell ref="C236:E236"/>
-    <mergeCell ref="C277:E277"/>
-    <mergeCell ref="C274:E274"/>
-    <mergeCell ref="C273:E273"/>
-    <mergeCell ref="A253:B264"/>
-    <mergeCell ref="A228:B235"/>
-    <mergeCell ref="A237:B251"/>
-    <mergeCell ref="C117:E117"/>
-    <mergeCell ref="C122:E122"/>
-    <mergeCell ref="A199:B207"/>
-    <mergeCell ref="A209:B226"/>
-    <mergeCell ref="A297:B302"/>
-    <mergeCell ref="A304:B309"/>
-    <mergeCell ref="A266:B267"/>
-    <mergeCell ref="A269:B270"/>
-    <mergeCell ref="A272:B275"/>
-    <mergeCell ref="A277:B279"/>
-    <mergeCell ref="A281:B289"/>
-    <mergeCell ref="A294:B295"/>
-    <mergeCell ref="A118:B121"/>
-    <mergeCell ref="C153:E153"/>
-    <mergeCell ref="C154:E154"/>
-    <mergeCell ref="C151:E151"/>
-    <mergeCell ref="C143:E143"/>
-    <mergeCell ref="A123:B142"/>
-    <mergeCell ref="A144:B150"/>
-    <mergeCell ref="A152:B152"/>
-    <mergeCell ref="A58:B70"/>
-    <mergeCell ref="C110:E110"/>
-    <mergeCell ref="A110:B116"/>
-    <mergeCell ref="A102:B108"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="C49:E49"/>
-    <mergeCell ref="A47:B56"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="C60:E60"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="C92:E92"/>
-    <mergeCell ref="C101:E101"/>
-    <mergeCell ref="C109:E109"/>
-    <mergeCell ref="C71:E71"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>